<commit_message>
Added the points that michelle found
</commit_message>
<xml_diff>
--- a/Event_Points.xlsx
+++ b/Event_Points.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="159">
   <si>
     <t xml:space="preserve">Narrowed Point</t>
   </si>
@@ -365,6 +365,138 @@
   </si>
   <si>
     <t xml:space="preserve">2018-08-28T01:30:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-12T08:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-12T20:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-15T00:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-15T09:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-17T04:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-17T16:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-19T14:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-19T20:30:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-22T04:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-22T10:15:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-24T12:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-24T15:30:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-26T20:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-27T05:45:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-29T04:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-29T11:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-31T08:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-08-31T17:45:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-05T04:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-05T11:15:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-10T00:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-10T08:30:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-12T08:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-12T14:30:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-17T00:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-17T09:45:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-19T08:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-19T16:45:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-21T20:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-22T05:15:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-24T00:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-24T09:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-29T00:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-29T07:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-10-01T08:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-10-01T10:30:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-10-03T20:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-10-04T00:45:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-10-06T00:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-10-06T08:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-10-08T04:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-10-08T14:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-10-11T00:00:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-10-11T04:30:00.000</t>
   </si>
 </sst>
 </file>
@@ -462,7 +594,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -507,6 +639,14 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,13 +667,14 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="29.57"/>
@@ -1707,9 +1848,16 @@
       <c r="X26" s="7"/>
       <c r="Y26" s="7"/>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+    <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>116</v>
+      </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -1732,10 +1880,16 @@
       <c r="X27" s="7"/>
       <c r="Y27" s="7"/>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+    <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -1759,10 +1913,16 @@
       <c r="X28" s="7"/>
       <c r="Y28" s="7"/>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
+    <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>120</v>
+      </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -1786,10 +1946,16 @@
       <c r="X29" s="7"/>
       <c r="Y29" s="7"/>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>122</v>
+      </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -1813,10 +1979,16 @@
       <c r="X30" s="7"/>
       <c r="Y30" s="7"/>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+    <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>124</v>
+      </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -1840,10 +2012,16 @@
       <c r="X31" s="7"/>
       <c r="Y31" s="7"/>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>126</v>
+      </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -1867,10 +2045,16 @@
       <c r="X32" s="7"/>
       <c r="Y32" s="7"/>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
+    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>128</v>
+      </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -1894,10 +2078,16 @@
       <c r="X33" s="7"/>
       <c r="Y33" s="7"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
+    <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>130</v>
+      </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -1921,10 +2111,16 @@
       <c r="X34" s="7"/>
       <c r="Y34" s="7"/>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
+    <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>132</v>
+      </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -1948,10 +2144,16 @@
       <c r="X35" s="7"/>
       <c r="Y35" s="7"/>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
+    <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>134</v>
+      </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -1975,10 +2177,16 @@
       <c r="X36" s="7"/>
       <c r="Y36" s="7"/>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
+    <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>136</v>
+      </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2002,10 +2210,16 @@
       <c r="X37" s="7"/>
       <c r="Y37" s="7"/>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
+    <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>138</v>
+      </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2029,10 +2243,16 @@
       <c r="X38" s="7"/>
       <c r="Y38" s="7"/>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
+    <row r="39" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B39" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>140</v>
+      </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
@@ -2056,10 +2276,16 @@
       <c r="X39" s="7"/>
       <c r="Y39" s="7"/>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
+    <row r="40" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>142</v>
+      </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
@@ -2083,10 +2309,16 @@
       <c r="X40" s="7"/>
       <c r="Y40" s="7"/>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
+    <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
@@ -2110,10 +2342,16 @@
       <c r="X41" s="7"/>
       <c r="Y41" s="7"/>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
+    <row r="42" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>146</v>
+      </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
@@ -2137,10 +2375,16 @@
       <c r="X42" s="7"/>
       <c r="Y42" s="7"/>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
+    <row r="43" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B43" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>148</v>
+      </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
@@ -2164,10 +2408,16 @@
       <c r="X43" s="7"/>
       <c r="Y43" s="7"/>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
+    <row r="44" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B44" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>150</v>
+      </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
@@ -2191,10 +2441,16 @@
       <c r="X44" s="7"/>
       <c r="Y44" s="7"/>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
+    <row r="45" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>152</v>
+      </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
@@ -2218,10 +2474,16 @@
       <c r="X45" s="7"/>
       <c r="Y45" s="7"/>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
+    <row r="46" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>154</v>
+      </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -2245,10 +2507,16 @@
       <c r="X46" s="7"/>
       <c r="Y46" s="7"/>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
+    <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>156</v>
+      </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
@@ -2272,10 +2540,16 @@
       <c r="X47" s="7"/>
       <c r="Y47" s="7"/>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
+    <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B48" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>158</v>
+      </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>

</xml_diff>

<commit_message>
took some points out that were on the day side
</commit_message>
<xml_diff>
--- a/Event_Points.xlsx
+++ b/Event_Points.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="125">
   <si>
     <t xml:space="preserve">Narrowed Point</t>
   </si>
@@ -52,25 +52,7 @@
     <t xml:space="preserve">Notes </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2001-08-15 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">09:09:38.000</t>
-    </r>
+    <t xml:space="preserve">2001-08-15 09:09:38.000</t>
   </si>
   <si>
     <t xml:space="preserve">2001-08-15T09:00:00.000</t>
@@ -82,25 +64,7 @@
     <t xml:space="preserve">2001-08-17T16:00:00.000</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2001-08-19 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">20:20:00.500</t>
-    </r>
+    <t xml:space="preserve">2001-08-19 20:20:00.500</t>
   </si>
   <si>
     <t xml:space="preserve">2001-08-19T20:30:00.000</t>
@@ -136,12 +100,6 @@
     <t xml:space="preserve">2001-10-01T10:30:00.000</t>
   </si>
   <si>
-    <t xml:space="preserve">2001-10-03 00:41:24.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2001-10-04T00:45:00.000</t>
-  </si>
-  <si>
     <t xml:space="preserve">2001-10-11 03:50:04.500</t>
   </si>
   <si>
@@ -319,15 +277,6 @@
     <t xml:space="preserve">BLEH, LARGE CHUNKS OF MISSING CIS DATA</t>
   </si>
   <si>
-    <t xml:space="preserve">2003-11-21 19:30:18.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2003-11-21T20:00:00.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">about 4.5</t>
-  </si>
-  <si>
     <t xml:space="preserve">2004-08-31 14:19:12.000</t>
   </si>
   <si>
@@ -391,13 +340,16 @@
     <t xml:space="preserve">85.6 to 100.6 shallow trough</t>
   </si>
   <si>
-    <t xml:space="preserve">2016-09-02 09:51:35.000</t>
+    <t xml:space="preserve">2016-09-03 19:25:45.000</t>
   </si>
   <si>
     <t xml:space="preserve">4</t>
   </si>
   <si>
-    <t xml:space="preserve">2016-09-02T10:00:00.000</t>
+    <t xml:space="preserve">2016-09-03T19:30:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">about 4.7</t>
   </si>
   <si>
     <t xml:space="preserve">96.9 to 99.0 up and down spike</t>
@@ -406,15 +358,6 @@
     <t xml:space="preserve">HOT GARBAGE, C1 CIS SUX, C4 CIS IS MEH</t>
   </si>
   <si>
-    <t xml:space="preserve">2016-09-03 19:25:45.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-09-03T19:30:00.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">about 4.7</t>
-  </si>
-  <si>
     <t xml:space="preserve">2017-09-07 04:31:35.000</t>
   </si>
   <si>
@@ -434,15 +377,6 @@
   </si>
   <si>
     <t xml:space="preserve">76.4 to 72.9 down linear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-09-17 08:20:05.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017-09-17T06:00:00.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">about 3.8</t>
   </si>
   <si>
     <t xml:space="preserve">2018-08-25 22:32:10.000</t>
@@ -473,7 +407,7 @@
     <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ h:mm:ss"/>
     <numFmt numFmtId="167" formatCode="yyyy/m/d\ h:mm:ss"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -508,12 +442,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -613,7 +541,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -634,13 +562,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y211"/>
+  <dimension ref="A1:Y207"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.98"/>
@@ -996,23 +924,33 @@
       <c r="X10" s="8"/>
       <c r="Y10" s="8"/>
     </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="F11" s="10" t="n">
+        <v>37489.1041666667</v>
+      </c>
+      <c r="G11" s="10" t="n">
+        <v>37489.6041666667</v>
+      </c>
       <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="I11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
@@ -1030,31 +968,33 @@
       <c r="Y11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
-        <v>30</v>
+      <c r="A12" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="E12" s="8" t="n">
+        <v>177.7</v>
+      </c>
       <c r="F12" s="10" t="n">
-        <v>37489.1041666667</v>
+        <v>37507.9375</v>
       </c>
       <c r="G12" s="10" t="n">
-        <v>37489.6041666667</v>
+        <v>37508.4375</v>
       </c>
       <c r="H12" s="8"/>
-      <c r="I12" s="2" t="s">
-        <v>34</v>
+      <c r="I12" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
@@ -1074,32 +1014,32 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E13" s="8" t="n">
-        <v>177.7</v>
-      </c>
-      <c r="F13" s="10" t="n">
-        <v>37507.9375</v>
-      </c>
-      <c r="G13" s="10" t="n">
-        <v>37508.4375</v>
+        <v>178.1</v>
+      </c>
+      <c r="F13" s="11" t="n">
+        <v>37545.9166666667</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <v>37546.4166666667</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
@@ -1119,32 +1059,30 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="8" t="n">
-        <v>178.1</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E14" s="8"/>
       <c r="F14" s="11" t="n">
-        <v>37545.9166666667</v>
+        <v>37548.125</v>
       </c>
       <c r="G14" s="11" t="n">
-        <v>37546.4166666667</v>
+        <v>37548.625</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
@@ -1164,30 +1102,32 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="8"/>
+        <v>50</v>
+      </c>
+      <c r="E15" s="8" t="n">
+        <v>158.5</v>
+      </c>
       <c r="F15" s="11" t="n">
-        <v>37548.125</v>
+        <v>37552.9166666667</v>
       </c>
       <c r="G15" s="11" t="n">
-        <v>37548.625</v>
+        <v>37553.4166666667</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
@@ -1207,32 +1147,32 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E16" s="8" t="n">
-        <v>158.5</v>
-      </c>
-      <c r="F16" s="11" t="n">
-        <v>37552.9166666667</v>
-      </c>
-      <c r="G16" s="11" t="n">
-        <v>37553.4166666667</v>
+        <v>123.7</v>
+      </c>
+      <c r="F16" s="10" t="n">
+        <v>37855.2708333333</v>
+      </c>
+      <c r="G16" s="10" t="n">
+        <v>37855.7708333333</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
@@ -1252,32 +1192,32 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E17" s="8" t="n">
-        <v>123.7</v>
+        <v>107</v>
       </c>
       <c r="F17" s="10" t="n">
-        <v>37855.2708333333</v>
+        <v>37881.2916666667</v>
       </c>
       <c r="G17" s="10" t="n">
-        <v>37855.7708333333</v>
+        <v>37516.7916666667</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
@@ -1297,32 +1237,32 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E18" s="8" t="n">
-        <v>107</v>
-      </c>
-      <c r="F18" s="10" t="n">
-        <v>37881.2916666667</v>
-      </c>
-      <c r="G18" s="10" t="n">
-        <v>37516.7916666667</v>
+        <v>141</v>
+      </c>
+      <c r="F18" s="11" t="n">
+        <v>37942.9166666667</v>
+      </c>
+      <c r="G18" s="11" t="n">
+        <v>37943.4166666667</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
@@ -1342,32 +1282,32 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E19" s="8" t="n">
         <v>141</v>
       </c>
       <c r="F19" s="11" t="n">
-        <v>37942.9166666667</v>
+        <v>37943.5</v>
       </c>
       <c r="G19" s="11" t="n">
-        <v>37943.4166666667</v>
+        <v>37944</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
@@ -1387,32 +1327,32 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E20" s="8" t="n">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="F20" s="11" t="n">
-        <v>37943.5</v>
+        <v>37945.5</v>
       </c>
       <c r="G20" s="11" t="n">
-        <v>37944</v>
+        <v>37946</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
@@ -1432,32 +1372,32 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E21" s="8" t="n">
-        <v>171</v>
+        <v>172.8</v>
       </c>
       <c r="F21" s="11" t="n">
-        <v>37945.5</v>
+        <v>37946</v>
       </c>
       <c r="G21" s="11" t="n">
-        <v>37946</v>
+        <v>37946.5</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
@@ -1477,32 +1417,32 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E22" s="8" t="n">
         <v>172.8</v>
       </c>
       <c r="F22" s="11" t="n">
-        <v>37946</v>
+        <v>37946.2916666667</v>
       </c>
       <c r="G22" s="11" t="n">
-        <v>37946.5</v>
+        <v>37946.7916666667</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
@@ -1522,32 +1462,32 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E23" s="8" t="n">
-        <v>172.8</v>
-      </c>
-      <c r="F23" s="11" t="n">
-        <v>37946.2916666667</v>
-      </c>
-      <c r="G23" s="11" t="n">
-        <v>37946.7916666667</v>
+        <v>89.7</v>
+      </c>
+      <c r="F23" s="10" t="n">
+        <v>38230.3333333333</v>
+      </c>
+      <c r="G23" s="10" t="n">
+        <v>38230.8333333333</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="4" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
@@ -1567,32 +1507,32 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="E24" s="8" t="n">
-        <v>172.8</v>
-      </c>
-      <c r="F24" s="11" t="n">
-        <v>37946.5833333333</v>
-      </c>
-      <c r="G24" s="11" t="n">
-        <v>37947.0833333333</v>
+        <v>116</v>
+      </c>
+      <c r="F24" s="10" t="n">
+        <v>38244.6875</v>
+      </c>
+      <c r="G24" s="10" t="n">
+        <v>38245.1875</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="4" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
@@ -1612,32 +1552,32 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E25" s="8" t="n">
-        <v>89.7</v>
+        <v>105.5</v>
       </c>
       <c r="F25" s="10" t="n">
-        <v>38230.3333333333</v>
+        <v>38247.0833333333</v>
       </c>
       <c r="G25" s="10" t="n">
-        <v>38230.8333333333</v>
+        <v>38247.5833333333</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
@@ -1657,32 +1597,32 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="E26" s="8" t="n">
-        <v>116</v>
+        <v>100.7</v>
       </c>
       <c r="F26" s="10" t="n">
-        <v>38244.6875</v>
+        <v>38588.1458333333</v>
       </c>
       <c r="G26" s="10" t="n">
-        <v>38245.1875</v>
+        <v>38588.6458333333</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="4" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
@@ -1702,29 +1642,29 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="E27" s="8" t="n">
-        <v>105.5</v>
+        <v>85.6</v>
       </c>
       <c r="F27" s="10" t="n">
-        <v>38247.0833333333</v>
+        <v>38595.1041666667</v>
       </c>
       <c r="G27" s="10" t="n">
-        <v>38247.5833333333</v>
+        <v>38595.6041666667</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="4" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>102</v>
@@ -1747,32 +1687,32 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E28" s="8" t="n">
         <v>100.7</v>
       </c>
       <c r="F28" s="10" t="n">
-        <v>38588.1458333333</v>
+        <v>42616.5625</v>
       </c>
       <c r="G28" s="10" t="n">
-        <v>38588.6458333333</v>
+        <v>42617.0625</v>
       </c>
       <c r="H28" s="8"/>
       <c r="I28" s="4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
@@ -1792,32 +1732,30 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>92</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="D29" s="12"/>
       <c r="E29" s="8" t="n">
-        <v>85.6</v>
+        <v>130.4</v>
       </c>
       <c r="F29" s="10" t="n">
-        <v>38595.1041666667</v>
+        <v>42984.9583333333</v>
       </c>
       <c r="G29" s="10" t="n">
-        <v>38595.6041666667</v>
+        <v>42985.4583333333</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="4" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
@@ -1837,32 +1775,32 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="E30" s="8" t="n">
-        <v>96.3</v>
+        <v>75.1</v>
       </c>
       <c r="F30" s="10" t="n">
-        <v>42615.1666666667</v>
+        <v>42991.75</v>
       </c>
       <c r="G30" s="10" t="n">
-        <v>42615.6666666667</v>
+        <v>42992.25</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
@@ -1882,32 +1820,32 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="E31" s="8" t="n">
-        <v>100.7</v>
+        <v>73.1</v>
       </c>
       <c r="F31" s="10" t="n">
-        <v>42616.5625</v>
+        <v>43337.5208333333</v>
       </c>
       <c r="G31" s="10" t="n">
-        <v>42617.0625</v>
+        <v>43338.0208333333</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="4" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
@@ -1927,30 +1865,32 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32" s="12"/>
+        <v>107</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="E32" s="8" t="n">
-        <v>130.4</v>
+        <v>70.6</v>
       </c>
       <c r="F32" s="10" t="n">
-        <v>42984.9583333333</v>
+        <v>43339.8125</v>
       </c>
       <c r="G32" s="10" t="n">
-        <v>42985.4583333333</v>
+        <v>43340.3125</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="4" t="s">
         <v>121</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
@@ -1969,34 +1909,16 @@
       <c r="Y32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E33" s="8" t="n">
-        <v>75.1</v>
-      </c>
-      <c r="F33" s="10" t="n">
-        <v>42991.75</v>
-      </c>
-      <c r="G33" s="10" t="n">
-        <v>42992.25</v>
-      </c>
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
       <c r="H33" s="8"/>
-      <c r="I33" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
@@ -2014,34 +1936,16 @@
       <c r="Y33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E34" s="8" t="n">
-        <v>72.9</v>
-      </c>
-      <c r="F34" s="10" t="n">
-        <v>42995</v>
-      </c>
-      <c r="G34" s="10" t="n">
-        <v>42995.5</v>
-      </c>
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
       <c r="H34" s="8"/>
-      <c r="I34" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
@@ -2059,34 +1963,16 @@
       <c r="Y34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E35" s="8" t="n">
-        <v>73.1</v>
-      </c>
-      <c r="F35" s="10" t="n">
-        <v>43337.5208333333</v>
-      </c>
-      <c r="G35" s="10" t="n">
-        <v>43338.0208333333</v>
-      </c>
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
       <c r="H35" s="8"/>
-      <c r="I35" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
@@ -2104,34 +1990,16 @@
       <c r="Y35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E36" s="8" t="n">
-        <v>70.6</v>
-      </c>
-      <c r="F36" s="10" t="n">
-        <v>43339.8125</v>
-      </c>
-      <c r="G36" s="10" t="n">
-        <v>43340.3125</v>
-      </c>
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
@@ -4525,112 +4393,112 @@
       <c r="Y124" s="8"/>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="8"/>
-      <c r="B125" s="8"/>
-      <c r="C125" s="8"/>
-      <c r="D125" s="8"/>
-      <c r="E125" s="8"/>
-      <c r="F125" s="8"/>
-      <c r="G125" s="8"/>
-      <c r="H125" s="8"/>
-      <c r="I125" s="8"/>
-      <c r="J125" s="8"/>
-      <c r="K125" s="8"/>
-      <c r="L125" s="8"/>
-      <c r="M125" s="8"/>
-      <c r="N125" s="8"/>
-      <c r="O125" s="8"/>
-      <c r="P125" s="8"/>
-      <c r="Q125" s="8"/>
-      <c r="R125" s="8"/>
-      <c r="S125" s="8"/>
-      <c r="T125" s="8"/>
-      <c r="U125" s="8"/>
-      <c r="V125" s="8"/>
-      <c r="W125" s="8"/>
-      <c r="X125" s="8"/>
-      <c r="Y125" s="8"/>
+      <c r="A125" s="9"/>
+      <c r="B125" s="9"/>
+      <c r="C125" s="9"/>
+      <c r="D125" s="9"/>
+      <c r="E125" s="9"/>
+      <c r="F125" s="9"/>
+      <c r="G125" s="9"/>
+      <c r="H125" s="9"/>
+      <c r="I125" s="9"/>
+      <c r="J125" s="9"/>
+      <c r="K125" s="9"/>
+      <c r="L125" s="9"/>
+      <c r="M125" s="9"/>
+      <c r="N125" s="9"/>
+      <c r="O125" s="9"/>
+      <c r="P125" s="9"/>
+      <c r="Q125" s="9"/>
+      <c r="R125" s="9"/>
+      <c r="S125" s="9"/>
+      <c r="T125" s="9"/>
+      <c r="U125" s="9"/>
+      <c r="V125" s="9"/>
+      <c r="W125" s="9"/>
+      <c r="X125" s="9"/>
+      <c r="Y125" s="9"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="8"/>
-      <c r="B126" s="8"/>
-      <c r="C126" s="8"/>
-      <c r="D126" s="8"/>
-      <c r="E126" s="8"/>
-      <c r="F126" s="8"/>
-      <c r="G126" s="8"/>
-      <c r="H126" s="8"/>
-      <c r="I126" s="8"/>
-      <c r="J126" s="8"/>
-      <c r="K126" s="8"/>
-      <c r="L126" s="8"/>
-      <c r="M126" s="8"/>
-      <c r="N126" s="8"/>
-      <c r="O126" s="8"/>
-      <c r="P126" s="8"/>
-      <c r="Q126" s="8"/>
-      <c r="R126" s="8"/>
-      <c r="S126" s="8"/>
-      <c r="T126" s="8"/>
-      <c r="U126" s="8"/>
-      <c r="V126" s="8"/>
-      <c r="W126" s="8"/>
-      <c r="X126" s="8"/>
-      <c r="Y126" s="8"/>
+      <c r="A126" s="9"/>
+      <c r="B126" s="9"/>
+      <c r="C126" s="9"/>
+      <c r="D126" s="9"/>
+      <c r="E126" s="9"/>
+      <c r="F126" s="9"/>
+      <c r="G126" s="9"/>
+      <c r="H126" s="9"/>
+      <c r="I126" s="9"/>
+      <c r="J126" s="9"/>
+      <c r="K126" s="9"/>
+      <c r="L126" s="9"/>
+      <c r="M126" s="9"/>
+      <c r="N126" s="9"/>
+      <c r="O126" s="9"/>
+      <c r="P126" s="9"/>
+      <c r="Q126" s="9"/>
+      <c r="R126" s="9"/>
+      <c r="S126" s="9"/>
+      <c r="T126" s="9"/>
+      <c r="U126" s="9"/>
+      <c r="V126" s="9"/>
+      <c r="W126" s="9"/>
+      <c r="X126" s="9"/>
+      <c r="Y126" s="9"/>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="8"/>
-      <c r="B127" s="8"/>
-      <c r="C127" s="8"/>
-      <c r="D127" s="8"/>
-      <c r="E127" s="8"/>
-      <c r="F127" s="8"/>
-      <c r="G127" s="8"/>
-      <c r="H127" s="8"/>
-      <c r="I127" s="8"/>
-      <c r="J127" s="8"/>
-      <c r="K127" s="8"/>
-      <c r="L127" s="8"/>
-      <c r="M127" s="8"/>
-      <c r="N127" s="8"/>
-      <c r="O127" s="8"/>
-      <c r="P127" s="8"/>
-      <c r="Q127" s="8"/>
-      <c r="R127" s="8"/>
-      <c r="S127" s="8"/>
-      <c r="T127" s="8"/>
-      <c r="U127" s="8"/>
-      <c r="V127" s="8"/>
-      <c r="W127" s="8"/>
-      <c r="X127" s="8"/>
-      <c r="Y127" s="8"/>
+      <c r="A127" s="9"/>
+      <c r="B127" s="9"/>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
+      <c r="F127" s="9"/>
+      <c r="G127" s="9"/>
+      <c r="H127" s="9"/>
+      <c r="I127" s="9"/>
+      <c r="J127" s="9"/>
+      <c r="K127" s="9"/>
+      <c r="L127" s="9"/>
+      <c r="M127" s="9"/>
+      <c r="N127" s="9"/>
+      <c r="O127" s="9"/>
+      <c r="P127" s="9"/>
+      <c r="Q127" s="9"/>
+      <c r="R127" s="9"/>
+      <c r="S127" s="9"/>
+      <c r="T127" s="9"/>
+      <c r="U127" s="9"/>
+      <c r="V127" s="9"/>
+      <c r="W127" s="9"/>
+      <c r="X127" s="9"/>
+      <c r="Y127" s="9"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="8"/>
-      <c r="B128" s="8"/>
-      <c r="C128" s="8"/>
-      <c r="D128" s="8"/>
-      <c r="E128" s="8"/>
-      <c r="F128" s="8"/>
-      <c r="G128" s="8"/>
-      <c r="H128" s="8"/>
-      <c r="I128" s="8"/>
-      <c r="J128" s="8"/>
-      <c r="K128" s="8"/>
-      <c r="L128" s="8"/>
-      <c r="M128" s="8"/>
-      <c r="N128" s="8"/>
-      <c r="O128" s="8"/>
-      <c r="P128" s="8"/>
-      <c r="Q128" s="8"/>
-      <c r="R128" s="8"/>
-      <c r="S128" s="8"/>
-      <c r="T128" s="8"/>
-      <c r="U128" s="8"/>
-      <c r="V128" s="8"/>
-      <c r="W128" s="8"/>
-      <c r="X128" s="8"/>
-      <c r="Y128" s="8"/>
+      <c r="A128" s="9"/>
+      <c r="B128" s="9"/>
+      <c r="C128" s="9"/>
+      <c r="D128" s="9"/>
+      <c r="E128" s="9"/>
+      <c r="F128" s="9"/>
+      <c r="G128" s="9"/>
+      <c r="H128" s="9"/>
+      <c r="I128" s="9"/>
+      <c r="J128" s="9"/>
+      <c r="K128" s="9"/>
+      <c r="L128" s="9"/>
+      <c r="M128" s="9"/>
+      <c r="N128" s="9"/>
+      <c r="O128" s="9"/>
+      <c r="P128" s="9"/>
+      <c r="Q128" s="9"/>
+      <c r="R128" s="9"/>
+      <c r="S128" s="9"/>
+      <c r="T128" s="9"/>
+      <c r="U128" s="9"/>
+      <c r="V128" s="9"/>
+      <c r="W128" s="9"/>
+      <c r="X128" s="9"/>
+      <c r="Y128" s="9"/>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="9"/>
@@ -6765,114 +6633,6 @@
       <c r="X207" s="9"/>
       <c r="Y207" s="9"/>
     </row>
-    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="9"/>
-      <c r="B208" s="9"/>
-      <c r="C208" s="9"/>
-      <c r="D208" s="9"/>
-      <c r="E208" s="9"/>
-      <c r="F208" s="9"/>
-      <c r="G208" s="9"/>
-      <c r="H208" s="9"/>
-      <c r="I208" s="9"/>
-      <c r="J208" s="9"/>
-      <c r="K208" s="9"/>
-      <c r="L208" s="9"/>
-      <c r="M208" s="9"/>
-      <c r="N208" s="9"/>
-      <c r="O208" s="9"/>
-      <c r="P208" s="9"/>
-      <c r="Q208" s="9"/>
-      <c r="R208" s="9"/>
-      <c r="S208" s="9"/>
-      <c r="T208" s="9"/>
-      <c r="U208" s="9"/>
-      <c r="V208" s="9"/>
-      <c r="W208" s="9"/>
-      <c r="X208" s="9"/>
-      <c r="Y208" s="9"/>
-    </row>
-    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="9"/>
-      <c r="B209" s="9"/>
-      <c r="C209" s="9"/>
-      <c r="D209" s="9"/>
-      <c r="E209" s="9"/>
-      <c r="F209" s="9"/>
-      <c r="G209" s="9"/>
-      <c r="H209" s="9"/>
-      <c r="I209" s="9"/>
-      <c r="J209" s="9"/>
-      <c r="K209" s="9"/>
-      <c r="L209" s="9"/>
-      <c r="M209" s="9"/>
-      <c r="N209" s="9"/>
-      <c r="O209" s="9"/>
-      <c r="P209" s="9"/>
-      <c r="Q209" s="9"/>
-      <c r="R209" s="9"/>
-      <c r="S209" s="9"/>
-      <c r="T209" s="9"/>
-      <c r="U209" s="9"/>
-      <c r="V209" s="9"/>
-      <c r="W209" s="9"/>
-      <c r="X209" s="9"/>
-      <c r="Y209" s="9"/>
-    </row>
-    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="9"/>
-      <c r="B210" s="9"/>
-      <c r="C210" s="9"/>
-      <c r="D210" s="9"/>
-      <c r="E210" s="9"/>
-      <c r="F210" s="9"/>
-      <c r="G210" s="9"/>
-      <c r="H210" s="9"/>
-      <c r="I210" s="9"/>
-      <c r="J210" s="9"/>
-      <c r="K210" s="9"/>
-      <c r="L210" s="9"/>
-      <c r="M210" s="9"/>
-      <c r="N210" s="9"/>
-      <c r="O210" s="9"/>
-      <c r="P210" s="9"/>
-      <c r="Q210" s="9"/>
-      <c r="R210" s="9"/>
-      <c r="S210" s="9"/>
-      <c r="T210" s="9"/>
-      <c r="U210" s="9"/>
-      <c r="V210" s="9"/>
-      <c r="W210" s="9"/>
-      <c r="X210" s="9"/>
-      <c r="Y210" s="9"/>
-    </row>
-    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="9"/>
-      <c r="B211" s="9"/>
-      <c r="C211" s="9"/>
-      <c r="D211" s="9"/>
-      <c r="E211" s="9"/>
-      <c r="F211" s="9"/>
-      <c r="G211" s="9"/>
-      <c r="H211" s="9"/>
-      <c r="I211" s="9"/>
-      <c r="J211" s="9"/>
-      <c r="K211" s="9"/>
-      <c r="L211" s="9"/>
-      <c r="M211" s="9"/>
-      <c r="N211" s="9"/>
-      <c r="O211" s="9"/>
-      <c r="P211" s="9"/>
-      <c r="Q211" s="9"/>
-      <c r="R211" s="9"/>
-      <c r="S211" s="9"/>
-      <c r="T211" s="9"/>
-      <c r="U211" s="9"/>
-      <c r="V211" s="9"/>
-      <c r="W211" s="9"/>
-      <c r="X211" s="9"/>
-      <c r="Y211" s="9"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Adding Event points as it is atm so you can produce things super quickly
</commit_message>
<xml_diff>
--- a/Event_Points.xlsx
+++ b/Event_Points.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="459">
   <si>
     <t xml:space="preserve">Narrowed Point</t>
   </si>
@@ -72,139 +72,139 @@
     <t xml:space="preserve">2001-09-12 14:23:07.000</t>
   </si>
   <si>
+    <t xml:space="preserve">2.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-21 05:10:55.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-09-24 10:42:00.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-10-01 10:34:44.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001-10-11 03:50:04.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-21 08:28:45.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-09-09 05:56:29.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">177.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-10-17 04:11:55.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">178.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-10-19 09:27:06.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-10-24 05:07:14.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">158.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-02 07:26:19.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-04 15:25:16.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-06 20:38:43.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-09 11:55:23.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-11 16:21:08.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-14 05:58:38.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-16 12:44:52.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-18 19:38:57.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-21 08:28:52.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-23 13:50:45.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-25 19:36:51.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-28 10:28:23.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-08-31 15:23:08.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-09-02 05:32:25.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2002-09-04 12:00:00.000</t>
+  </si>
+  <si>
     <t xml:space="preserve">SKIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2001-09-21 05:10:55.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2001-09-24 10:42:00.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2001-10-01 10:34:44.500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2001-10-11 03:50:04.500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-21 08:28:45.500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-09-09 05:56:29.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">177.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-10-17 04:11:55.500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">178.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-10-19 09:27:06.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-10-24 05:07:14.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">158.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-02 07:26:19.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-04 15:25:16.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-06 20:38:43.500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-09 11:55:23.500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-11 16:21:08.500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-14 05:58:38.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-16 12:44:52.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-18 19:38:57.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-21 08:28:52.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-23 13:50:45.500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-25 19:36:51.500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-28 10:28:23.500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-08-31 15:23:08.500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-09-02 05:32:25.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002-09-04 12:00:00.000</t>
   </si>
   <si>
     <t xml:space="preserve">4.85</t>
@@ -1681,11 +1681,11 @@
   </sheetPr>
   <dimension ref="A1:Q1144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H83" activeCellId="0" sqref="H83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="22.01"/>
@@ -1843,11 +1843,9 @@
       <c r="B6" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="0" t="n">
@@ -1867,16 +1865,14 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C7" s="8"/>
       <c r="D7" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="0" t="n">
@@ -1896,16 +1892,14 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C8" s="8"/>
       <c r="D8" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="0" t="n">
@@ -1925,16 +1919,14 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C9" s="8"/>
       <c r="D9" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="0" t="n">
@@ -1954,16 +1946,14 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="0" t="n">
@@ -1983,16 +1973,14 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="0" t="n">
@@ -2012,19 +2000,17 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>-19.7070707070707</v>
@@ -2043,19 +2029,17 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>-13.9744075829384</v>
@@ -2074,16 +2058,14 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>35</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="0" t="n">
@@ -2103,19 +2085,17 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>36.1083682008368</v>
@@ -2134,16 +2114,14 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="0" t="n">
@@ -2163,16 +2141,14 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="0" t="n">
@@ -2192,16 +2168,14 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="0" t="n">
@@ -2221,16 +2195,14 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="0" t="n">
@@ -2250,16 +2222,14 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C20" s="8"/>
       <c r="D20" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="0" t="n">
@@ -2279,16 +2249,14 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>47</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="0" t="n">
@@ -2308,16 +2276,14 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="0" t="n">
@@ -2337,16 +2303,14 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="0" t="n">
@@ -2366,16 +2330,14 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>27</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="0" t="n">
@@ -2395,16 +2357,14 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="0" t="n">
@@ -2424,16 +2384,14 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="0" t="n">
@@ -2453,16 +2411,14 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="0" t="n">
@@ -2482,16 +2438,14 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="0" t="n">
@@ -2511,14 +2465,12 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C29" s="8"/>
       <c r="D29" s="9" t="s">
         <v>12</v>
       </c>
@@ -2540,13 +2492,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>61</v>
@@ -2574,13 +2526,11 @@
         <v>63</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C31" s="8"/>
       <c r="D31" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="0" t="n">
@@ -2603,11 +2553,9 @@
         <v>64</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C32" s="8"/>
       <c r="D32" s="9" t="s">
         <v>65</v>
       </c>
@@ -2632,13 +2580,11 @@
         <v>66</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C33" s="8"/>
       <c r="D33" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="0" t="n">
@@ -2661,11 +2607,9 @@
         <v>67</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C34" s="8"/>
       <c r="D34" s="9" t="s">
         <v>68</v>
       </c>
@@ -2690,13 +2634,11 @@
         <v>69</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C35" s="8"/>
       <c r="D35" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E35" s="10"/>
       <c r="F35" s="0" t="n">
@@ -2719,13 +2661,11 @@
         <v>70</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C36" s="8"/>
       <c r="D36" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="0" t="n">
@@ -2748,13 +2688,11 @@
         <v>71</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C37" s="8"/>
       <c r="D37" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="0" t="n">
@@ -2777,11 +2715,9 @@
         <v>72</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C38" s="8"/>
       <c r="D38" s="9" t="s">
         <v>73</v>
       </c>
@@ -2806,13 +2742,13 @@
         <v>74</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E39" s="10"/>
       <c r="F39" s="0" t="n">
@@ -2837,11 +2773,9 @@
         <v>76</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C40" s="8"/>
       <c r="D40" s="9" t="s">
         <v>77</v>
       </c>
@@ -2866,11 +2800,9 @@
         <v>78</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C41" s="8"/>
       <c r="D41" s="9" t="s">
         <v>79</v>
       </c>
@@ -2895,11 +2827,9 @@
         <v>80</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C42" s="8"/>
       <c r="D42" s="9" t="s">
         <v>81</v>
       </c>
@@ -2927,7 +2857,7 @@
         <v>83</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>84</v>
@@ -2957,11 +2887,9 @@
         <v>87</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C44" s="8"/>
       <c r="D44" s="9" t="s">
         <v>88</v>
       </c>
@@ -2988,13 +2916,11 @@
         <v>90</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C45" s="8"/>
       <c r="D45" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E45" s="10" t="s">
         <v>91</v>
@@ -3019,11 +2945,9 @@
         <v>92</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C46" s="8"/>
       <c r="D46" s="9" t="s">
         <v>93</v>
       </c>
@@ -3050,11 +2974,9 @@
         <v>94</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C47" s="8"/>
       <c r="D47" s="9" t="s">
         <v>95</v>
       </c>
@@ -3081,11 +3003,9 @@
         <v>97</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C48" s="8"/>
       <c r="D48" s="9" t="s">
         <v>98</v>
       </c>
@@ -3112,13 +3032,11 @@
         <v>100</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C49" s="8"/>
       <c r="D49" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E49" s="10" t="s">
         <v>99</v>
@@ -3143,11 +3061,9 @@
         <v>101</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C50" s="8"/>
       <c r="D50" s="9" t="s">
         <v>102</v>
       </c>
@@ -3174,9 +3090,7 @@
       <c r="B51" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C51" s="8"/>
       <c r="D51" s="9" t="s">
         <v>12</v>
       </c>
@@ -3203,9 +3117,7 @@
       <c r="B52" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C52" s="8"/>
       <c r="D52" s="9" t="s">
         <v>93</v>
       </c>
@@ -3232,9 +3144,7 @@
       <c r="B53" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C53" s="8"/>
       <c r="D53" s="9" t="s">
         <v>107</v>
       </c>
@@ -3261,9 +3171,7 @@
       <c r="B54" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C54" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C54" s="8"/>
       <c r="D54" s="9" t="s">
         <v>109</v>
       </c>
@@ -3290,11 +3198,9 @@
       <c r="B55" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C55" s="8"/>
       <c r="D55" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E55" s="10"/>
       <c r="F55" s="0" t="n">
@@ -3319,9 +3225,7 @@
       <c r="B56" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C56" s="8"/>
       <c r="D56" s="9" t="s">
         <v>112</v>
       </c>
@@ -3348,9 +3252,7 @@
       <c r="B57" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C57" s="8"/>
       <c r="D57" s="9" t="s">
         <v>93</v>
       </c>
@@ -3378,7 +3280,7 @@
         <v>104</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>115</v>
@@ -3409,7 +3311,7 @@
         <v>104</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>102</v>
@@ -3437,13 +3339,11 @@
         <v>117</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C60" s="8"/>
       <c r="D60" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E60" s="10"/>
       <c r="F60" s="0" t="n">
@@ -3466,11 +3366,9 @@
         <v>118</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C61" s="8"/>
       <c r="D61" s="9" t="s">
         <v>119</v>
       </c>
@@ -3495,13 +3393,11 @@
         <v>120</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C62" s="8"/>
       <c r="D62" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E62" s="10"/>
       <c r="F62" s="0" t="n">
@@ -3524,13 +3420,11 @@
         <v>121</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C63" s="8"/>
       <c r="D63" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E63" s="10"/>
       <c r="F63" s="0" t="n">
@@ -3553,13 +3447,11 @@
         <v>122</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C64" s="8"/>
       <c r="D64" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E64" s="10"/>
       <c r="F64" s="0" t="n">
@@ -3582,10 +3474,10 @@
         <v>123</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>124</v>
@@ -3613,13 +3505,13 @@
         <v>125</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E66" s="10"/>
       <c r="F66" s="0" t="n">
@@ -3644,11 +3536,9 @@
         <v>126</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C67" s="8"/>
       <c r="D67" s="9" t="s">
         <v>127</v>
       </c>
@@ -3673,11 +3563,9 @@
         <v>128</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C68" s="8"/>
       <c r="D68" s="9" t="s">
         <v>129</v>
       </c>
@@ -3702,11 +3590,9 @@
         <v>130</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C69" s="8"/>
       <c r="D69" s="9" t="s">
         <v>77</v>
       </c>
@@ -3731,11 +3617,9 @@
         <v>131</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C70" s="8"/>
       <c r="D70" s="9" t="s">
         <v>88</v>
       </c>
@@ -3760,11 +3644,9 @@
         <v>132</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C71" s="8"/>
       <c r="D71" s="9" t="s">
         <v>133</v>
       </c>
@@ -3791,9 +3673,7 @@
       <c r="B72" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C72" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C72" s="8"/>
       <c r="D72" s="9" t="s">
         <v>135</v>
       </c>
@@ -3820,9 +3700,7 @@
       <c r="B73" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C73" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C73" s="8"/>
       <c r="D73" s="9" t="s">
         <v>93</v>
       </c>
@@ -3849,9 +3727,7 @@
       <c r="B74" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C74" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C74" s="8"/>
       <c r="D74" s="9" t="s">
         <v>112</v>
       </c>
@@ -3876,13 +3752,11 @@
         <v>138</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C75" s="8"/>
       <c r="D75" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E75" s="10" t="s">
         <v>139</v>
@@ -3907,11 +3781,9 @@
         <v>140</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C76" s="8"/>
       <c r="D76" s="9" t="s">
         <v>112</v>
       </c>
@@ -3938,13 +3810,11 @@
         <v>142</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C77" s="8"/>
       <c r="D77" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>143</v>
@@ -3969,13 +3839,11 @@
         <v>144</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C78" s="8"/>
       <c r="D78" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E78" s="10"/>
       <c r="F78" s="0" t="n">
@@ -3998,11 +3866,9 @@
         <v>145</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C79" s="8"/>
       <c r="D79" s="9" t="s">
         <v>146</v>
       </c>
@@ -4029,11 +3895,9 @@
       <c r="B80" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C80" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C80" s="8"/>
       <c r="D80" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E80" s="10"/>
       <c r="F80" s="0" t="n">
@@ -4058,9 +3922,7 @@
       <c r="B81" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C81" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C81" s="8"/>
       <c r="D81" s="9" t="s">
         <v>149</v>
       </c>
@@ -4087,9 +3949,7 @@
       <c r="B82" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C82" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C82" s="8"/>
       <c r="D82" s="9" t="s">
         <v>151</v>
       </c>
@@ -4114,13 +3974,11 @@
         <v>152</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C83" s="8"/>
       <c r="D83" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E83" s="10"/>
       <c r="F83" s="0" t="n">
@@ -4143,13 +4001,11 @@
         <v>153</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C84" s="8"/>
       <c r="D84" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E84" s="10"/>
       <c r="F84" s="0" t="n">
@@ -4172,11 +4028,9 @@
         <v>154</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C85" s="8"/>
       <c r="D85" s="9" t="s">
         <v>129</v>
       </c>
@@ -4201,11 +4055,9 @@
         <v>155</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C86" s="8"/>
       <c r="D86" s="13" t="n">
         <v>1</v>
       </c>
@@ -4233,7 +4085,7 @@
         <v>83</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D87" s="13" t="n">
         <v>2.3</v>
@@ -4264,7 +4116,7 @@
         <v>104</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D88" s="13" t="n">
         <v>0.7</v>
@@ -4293,7 +4145,7 @@
         <v>83</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D89" s="13" t="n">
         <v>1.7</v>
@@ -4322,7 +4174,7 @@
         <v>83</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>79</v>
@@ -4351,10 +4203,10 @@
         <v>83</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E91" s="10"/>
       <c r="F91" s="0" t="n">
@@ -4380,10 +4232,10 @@
         <v>83</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E92" s="10"/>
       <c r="F92" s="0" t="n">
@@ -4406,10 +4258,10 @@
         <v>162</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D93" s="9" t="s">
         <v>163</v>
@@ -4435,10 +4287,10 @@
         <v>164</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D94" s="9" t="s">
         <v>112</v>
@@ -4464,13 +4316,13 @@
         <v>165</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E95" s="10"/>
       <c r="F95" s="0" t="n">
@@ -4493,13 +4345,13 @@
         <v>166</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E96" s="10"/>
       <c r="F96" s="0" t="n">
@@ -4522,13 +4374,13 @@
         <v>167</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E97" s="10"/>
       <c r="F97" s="0" t="n">
@@ -4551,10 +4403,10 @@
         <v>168</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D98" s="9" t="s">
         <v>169</v>
@@ -4580,13 +4432,13 @@
         <v>170</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E99" s="10"/>
       <c r="F99" s="0" t="n">
@@ -4609,10 +4461,10 @@
         <v>171</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D100" s="9" t="s">
         <v>77</v>
@@ -4641,7 +4493,7 @@
         <v>83</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>95</v>
@@ -4672,7 +4524,7 @@
         <v>83</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>175</v>
@@ -4703,10 +4555,10 @@
         <v>104</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E103" s="10"/>
       <c r="F103" s="0" t="n">
@@ -4734,10 +4586,10 @@
         <v>104</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E104" s="10"/>
       <c r="F104" s="0" t="n">
@@ -4763,7 +4615,7 @@
         <v>104</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>180</v>
@@ -4792,10 +4644,10 @@
         <v>104</v>
       </c>
       <c r="C106" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D106" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="D106" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="E106" s="10"/>
       <c r="F106" s="0" t="n">
@@ -4821,10 +4673,10 @@
         <v>104</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E107" s="10"/>
       <c r="F107" s="0" t="n">
@@ -4850,10 +4702,10 @@
         <v>104</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E108" s="10"/>
       <c r="F108" s="0" t="n">
@@ -4879,10 +4731,10 @@
         <v>104</v>
       </c>
       <c r="C109" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D109" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="D109" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="E109" s="10"/>
       <c r="F109" s="0" t="n">
@@ -4908,7 +4760,7 @@
         <v>104</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>186</v>
@@ -4937,7 +4789,7 @@
         <v>104</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>12</v>
@@ -4966,7 +4818,7 @@
         <v>104</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>95</v>
@@ -4995,7 +4847,7 @@
         <v>104</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>77</v>
@@ -5024,7 +4876,7 @@
         <v>104</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>191</v>
@@ -5053,7 +4905,7 @@
         <v>104</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>175</v>
@@ -5082,10 +4934,10 @@
         <v>104</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E116" s="10"/>
       <c r="F116" s="0" t="n">
@@ -5113,7 +4965,7 @@
         <v>104</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>196</v>
@@ -5144,10 +4996,10 @@
         <v>104</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E118" s="10"/>
       <c r="F118" s="0" t="n">
@@ -5175,7 +5027,7 @@
         <v>104</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>109</v>
@@ -5206,7 +5058,7 @@
         <v>104</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D120" s="9" t="s">
         <v>200</v>
@@ -5237,7 +5089,7 @@
         <v>104</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D121" s="9" t="s">
         <v>202</v>
@@ -5268,10 +5120,10 @@
         <v>104</v>
       </c>
       <c r="C122" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D122" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="D122" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="E122" s="10"/>
       <c r="F122" s="0" t="n">
@@ -5299,10 +5151,10 @@
         <v>104</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E123" s="10"/>
       <c r="F123" s="0" t="n">
@@ -5330,7 +5182,7 @@
         <v>104</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D124" s="9" t="s">
         <v>102</v>
@@ -5363,7 +5215,7 @@
         <v>104</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>207</v>
@@ -5394,10 +5246,10 @@
         <v>104</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D126" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E126" s="8"/>
       <c r="F126" s="0" t="n">
@@ -5425,10 +5277,10 @@
         <v>104</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E127" s="8"/>
       <c r="F127" s="0" t="n">
@@ -5456,10 +5308,10 @@
         <v>104</v>
       </c>
       <c r="C128" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D128" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="D128" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="E128" s="8"/>
       <c r="F128" s="0" t="n">
@@ -5487,7 +5339,7 @@
         <v>104</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D129" s="9" t="s">
         <v>109</v>
@@ -5518,10 +5370,10 @@
         <v>104</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D130" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E130" s="8"/>
       <c r="F130" s="0" t="n">
@@ -5547,7 +5399,7 @@
         <v>104</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D131" s="9" t="s">
         <v>133</v>
@@ -5576,10 +5428,10 @@
         <v>104</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D132" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E132" s="8"/>
       <c r="F132" s="0" t="n">
@@ -5605,10 +5457,10 @@
         <v>104</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E133" s="8"/>
       <c r="F133" s="0" t="n">
@@ -5634,10 +5486,10 @@
         <v>104</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E134" s="8"/>
       <c r="F134" s="0" t="n">
@@ -5663,10 +5515,10 @@
         <v>104</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D135" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E135" s="8"/>
       <c r="F135" s="0" t="n">
@@ -5692,10 +5544,10 @@
         <v>104</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E136" s="8"/>
       <c r="F136" s="0" t="n">
@@ -5721,7 +5573,7 @@
         <v>104</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D137" s="9" t="s">
         <v>77</v>
@@ -5750,7 +5602,7 @@
         <v>104</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D138" s="9" t="s">
         <v>102</v>
@@ -5779,7 +5631,7 @@
         <v>104</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D139" s="9" t="s">
         <v>93</v>
@@ -5808,10 +5660,10 @@
         <v>104</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E140" s="8"/>
       <c r="F140" s="0" t="n">
@@ -5837,10 +5689,10 @@
         <v>104</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D141" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E141" s="8"/>
       <c r="F141" s="0" t="n">
@@ -5866,7 +5718,7 @@
         <v>104</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D142" s="9" t="s">
         <v>77</v>
@@ -5895,7 +5747,7 @@
         <v>104</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D143" s="9" t="s">
         <v>12</v>
@@ -5924,7 +5776,7 @@
         <v>104</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D144" s="9" t="s">
         <v>163</v>
@@ -5953,7 +5805,7 @@
         <v>104</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D145" s="9" t="s">
         <v>228</v>
@@ -5982,10 +5834,10 @@
         <v>104</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D146" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E146" s="8"/>
       <c r="F146" s="0" t="n">
@@ -6011,7 +5863,7 @@
         <v>104</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D147" s="9" t="s">
         <v>77</v>
@@ -6040,10 +5892,10 @@
         <v>104</v>
       </c>
       <c r="C148" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D148" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="D148" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="E148" s="8"/>
       <c r="F148" s="0" t="n">
@@ -6069,7 +5921,7 @@
         <v>104</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D149" s="9" t="s">
         <v>10</v>
@@ -6098,7 +5950,7 @@
         <v>104</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D150" s="9" t="s">
         <v>234</v>
@@ -6127,10 +5979,10 @@
         <v>104</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D151" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E151" s="8"/>
       <c r="F151" s="0" t="n">
@@ -6156,10 +6008,10 @@
         <v>104</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D152" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E152" s="8"/>
       <c r="F152" s="0" t="n">
@@ -6185,10 +6037,10 @@
         <v>104</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D153" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E153" s="8"/>
       <c r="F153" s="0" t="n">
@@ -6214,7 +6066,7 @@
         <v>104</v>
       </c>
       <c r="C154" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D154" s="9" t="s">
         <v>239</v>
@@ -6243,7 +6095,7 @@
         <v>104</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D155" s="9" t="s">
         <v>109</v>
@@ -6272,7 +6124,7 @@
         <v>104</v>
       </c>
       <c r="C156" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D156" s="9" t="s">
         <v>242</v>
@@ -6301,10 +6153,10 @@
         <v>104</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D157" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E157" s="8"/>
       <c r="F157" s="0" t="n">
@@ -6330,10 +6182,10 @@
         <v>104</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D158" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E158" s="8"/>
       <c r="F158" s="0" t="n">
@@ -6359,7 +6211,7 @@
         <v>104</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D159" s="9" t="s">
         <v>102</v>
@@ -6388,7 +6240,7 @@
         <v>104</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D160" s="9" t="s">
         <v>93</v>
@@ -6417,7 +6269,7 @@
         <v>104</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D161" s="9" t="s">
         <v>109</v>
@@ -6446,10 +6298,10 @@
         <v>104</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D162" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E162" s="8"/>
       <c r="F162" s="0" t="n">
@@ -6475,7 +6327,7 @@
         <v>104</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D163" s="9" t="s">
         <v>250</v>
@@ -6501,10 +6353,10 @@
         <v>104</v>
       </c>
       <c r="C164" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D164" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="D164" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="E164" s="8"/>
       <c r="F164" s="0" t="n">
@@ -6530,7 +6382,7 @@
         <v>104</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D165" s="9" t="s">
         <v>253</v>
@@ -6559,7 +6411,7 @@
         <v>104</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D166" s="9" t="s">
         <v>255</v>
@@ -6588,10 +6440,10 @@
         <v>104</v>
       </c>
       <c r="C167" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D167" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="D167" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="E167" s="8"/>
       <c r="F167" s="0" t="n">
@@ -6617,10 +6469,10 @@
         <v>104</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D168" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E168" s="8"/>
       <c r="F168" s="0" t="n">
@@ -6646,7 +6498,7 @@
         <v>104</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D169" s="9" t="s">
         <v>259</v>
@@ -6675,10 +6527,10 @@
         <v>104</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D170" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E170" s="8"/>
       <c r="F170" s="0" t="n">
@@ -6704,10 +6556,10 @@
         <v>104</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D171" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E171" s="8"/>
       <c r="F171" s="0" t="n">
@@ -6733,7 +6585,7 @@
         <v>104</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D172" s="9" t="s">
         <v>263</v>
@@ -6764,10 +6616,10 @@
         <v>104</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D173" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E173" s="10" t="s">
         <v>266</v>
@@ -6795,7 +6647,7 @@
         <v>104</v>
       </c>
       <c r="C174" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D174" s="9" t="s">
         <v>268</v>
@@ -6826,7 +6678,7 @@
         <v>104</v>
       </c>
       <c r="C175" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D175" s="9" t="s">
         <v>102</v>
@@ -6857,7 +6709,7 @@
         <v>104</v>
       </c>
       <c r="C176" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D176" s="9" t="s">
         <v>273</v>
@@ -6888,10 +6740,10 @@
         <v>104</v>
       </c>
       <c r="C177" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D177" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E177" s="8"/>
       <c r="F177" s="0" t="n">
@@ -6917,7 +6769,7 @@
         <v>104</v>
       </c>
       <c r="C178" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D178" s="9" t="s">
         <v>277</v>
@@ -6946,7 +6798,7 @@
         <v>104</v>
       </c>
       <c r="C179" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D179" s="9" t="s">
         <v>93</v>
@@ -6975,10 +6827,10 @@
         <v>104</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D180" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E180" s="8"/>
       <c r="F180" s="0" t="n">
@@ -7004,10 +6856,10 @@
         <v>104</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D181" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E181" s="8"/>
       <c r="F181" s="0" t="n">
@@ -7033,10 +6885,10 @@
         <v>104</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D182" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E182" s="8"/>
       <c r="F182" s="0" t="n">
@@ -7062,7 +6914,7 @@
         <v>104</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D183" s="9" t="s">
         <v>283</v>
@@ -7091,7 +6943,7 @@
         <v>104</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D184" s="9" t="s">
         <v>12</v>
@@ -7120,7 +6972,7 @@
         <v>104</v>
       </c>
       <c r="C185" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D185" s="9" t="s">
         <v>180</v>
@@ -7149,10 +7001,10 @@
         <v>104</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D186" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E186" s="8"/>
       <c r="F186" s="0" t="n">
@@ -7180,7 +7032,7 @@
         <v>104</v>
       </c>
       <c r="C187" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D187" s="9" t="s">
         <v>102</v>
@@ -7211,7 +7063,7 @@
         <v>104</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D188" s="9" t="s">
         <v>273</v>
@@ -7242,10 +7094,10 @@
         <v>104</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D189" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E189" s="8"/>
       <c r="F189" s="0" t="n">
@@ -7273,7 +7125,7 @@
         <v>104</v>
       </c>
       <c r="C190" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D190" s="9" t="s">
         <v>109</v>
@@ -7302,7 +7154,7 @@
         <v>104</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D191" s="9" t="s">
         <v>102</v>
@@ -7331,7 +7183,7 @@
         <v>104</v>
       </c>
       <c r="C192" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D192" s="9" t="s">
         <v>112</v>
@@ -7360,10 +7212,10 @@
         <v>104</v>
       </c>
       <c r="C193" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D193" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E193" s="8"/>
       <c r="F193" s="0" t="n">
@@ -7389,10 +7241,10 @@
         <v>104</v>
       </c>
       <c r="C194" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D194" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E194" s="8"/>
       <c r="F194" s="0" t="n">
@@ -7418,7 +7270,7 @@
         <v>104</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>77</v>
@@ -7447,7 +7299,7 @@
         <v>104</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D196" s="9" t="s">
         <v>77</v>
@@ -7476,7 +7328,7 @@
         <v>104</v>
       </c>
       <c r="C197" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D197" s="9" t="s">
         <v>298</v>
@@ -7505,10 +7357,10 @@
         <v>104</v>
       </c>
       <c r="C198" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D198" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="D198" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="E198" s="8"/>
       <c r="F198" s="0" t="n">
@@ -7534,7 +7386,7 @@
         <v>104</v>
       </c>
       <c r="C199" s="8" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D199" s="9" t="s">
         <v>301</v>
@@ -11106,7 +10958,7 @@
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.06"/>
@@ -11383,13 +11235,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>328</v>
@@ -11415,7 +11267,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>1</v>
@@ -11459,7 +11311,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>1</v>
@@ -11503,7 +11355,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>1</v>
@@ -11545,10 +11397,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>312</v>
@@ -11587,10 +11439,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="17" t="s">
@@ -11629,10 +11481,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="17" t="s">
@@ -11671,10 +11523,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="17" t="s">
@@ -11713,10 +11565,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>338</v>
@@ -11757,10 +11609,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -11785,10 +11637,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -11813,10 +11665,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -11841,10 +11693,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -11869,10 +11721,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -11897,10 +11749,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -11925,10 +11777,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -11953,10 +11805,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -11981,10 +11833,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -12009,10 +11861,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -12037,10 +11889,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -12065,10 +11917,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -12093,10 +11945,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -12121,10 +11973,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -12149,10 +12001,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -12180,7 +12032,7 @@
         <v>63</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -12208,7 +12060,7 @@
         <v>64</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
@@ -12236,7 +12088,7 @@
         <v>66</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
@@ -12264,7 +12116,7 @@
         <v>67</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
@@ -12292,7 +12144,7 @@
         <v>69</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
@@ -12320,7 +12172,7 @@
         <v>70</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
@@ -12348,7 +12200,7 @@
         <v>71</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
@@ -12376,7 +12228,7 @@
         <v>72</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
@@ -12404,7 +12256,7 @@
         <v>74</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
@@ -12432,7 +12284,7 @@
         <v>76</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
@@ -12460,7 +12312,7 @@
         <v>78</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
@@ -12488,7 +12340,7 @@
         <v>80</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
@@ -12558,7 +12410,7 @@
         <v>87</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="17" t="s">
@@ -12600,10 +12452,10 @@
         <v>90</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="10"/>
@@ -12630,10 +12482,10 @@
         <v>92</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="10"/>
@@ -12660,7 +12512,7 @@
         <v>94</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>343</v>
@@ -12704,10 +12556,10 @@
         <v>97</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="10"/>
@@ -12734,10 +12586,10 @@
         <v>100</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="10"/>
@@ -12764,7 +12616,7 @@
         <v>101</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C50" s="17"/>
       <c r="D50" s="19"/>
@@ -13044,7 +12896,7 @@
         <v>117</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C60" s="17"/>
       <c r="D60" s="19"/>
@@ -13072,7 +12924,7 @@
         <v>118</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C61" s="17"/>
       <c r="D61" s="19"/>
@@ -13100,7 +12952,7 @@
         <v>120</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C62" s="17"/>
       <c r="D62" s="19"/>
@@ -13128,7 +12980,7 @@
         <v>121</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C63" s="17"/>
       <c r="D63" s="19"/>
@@ -13156,7 +13008,7 @@
         <v>122</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C64" s="17"/>
       <c r="D64" s="19"/>
@@ -13184,7 +13036,7 @@
         <v>123</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C65" s="17"/>
       <c r="D65" s="19"/>
@@ -13212,7 +13064,7 @@
         <v>125</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C66" s="17"/>
       <c r="D66" s="19"/>
@@ -13240,7 +13092,7 @@
         <v>126</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C67" s="17"/>
       <c r="D67" s="19"/>
@@ -13268,7 +13120,7 @@
         <v>128</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C68" s="17"/>
       <c r="D68" s="19"/>
@@ -13296,7 +13148,7 @@
         <v>130</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C69" s="17"/>
       <c r="D69" s="19"/>
@@ -13324,7 +13176,7 @@
         <v>131</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C70" s="17"/>
       <c r="D70" s="19"/>
@@ -13352,7 +13204,7 @@
         <v>132</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C71" s="17"/>
       <c r="D71" s="19"/>
@@ -13464,7 +13316,7 @@
         <v>138</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C75" s="18"/>
       <c r="D75" s="17" t="s">
@@ -13506,7 +13358,7 @@
         <v>140</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C76" s="18"/>
       <c r="D76" s="17" t="s">
@@ -13548,7 +13400,7 @@
         <v>142</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C77" s="18"/>
       <c r="D77" s="17" t="s">
@@ -13590,7 +13442,7 @@
         <v>144</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C78" s="18"/>
       <c r="D78" s="17"/>
@@ -13618,7 +13470,7 @@
         <v>145</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C79" s="18"/>
       <c r="D79" s="17"/>
@@ -13730,7 +13582,7 @@
         <v>152</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C83" s="18"/>
       <c r="D83" s="17"/>
@@ -13758,7 +13610,7 @@
         <v>153</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C84" s="18"/>
       <c r="D84" s="17"/>
@@ -13786,7 +13638,7 @@
         <v>154</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C85" s="18"/>
       <c r="D85" s="17"/>
@@ -13814,7 +13666,7 @@
         <v>155</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C86" s="18"/>
       <c r="D86" s="17"/>
@@ -14010,7 +13862,7 @@
         <v>162</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C93" s="18"/>
       <c r="D93" s="17"/>
@@ -14038,7 +13890,7 @@
         <v>164</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C94" s="18"/>
       <c r="D94" s="17"/>
@@ -14066,7 +13918,7 @@
         <v>165</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C95" s="18"/>
       <c r="D95" s="17"/>
@@ -14094,7 +13946,7 @@
         <v>166</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C96" s="18"/>
       <c r="D96" s="17"/>
@@ -14122,7 +13974,7 @@
         <v>167</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C97" s="18"/>
       <c r="D97" s="17"/>
@@ -14150,7 +14002,7 @@
         <v>168</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C98" s="18"/>
       <c r="D98" s="17"/>
@@ -14178,7 +14030,7 @@
         <v>170</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C99" s="18"/>
       <c r="D99" s="17"/>
@@ -14206,7 +14058,7 @@
         <v>171</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C100" s="18"/>
       <c r="D100" s="17"/>
@@ -21548,7 +21400,7 @@
       <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.43"/>

</xml_diff>

<commit_message>
Identifying which events to skip and which events are clean to run!
</commit_message>
<xml_diff>
--- a/Event_Points.xlsx
+++ b/Event_Points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michellexbui/python/tailwagtools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD875AFA-1121-004F-A4B3-9F3C5AFB2719}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3035FD2-1E08-4144-A046-D167A805F00B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12280" yWindow="460" windowWidth="16520" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15480" yWindow="460" windowWidth="13220" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4457" uniqueCount="1412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4438" uniqueCount="1419">
   <si>
     <t>Narrowed Point</t>
   </si>
@@ -4264,6 +4264,27 @@
   </si>
   <si>
     <t>F10.7 data from here</t>
+  </si>
+  <si>
+    <t>North/South/??</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>CLEAN</t>
+  </si>
+  <si>
+    <t>LACKING</t>
+  </si>
+  <si>
+    <t>MESSY</t>
   </si>
 </sst>
 </file>
@@ -4276,7 +4297,7 @@
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\Thh:mm:ss"/>
     <numFmt numFmtId="167" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4332,13 +4353,62 @@
       <name val="Cambria"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="DejaVu Serif"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -4368,7 +4438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4440,6 +4510,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4757,7 +4853,7 @@
   <dimension ref="A1:Z1128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="13"/>
@@ -4774,6 +4870,7 @@
     <col min="16" max="16" width="28.5" customWidth="1"/>
     <col min="17" max="17" width="33.6640625" customWidth="1"/>
     <col min="18" max="19" width="22.1640625" customWidth="1"/>
+    <col min="21" max="21" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" customHeight="1">
@@ -4783,7 +4880,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="38" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -4834,8 +4931,12 @@
       <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
+      <c r="T1" s="5" t="s">
+        <v>1412</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>1413</v>
+      </c>
       <c r="V1" s="5"/>
       <c r="W1" s="5"/>
       <c r="X1" s="5"/>
@@ -4849,7 +4950,9 @@
       <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D2" s="9" t="s">
         <v>21</v>
       </c>
@@ -4888,8 +4991,12 @@
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
+      <c r="T2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>1418</v>
+      </c>
       <c r="V2" s="8"/>
       <c r="W2" s="8"/>
       <c r="X2" s="8"/>
@@ -4903,7 +5010,7 @@
       <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -4944,8 +5051,12 @@
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
+      <c r="T3" s="8" t="s">
+        <v>1414</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>1417</v>
+      </c>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
@@ -4959,9 +5070,7 @@
       <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C4" s="39"/>
       <c r="D4" s="9" t="s">
         <v>37</v>
       </c>
@@ -5000,8 +5109,12 @@
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
+      <c r="T4" s="8" t="s">
+        <v>1415</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>1416</v>
+      </c>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
@@ -5015,7 +5128,7 @@
       <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -5056,8 +5169,12 @@
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
+      <c r="T5" s="8" t="s">
+        <v>1415</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>1418</v>
+      </c>
       <c r="V5" s="8"/>
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
@@ -5071,7 +5188,7 @@
       <c r="B6" s="7">
         <v>1</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -5120,61 +5237,61 @@
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
     </row>
-    <row r="7" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:26" s="37" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A7" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="34">
         <v>1</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7">
+      <c r="E7" s="36"/>
+      <c r="F7" s="37">
         <v>14.4867521367521</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8" t="s">
+      <c r="I7" s="33"/>
+      <c r="J7" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="M7" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="N7" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="O7" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="33"/>
+      <c r="X7" s="33"/>
+      <c r="Y7" s="33"/>
+      <c r="Z7" s="33"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1">
       <c r="A8" s="6" t="s">
@@ -5183,9 +5300,7 @@
       <c r="B8" s="7">
         <v>1</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C8" s="39"/>
       <c r="D8" s="9" t="s">
         <v>67</v>
       </c>
@@ -5239,7 +5354,7 @@
       <c r="B9" s="7">
         <v>1</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -5295,7 +5410,7 @@
       <c r="B10" s="7">
         <v>1</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -5351,7 +5466,7 @@
       <c r="B11" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="9" t="s">
@@ -5407,9 +5522,7 @@
       <c r="B12" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C12" s="39"/>
       <c r="D12" s="9" t="s">
         <v>96</v>
       </c>
@@ -5463,7 +5576,7 @@
       <c r="B13" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -5519,9 +5632,7 @@
       <c r="B14" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C14" s="39"/>
       <c r="D14" s="9" t="s">
         <v>52</v>
       </c>
@@ -5575,9 +5686,7 @@
       <c r="B15" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C15" s="39"/>
       <c r="D15" s="9" t="s">
         <v>89</v>
       </c>
@@ -5631,9 +5740,7 @@
       <c r="B16" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C16" s="41"/>
       <c r="D16" s="9" t="s">
         <v>125</v>
       </c>
@@ -5687,7 +5794,7 @@
       <c r="B17" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="9" t="s">
@@ -5743,7 +5850,7 @@
       <c r="B18" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -5799,7 +5906,7 @@
       <c r="B19" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="9" t="s">
@@ -5855,7 +5962,7 @@
       <c r="B20" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -5911,9 +6018,7 @@
       <c r="B21" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C21" s="39"/>
       <c r="D21" s="9" t="s">
         <v>154</v>
       </c>
@@ -5967,9 +6072,7 @@
       <c r="B22" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C22" s="39"/>
       <c r="D22" s="9" t="s">
         <v>162</v>
       </c>
@@ -6023,7 +6126,7 @@
       <c r="B23" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="40" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -6079,7 +6182,7 @@
       <c r="B24" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -6135,7 +6238,7 @@
       <c r="B25" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -6175,9 +6278,7 @@
       <c r="B26" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C26" s="39"/>
       <c r="D26" s="9" t="s">
         <v>162</v>
       </c>
@@ -6231,7 +6332,7 @@
       <c r="B27" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="40" t="s">
         <v>20</v>
       </c>
       <c r="D27" s="9" t="s">
@@ -6287,9 +6388,7 @@
       <c r="B28" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C28" s="39"/>
       <c r="D28" s="9" t="s">
         <v>197</v>
       </c>
@@ -6343,9 +6442,7 @@
       <c r="B29" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C29" s="39"/>
       <c r="D29" s="9" t="s">
         <v>205</v>
       </c>
@@ -6399,7 +6496,7 @@
       <c r="B30" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="9" t="s">
@@ -6455,9 +6552,7 @@
       <c r="B31" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C31" s="39"/>
       <c r="D31" s="9" t="s">
         <v>162</v>
       </c>
@@ -6511,7 +6606,7 @@
       <c r="B32" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="9" t="s">
@@ -6567,7 +6662,7 @@
       <c r="B33" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D33" s="9" t="s">
@@ -6623,9 +6718,7 @@
       <c r="B34" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C34" s="39"/>
       <c r="D34" s="9" t="s">
         <v>154</v>
       </c>
@@ -6663,7 +6756,7 @@
       <c r="B35" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="40" t="s">
         <v>20</v>
       </c>
       <c r="D35" s="9" t="s">
@@ -6719,7 +6812,7 @@
       <c r="B36" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="9" t="s">
@@ -6775,7 +6868,7 @@
       <c r="B37" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D37" s="9" t="s">
@@ -6831,7 +6924,7 @@
       <c r="B38" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D38" s="9" t="s">
@@ -6889,7 +6982,7 @@
       <c r="B39" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D39" s="9" t="s">
@@ -6945,7 +7038,7 @@
       <c r="B40" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D40" s="9" t="s">
@@ -7003,9 +7096,7 @@
       <c r="B41" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C41" s="39"/>
       <c r="D41" s="9" t="s">
         <v>286</v>
       </c>
@@ -7059,9 +7150,7 @@
       <c r="B42" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C42" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C42" s="39"/>
       <c r="D42" s="9" t="s">
         <v>37</v>
       </c>
@@ -7115,7 +7204,7 @@
       <c r="B43" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D43" s="9" t="s">
@@ -7171,7 +7260,7 @@
       <c r="B44" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -7227,9 +7316,7 @@
       <c r="B45" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C45" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C45" s="39"/>
       <c r="D45" s="9" t="s">
         <v>304</v>
       </c>
@@ -7283,9 +7370,7 @@
       <c r="B46" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C46" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C46" s="39"/>
       <c r="D46" s="9" t="s">
         <v>67</v>
       </c>
@@ -7339,9 +7424,7 @@
       <c r="B47" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C47" s="39"/>
       <c r="D47" s="9" t="s">
         <v>311</v>
       </c>
@@ -7395,7 +7478,7 @@
       <c r="B48" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D48" s="9" t="s">
@@ -7451,9 +7534,7 @@
       <c r="B49" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C49" s="39"/>
       <c r="D49" s="9" t="s">
         <v>320</v>
       </c>
@@ -7491,7 +7572,7 @@
       <c r="B50" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D50" s="9" t="s">
@@ -7531,7 +7612,7 @@
       <c r="B51" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D51" s="9" t="s">
@@ -7587,7 +7668,7 @@
       <c r="B52" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D52" s="9" t="s">
@@ -7643,7 +7724,7 @@
       <c r="B53" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D53" s="9" t="s">
@@ -7699,7 +7780,7 @@
       <c r="B54" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D54" s="9" t="s">
@@ -7755,7 +7836,7 @@
       <c r="B55" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D55" s="9" t="s">
@@ -7811,7 +7892,7 @@
       <c r="B56" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D56" s="9" t="s">
@@ -7851,7 +7932,7 @@
       <c r="B57" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D57" s="9" t="s">
@@ -7891,9 +7972,7 @@
       <c r="B58" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C58" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C58" s="39"/>
       <c r="D58" s="9" t="s">
         <v>361</v>
       </c>
@@ -7947,7 +8026,7 @@
       <c r="B59" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D59" s="9" t="s">
@@ -8003,9 +8082,7 @@
       <c r="B60" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C60" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C60" s="39"/>
       <c r="D60" s="9" t="s">
         <v>134</v>
       </c>
@@ -8059,9 +8136,7 @@
       <c r="B61" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C61" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C61" s="39"/>
       <c r="D61" s="9" t="s">
         <v>382</v>
       </c>
@@ -8115,9 +8190,7 @@
       <c r="B62" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C62" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C62" s="39"/>
       <c r="D62" s="9" t="s">
         <v>389</v>
       </c>
@@ -8171,7 +8244,7 @@
       <c r="B63" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D63" s="9" t="s">
@@ -8227,9 +8300,7 @@
       <c r="B64" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C64" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C64" s="39"/>
       <c r="D64" s="9" t="s">
         <v>298</v>
       </c>
@@ -8283,7 +8354,7 @@
       <c r="B65" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D65" s="9" t="s">
@@ -8339,9 +8410,7 @@
       <c r="B66" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C66" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C66" s="39"/>
       <c r="D66" s="9" t="s">
         <v>89</v>
       </c>
@@ -8397,7 +8466,7 @@
       <c r="B67" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D67" s="9" t="s">
@@ -8455,7 +8524,7 @@
       <c r="B68" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D68" s="9" t="s">
@@ -8513,7 +8582,7 @@
       <c r="B69" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="C69" s="40" t="s">
         <v>20</v>
       </c>
       <c r="D69" s="9" t="s">
@@ -8571,7 +8640,7 @@
       <c r="B70" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="C70" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D70" s="9" t="s">
@@ -8629,7 +8698,7 @@
       <c r="B71" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D71" s="9" t="s">
@@ -8685,7 +8754,7 @@
       <c r="B72" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D72" s="9" t="s">
@@ -8741,9 +8810,7 @@
       <c r="B73" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C73" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C73" s="39"/>
       <c r="D73" s="9" t="s">
         <v>162</v>
       </c>
@@ -8797,7 +8864,7 @@
       <c r="B74" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C74" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D74" s="9" t="s">
@@ -8853,9 +8920,7 @@
       <c r="B75" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C75" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C75" s="39"/>
       <c r="D75" s="9" t="s">
         <v>478</v>
       </c>
@@ -8909,9 +8974,7 @@
       <c r="B76" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C76" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C76" s="39"/>
       <c r="D76" s="9" t="s">
         <v>162</v>
       </c>
@@ -8965,7 +9028,7 @@
       <c r="B77" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C77" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D77" s="9" t="s">
@@ -9021,7 +9084,7 @@
       <c r="B78" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C78" s="8" t="s">
+      <c r="C78" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D78" s="9" t="s">
@@ -9069,7 +9132,7 @@
       <c r="B79" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C79" s="8" t="s">
+      <c r="C79" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D79" s="11">
@@ -9117,7 +9180,7 @@
       <c r="B80" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C80" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D80" s="11">
@@ -9157,7 +9220,7 @@
       <c r="B81" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C81" s="8" t="s">
+      <c r="C81" s="41" t="s">
         <v>20</v>
       </c>
       <c r="D81" s="11">
@@ -9213,7 +9276,7 @@
       <c r="B82" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C82" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D82" s="11">
@@ -9269,9 +9332,7 @@
       <c r="B83" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="C83" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C83" s="39"/>
       <c r="D83" s="9" t="s">
         <v>246</v>
       </c>
@@ -9325,9 +9386,7 @@
       <c r="B84" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="C84" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C84" s="39"/>
       <c r="D84" s="9" t="s">
         <v>260</v>
       </c>
@@ -9381,7 +9440,7 @@
       <c r="B85" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="C85" s="8" t="s">
+      <c r="C85" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D85" s="9" t="s">
@@ -9437,7 +9496,7 @@
       <c r="B86" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C86" s="8" t="s">
+      <c r="C86" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D86" s="9" t="s">
@@ -9493,7 +9552,7 @@
       <c r="B87" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C87" s="8" t="s">
+      <c r="C87" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D87" s="9" t="s">
@@ -9549,7 +9608,7 @@
       <c r="B88" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C88" s="8" t="s">
+      <c r="C88" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D88" s="9" t="s">
@@ -9605,7 +9664,7 @@
       <c r="B89" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C89" s="8" t="s">
+      <c r="C89" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D89" s="9" t="s">
@@ -9661,7 +9720,7 @@
       <c r="B90" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="8" t="s">
+      <c r="C90" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D90" s="9" t="s">
@@ -9717,7 +9776,7 @@
       <c r="B91" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="8" t="s">
+      <c r="C91" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D91" s="9" t="s">
@@ -9773,7 +9832,7 @@
       <c r="B92" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C92" s="8" t="s">
+      <c r="C92" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D92" s="9" t="s">
@@ -9829,7 +9888,7 @@
       <c r="B93" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C93" s="8" t="s">
+      <c r="C93" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D93" s="9" t="s">
@@ -9885,7 +9944,7 @@
       <c r="B94" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C94" s="8" t="s">
+      <c r="C94" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D94" s="9" t="s">
@@ -9925,7 +9984,7 @@
       <c r="B95" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C95" s="8" t="s">
+      <c r="C95" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D95" s="9" t="s">
@@ -9981,7 +10040,7 @@
       <c r="B96" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C96" s="8" t="s">
+      <c r="C96" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D96" s="9" t="s">
@@ -10037,7 +10096,7 @@
       <c r="B97" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C97" s="8" t="s">
+      <c r="C97" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D97" s="9" t="s">
@@ -10093,7 +10152,7 @@
       <c r="B98" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C98" s="8" t="s">
+      <c r="C98" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D98" s="9" t="s">
@@ -10149,7 +10208,7 @@
       <c r="B99" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C99" s="8" t="s">
+      <c r="C99" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D99" s="9" t="s">
@@ -10205,7 +10264,7 @@
       <c r="B100" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="C100" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D100" s="9" t="s">
@@ -10261,7 +10320,7 @@
       <c r="B101" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C101" s="8" t="s">
+      <c r="C101" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D101" s="9" t="s">
@@ -10317,7 +10376,7 @@
       <c r="B102" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C102" s="8" t="s">
+      <c r="C102" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D102" s="9" t="s">
@@ -10373,7 +10432,7 @@
       <c r="B103" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C103" s="8" t="s">
+      <c r="C103" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D103" s="9" t="s">
@@ -10429,7 +10488,7 @@
       <c r="B104" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C104" s="8" t="s">
+      <c r="C104" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D104" s="9" t="s">
@@ -10485,7 +10544,7 @@
       <c r="B105" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C105" s="8" t="s">
+      <c r="C105" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D105" s="9" t="s">
@@ -10541,7 +10600,7 @@
       <c r="B106" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C106" s="8" t="s">
+      <c r="C106" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D106" s="9" t="s">
@@ -10597,7 +10656,7 @@
       <c r="B107" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C107" s="8" t="s">
+      <c r="C107" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D107" s="9" t="s">
@@ -10637,7 +10696,7 @@
       <c r="B108" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C108" s="8" t="s">
+      <c r="C108" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D108" s="9" t="s">
@@ -10677,7 +10736,7 @@
       <c r="B109" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C109" s="8" t="s">
+      <c r="C109" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D109" s="9" t="s">
@@ -10717,7 +10776,7 @@
       <c r="B110" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C110" s="8" t="s">
+      <c r="C110" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D110" s="9" t="s">
@@ -10757,7 +10816,7 @@
       <c r="B111" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C111" s="8" t="s">
+      <c r="C111" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D111" s="9" t="s">
@@ -10797,7 +10856,7 @@
       <c r="B112" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C112" s="8" t="s">
+      <c r="C112" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D112" s="9" t="s">
@@ -10837,7 +10896,7 @@
       <c r="B113" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C113" s="8" t="s">
+      <c r="C113" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D113" s="9" t="s">
@@ -10877,7 +10936,7 @@
       <c r="B114" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C114" s="8" t="s">
+      <c r="C114" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D114" s="9" t="s">
@@ -10917,7 +10976,7 @@
       <c r="B115" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C115" s="8" t="s">
+      <c r="C115" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D115" s="9" t="s">
@@ -10957,7 +11016,7 @@
       <c r="B116" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C116" s="8" t="s">
+      <c r="C116" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D116" s="9" t="s">
@@ -10997,7 +11056,7 @@
       <c r="B117" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C117" s="8" t="s">
+      <c r="C117" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D117" s="9" t="s">
@@ -11037,7 +11096,7 @@
       <c r="B118" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C118" s="8" t="s">
+      <c r="C118" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D118" s="9" t="s">
@@ -11077,7 +11136,7 @@
       <c r="B119" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C119" s="8" t="s">
+      <c r="C119" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D119" s="9" t="s">
@@ -11117,7 +11176,7 @@
       <c r="B120" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C120" s="8" t="s">
+      <c r="C120" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D120" s="9" t="s">
@@ -11157,7 +11216,7 @@
       <c r="B121" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C121" s="8" t="s">
+      <c r="C121" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D121" s="9" t="s">
@@ -11197,7 +11256,7 @@
       <c r="B122" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C122" s="8" t="s">
+      <c r="C122" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D122" s="9" t="s">
@@ -11237,7 +11296,7 @@
       <c r="B123" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C123" s="8" t="s">
+      <c r="C123" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D123" s="9" t="s">
@@ -11277,7 +11336,7 @@
       <c r="B124" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C124" s="8" t="s">
+      <c r="C124" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D124" s="9" t="s">
@@ -11317,7 +11376,7 @@
       <c r="B125" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C125" s="8" t="s">
+      <c r="C125" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D125" s="9" t="s">
@@ -11357,7 +11416,7 @@
       <c r="B126" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C126" s="8" t="s">
+      <c r="C126" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D126" s="9" t="s">
@@ -11397,7 +11456,7 @@
       <c r="B127" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C127" s="8" t="s">
+      <c r="C127" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D127" s="9" t="s">
@@ -11437,7 +11496,7 @@
       <c r="B128" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C128" s="8" t="s">
+      <c r="C128" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D128" s="9" t="s">
@@ -11477,7 +11536,7 @@
       <c r="B129" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C129" s="8" t="s">
+      <c r="C129" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D129" s="9" t="s">
@@ -11517,7 +11576,7 @@
       <c r="B130" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C130" s="8" t="s">
+      <c r="C130" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D130" s="9" t="s">
@@ -11573,7 +11632,7 @@
       <c r="B131" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C131" s="8" t="s">
+      <c r="C131" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D131" s="9" t="s">
@@ -11629,7 +11688,7 @@
       <c r="B132" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C132" s="8" t="s">
+      <c r="C132" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D132" s="9" t="s">
@@ -11669,7 +11728,7 @@
       <c r="B133" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C133" s="8" t="s">
+      <c r="C133" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D133" s="9" t="s">
@@ -11709,7 +11768,7 @@
       <c r="B134" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C134" s="8" t="s">
+      <c r="C134" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D134" s="9" t="s">
@@ -11765,7 +11824,7 @@
       <c r="B135" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C135" s="8" t="s">
+      <c r="C135" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D135" s="9" t="s">
@@ -11805,7 +11864,7 @@
       <c r="B136" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C136" s="8" t="s">
+      <c r="C136" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D136" s="9" t="s">
@@ -11845,7 +11904,7 @@
       <c r="B137" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C137" s="8" t="s">
+      <c r="C137" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D137" s="9" t="s">
@@ -11901,7 +11960,7 @@
       <c r="B138" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C138" s="8" t="s">
+      <c r="C138" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D138" s="9" t="s">
@@ -11941,7 +12000,7 @@
       <c r="B139" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C139" s="8" t="s">
+      <c r="C139" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D139" s="9" t="s">
@@ -11997,7 +12056,7 @@
       <c r="B140" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C140" s="8" t="s">
+      <c r="C140" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D140" s="9" t="s">
@@ -12053,7 +12112,7 @@
       <c r="B141" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C141" s="8" t="s">
+      <c r="C141" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D141" s="9" t="s">
@@ -12109,7 +12168,7 @@
       <c r="B142" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C142" s="8" t="s">
+      <c r="C142" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D142" s="9" t="s">
@@ -12149,7 +12208,7 @@
       <c r="B143" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C143" s="8" t="s">
+      <c r="C143" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D143" s="9" t="s">
@@ -12205,7 +12264,7 @@
       <c r="B144" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C144" s="8" t="s">
+      <c r="C144" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D144" s="9" t="s">
@@ -12261,7 +12320,7 @@
       <c r="B145" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C145" s="8" t="s">
+      <c r="C145" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D145" s="9" t="s">
@@ -12301,7 +12360,7 @@
       <c r="B146" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C146" s="8" t="s">
+      <c r="C146" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D146" s="9" t="s">
@@ -12357,7 +12416,7 @@
       <c r="B147" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C147" s="8" t="s">
+      <c r="C147" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D147" s="9" t="s">
@@ -12413,7 +12472,7 @@
       <c r="B148" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C148" s="8" t="s">
+      <c r="C148" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D148" s="9" t="s">
@@ -12469,7 +12528,7 @@
       <c r="B149" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C149" s="8" t="s">
+      <c r="C149" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D149" s="9" t="s">
@@ -12525,7 +12584,7 @@
       <c r="B150" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C150" s="8" t="s">
+      <c r="C150" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D150" s="9" t="s">
@@ -12581,7 +12640,7 @@
       <c r="B151" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C151" s="8" t="s">
+      <c r="C151" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D151" s="9" t="s">
@@ -12634,7 +12693,7 @@
       <c r="B152" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C152" s="8" t="s">
+      <c r="C152" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D152" s="9" t="s">
@@ -12674,7 +12733,7 @@
       <c r="B153" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C153" s="8" t="s">
+      <c r="C153" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D153" s="9" t="s">
@@ -12730,7 +12789,7 @@
       <c r="B154" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C154" s="8" t="s">
+      <c r="C154" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D154" s="9" t="s">
@@ -12770,7 +12829,7 @@
       <c r="B155" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C155" s="8" t="s">
+      <c r="C155" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D155" s="9" t="s">
@@ -12826,7 +12885,7 @@
       <c r="B156" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C156" s="8" t="s">
+      <c r="C156" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D156" s="9" t="s">
@@ -12882,7 +12941,7 @@
       <c r="B157" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C157" s="8" t="s">
+      <c r="C157" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D157" s="9" t="s">
@@ -12938,7 +12997,7 @@
       <c r="B158" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C158" s="8" t="s">
+      <c r="C158" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D158" s="9" t="s">
@@ -12994,7 +13053,7 @@
       <c r="B159" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C159" s="8" t="s">
+      <c r="C159" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D159" s="9" t="s">
@@ -13050,7 +13109,7 @@
       <c r="B160" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C160" s="8" t="s">
+      <c r="C160" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D160" s="9" t="s">
@@ -13106,7 +13165,7 @@
       <c r="B161" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C161" s="8" t="s">
+      <c r="C161" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D161" s="9" t="s">
@@ -13162,7 +13221,7 @@
       <c r="B162" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C162" s="8" t="s">
+      <c r="C162" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D162" s="9" t="s">
@@ -13202,7 +13261,7 @@
       <c r="B163" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C163" s="8" t="s">
+      <c r="C163" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D163" s="9" t="s">
@@ -13242,7 +13301,7 @@
       <c r="B164" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C164" s="8" t="s">
+      <c r="C164" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D164" s="9" t="s">
@@ -13282,7 +13341,7 @@
       <c r="B165" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C165" s="8" t="s">
+      <c r="C165" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D165" s="9" t="s">
@@ -13322,7 +13381,7 @@
       <c r="B166" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C166" s="8" t="s">
+      <c r="C166" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D166" s="9" t="s">
@@ -13362,7 +13421,7 @@
       <c r="B167" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C167" s="8" t="s">
+      <c r="C167" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D167" s="9" t="s">
@@ -13402,7 +13461,7 @@
       <c r="B168" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C168" s="8" t="s">
+      <c r="C168" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D168" s="9" t="s">
@@ -13458,7 +13517,7 @@
       <c r="B169" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C169" s="8" t="s">
+      <c r="C169" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D169" s="9" t="s">
@@ -13514,7 +13573,7 @@
       <c r="B170" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C170" s="8" t="s">
+      <c r="C170" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D170" s="9" t="s">
@@ -13554,7 +13613,7 @@
       <c r="B171" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C171" s="8" t="s">
+      <c r="C171" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D171" s="9" t="s">
@@ -13594,7 +13653,7 @@
       <c r="B172" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C172" s="8" t="s">
+      <c r="C172" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D172" s="9" t="s">
@@ -13634,7 +13693,7 @@
       <c r="B173" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C173" s="8" t="s">
+      <c r="C173" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D173" s="9" t="s">
@@ -13674,7 +13733,7 @@
       <c r="B174" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C174" s="8" t="s">
+      <c r="C174" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D174" s="9" t="s">
@@ -13714,7 +13773,7 @@
       <c r="B175" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C175" s="8" t="s">
+      <c r="C175" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D175" s="9" t="s">
@@ -13754,7 +13813,7 @@
       <c r="B176" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C176" s="8" t="s">
+      <c r="C176" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D176" s="9" t="s">
@@ -13794,7 +13853,7 @@
       <c r="B177" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C177" s="8" t="s">
+      <c r="C177" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D177" s="9" t="s">
@@ -13834,7 +13893,7 @@
       <c r="B178" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C178" s="8" t="s">
+      <c r="C178" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D178" s="9" t="s">
@@ -13890,7 +13949,7 @@
       <c r="B179" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C179" s="8" t="s">
+      <c r="C179" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D179" s="9" t="s">
@@ -13946,7 +14005,7 @@
       <c r="B180" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C180" s="8" t="s">
+      <c r="C180" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D180" s="9" t="s">
@@ -13986,7 +14045,7 @@
       <c r="B181" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C181" s="8" t="s">
+      <c r="C181" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D181" s="9" t="s">
@@ -14026,7 +14085,7 @@
       <c r="B182" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C182" s="8" t="s">
+      <c r="C182" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D182" s="9" t="s">
@@ -14066,7 +14125,7 @@
       <c r="B183" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C183" s="8" t="s">
+      <c r="C183" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D183" s="9" t="s">
@@ -14102,7 +14161,7 @@
     <row r="184" spans="1:26" ht="12.75" customHeight="1">
       <c r="A184" s="8"/>
       <c r="B184" s="8"/>
-      <c r="C184" s="8"/>
+      <c r="C184" s="39"/>
       <c r="D184" s="8"/>
       <c r="E184" s="8"/>
       <c r="G184" s="8"/>
@@ -14129,7 +14188,7 @@
     <row r="185" spans="1:26" ht="12.75" customHeight="1">
       <c r="A185" s="8"/>
       <c r="B185" s="8"/>
-      <c r="C185" s="8"/>
+      <c r="C185" s="39"/>
       <c r="D185" s="8"/>
       <c r="E185" s="8"/>
       <c r="G185" s="8"/>
@@ -14156,7 +14215,7 @@
     <row r="186" spans="1:26" ht="12.75" customHeight="1">
       <c r="A186" s="8"/>
       <c r="B186" s="8"/>
-      <c r="C186" s="8"/>
+      <c r="C186" s="39"/>
       <c r="D186" s="8"/>
       <c r="E186" s="8"/>
       <c r="G186" s="8"/>
@@ -14183,7 +14242,7 @@
     <row r="187" spans="1:26" ht="12.75" customHeight="1">
       <c r="A187" s="8"/>
       <c r="B187" s="8"/>
-      <c r="C187" s="8"/>
+      <c r="C187" s="39"/>
       <c r="D187" s="8"/>
       <c r="E187" s="8"/>
       <c r="G187" s="8"/>
@@ -14210,7 +14269,7 @@
     <row r="188" spans="1:26" ht="12.75" customHeight="1">
       <c r="A188" s="8"/>
       <c r="B188" s="8"/>
-      <c r="C188" s="8"/>
+      <c r="C188" s="39"/>
       <c r="D188" s="8"/>
       <c r="E188" s="8"/>
       <c r="G188" s="8"/>
@@ -14237,7 +14296,7 @@
     <row r="189" spans="1:26" ht="12.75" customHeight="1">
       <c r="A189" s="8"/>
       <c r="B189" s="8"/>
-      <c r="C189" s="8"/>
+      <c r="C189" s="39"/>
       <c r="D189" s="10"/>
       <c r="E189" s="8"/>
       <c r="G189" s="8"/>
@@ -14264,7 +14323,7 @@
     <row r="190" spans="1:26" ht="12.75" customHeight="1">
       <c r="A190" s="8"/>
       <c r="B190" s="8"/>
-      <c r="C190" s="8"/>
+      <c r="C190" s="39"/>
       <c r="D190" s="8"/>
       <c r="E190" s="8"/>
       <c r="G190" s="8"/>
@@ -14291,7 +14350,7 @@
     <row r="191" spans="1:26" ht="12.75" customHeight="1">
       <c r="A191" s="8"/>
       <c r="B191" s="8"/>
-      <c r="C191" s="8"/>
+      <c r="C191" s="39"/>
       <c r="D191" s="8"/>
       <c r="E191" s="8"/>
       <c r="G191" s="8"/>
@@ -14318,7 +14377,7 @@
     <row r="192" spans="1:26" ht="12.75" customHeight="1">
       <c r="A192" s="8"/>
       <c r="B192" s="8"/>
-      <c r="C192" s="8"/>
+      <c r="C192" s="39"/>
       <c r="D192" s="8"/>
       <c r="E192" s="8"/>
       <c r="G192" s="8"/>
@@ -14345,7 +14404,7 @@
     <row r="193" spans="1:26" ht="12.75" customHeight="1">
       <c r="A193" s="8"/>
       <c r="B193" s="8"/>
-      <c r="C193" s="8"/>
+      <c r="C193" s="39"/>
       <c r="D193" s="8"/>
       <c r="E193" s="8"/>
       <c r="G193" s="8"/>
@@ -14372,7 +14431,7 @@
     <row r="194" spans="1:26" ht="12.75" customHeight="1">
       <c r="A194" s="8"/>
       <c r="B194" s="8"/>
-      <c r="C194" s="8"/>
+      <c r="C194" s="39"/>
       <c r="D194" s="8"/>
       <c r="E194" s="8"/>
       <c r="G194" s="8"/>
@@ -14399,7 +14458,7 @@
     <row r="195" spans="1:26" ht="12.75" customHeight="1">
       <c r="A195" s="8"/>
       <c r="B195" s="8"/>
-      <c r="C195" s="8"/>
+      <c r="C195" s="39"/>
       <c r="D195" s="8"/>
       <c r="E195" s="8"/>
       <c r="G195" s="8"/>
@@ -14426,7 +14485,7 @@
     <row r="196" spans="1:26" ht="12.75" customHeight="1">
       <c r="A196" s="8"/>
       <c r="B196" s="8"/>
-      <c r="C196" s="8"/>
+      <c r="C196" s="39"/>
       <c r="D196" s="8"/>
       <c r="E196" s="8"/>
       <c r="G196" s="8"/>
@@ -14453,7 +14512,7 @@
     <row r="197" spans="1:26" ht="12.75" customHeight="1">
       <c r="A197" s="8"/>
       <c r="B197" s="8"/>
-      <c r="C197" s="8"/>
+      <c r="C197" s="39"/>
       <c r="D197" s="8"/>
       <c r="E197" s="8"/>
       <c r="G197" s="8"/>
@@ -14480,7 +14539,7 @@
     <row r="198" spans="1:26" ht="12.75" customHeight="1">
       <c r="A198" s="8"/>
       <c r="B198" s="8"/>
-      <c r="C198" s="8"/>
+      <c r="C198" s="39"/>
       <c r="D198" s="8"/>
       <c r="E198" s="8"/>
       <c r="G198" s="8"/>
@@ -14507,7 +14566,7 @@
     <row r="199" spans="1:26" ht="12.75" customHeight="1">
       <c r="A199" s="8"/>
       <c r="B199" s="8"/>
-      <c r="C199" s="8"/>
+      <c r="C199" s="39"/>
       <c r="D199" s="8"/>
       <c r="E199" s="8"/>
       <c r="G199" s="8"/>
@@ -14534,7 +14593,7 @@
     <row r="200" spans="1:26" ht="12.75" customHeight="1">
       <c r="A200" s="8"/>
       <c r="B200" s="8"/>
-      <c r="C200" s="8"/>
+      <c r="C200" s="39"/>
       <c r="D200" s="8"/>
       <c r="E200" s="8"/>
       <c r="G200" s="8"/>
@@ -14561,7 +14620,7 @@
     <row r="201" spans="1:26" ht="12.75" customHeight="1">
       <c r="A201" s="8"/>
       <c r="B201" s="8"/>
-      <c r="C201" s="8"/>
+      <c r="C201" s="39"/>
       <c r="D201" s="8"/>
       <c r="E201" s="8"/>
       <c r="G201" s="8"/>
@@ -14588,7 +14647,7 @@
     <row r="202" spans="1:26" ht="12.75" customHeight="1">
       <c r="A202" s="8"/>
       <c r="B202" s="8"/>
-      <c r="C202" s="8"/>
+      <c r="C202" s="39"/>
       <c r="D202" s="8"/>
       <c r="E202" s="8"/>
       <c r="G202" s="8"/>
@@ -14615,7 +14674,7 @@
     <row r="203" spans="1:26" ht="12.75" customHeight="1">
       <c r="A203" s="8"/>
       <c r="B203" s="8"/>
-      <c r="C203" s="8"/>
+      <c r="C203" s="39"/>
       <c r="D203" s="8"/>
       <c r="E203" s="8"/>
       <c r="G203" s="8"/>
@@ -14642,7 +14701,7 @@
     <row r="204" spans="1:26" ht="12.75" customHeight="1">
       <c r="A204" s="8"/>
       <c r="B204" s="8"/>
-      <c r="C204" s="8"/>
+      <c r="C204" s="39"/>
       <c r="D204" s="8"/>
       <c r="E204" s="8"/>
       <c r="G204" s="8"/>
@@ -14669,7 +14728,7 @@
     <row r="205" spans="1:26" ht="12.75" customHeight="1">
       <c r="A205" s="8"/>
       <c r="B205" s="8"/>
-      <c r="C205" s="8"/>
+      <c r="C205" s="39"/>
       <c r="D205" s="8"/>
       <c r="E205" s="8"/>
       <c r="G205" s="8"/>
@@ -14696,7 +14755,7 @@
     <row r="206" spans="1:26" ht="12.75" customHeight="1">
       <c r="A206" s="8"/>
       <c r="B206" s="8"/>
-      <c r="C206" s="8"/>
+      <c r="C206" s="39"/>
       <c r="D206" s="8"/>
       <c r="E206" s="8"/>
       <c r="G206" s="8"/>
@@ -14723,7 +14782,7 @@
     <row r="207" spans="1:26" ht="12.75" customHeight="1">
       <c r="A207" s="8"/>
       <c r="B207" s="8"/>
-      <c r="C207" s="8"/>
+      <c r="C207" s="39"/>
       <c r="D207" s="8"/>
       <c r="E207" s="8"/>
       <c r="G207" s="8"/>
@@ -14750,7 +14809,7 @@
     <row r="208" spans="1:26" ht="12.75" customHeight="1">
       <c r="A208" s="8"/>
       <c r="B208" s="8"/>
-      <c r="C208" s="8"/>
+      <c r="C208" s="39"/>
       <c r="D208" s="8"/>
       <c r="E208" s="8"/>
       <c r="G208" s="8"/>
@@ -14777,7 +14836,7 @@
     <row r="209" spans="1:26" ht="12.75" customHeight="1">
       <c r="A209" s="8"/>
       <c r="B209" s="8"/>
-      <c r="C209" s="8"/>
+      <c r="C209" s="39"/>
       <c r="D209" s="8"/>
       <c r="E209" s="8"/>
       <c r="G209" s="8"/>
@@ -14804,7 +14863,7 @@
     <row r="210" spans="1:26" ht="12.75" customHeight="1">
       <c r="A210" s="8"/>
       <c r="B210" s="8"/>
-      <c r="C210" s="8"/>
+      <c r="C210" s="39"/>
       <c r="D210" s="8"/>
       <c r="E210" s="8"/>
       <c r="G210" s="8"/>
@@ -14831,7 +14890,7 @@
     <row r="211" spans="1:26" ht="12.75" customHeight="1">
       <c r="A211" s="8"/>
       <c r="B211" s="8"/>
-      <c r="C211" s="8"/>
+      <c r="C211" s="39"/>
       <c r="D211" s="8"/>
       <c r="E211" s="8"/>
       <c r="G211" s="8"/>
@@ -14858,7 +14917,7 @@
     <row r="212" spans="1:26" ht="12.75" customHeight="1">
       <c r="A212" s="8"/>
       <c r="B212" s="8"/>
-      <c r="C212" s="8"/>
+      <c r="C212" s="39"/>
       <c r="D212" s="8"/>
       <c r="E212" s="8"/>
       <c r="G212" s="8"/>
@@ -14885,7 +14944,7 @@
     <row r="213" spans="1:26" ht="12.75" customHeight="1">
       <c r="A213" s="8"/>
       <c r="B213" s="8"/>
-      <c r="C213" s="8"/>
+      <c r="C213" s="39"/>
       <c r="D213" s="8"/>
       <c r="E213" s="8"/>
       <c r="G213" s="8"/>
@@ -14912,7 +14971,7 @@
     <row r="214" spans="1:26" ht="12.75" customHeight="1">
       <c r="A214" s="8"/>
       <c r="B214" s="8"/>
-      <c r="C214" s="8"/>
+      <c r="C214" s="39"/>
       <c r="D214" s="8"/>
       <c r="E214" s="8"/>
       <c r="G214" s="8"/>
@@ -14939,7 +14998,7 @@
     <row r="215" spans="1:26" ht="12.75" customHeight="1">
       <c r="A215" s="8"/>
       <c r="B215" s="8"/>
-      <c r="C215" s="8"/>
+      <c r="C215" s="39"/>
       <c r="D215" s="8"/>
       <c r="E215" s="8"/>
       <c r="G215" s="8"/>
@@ -14966,7 +15025,7 @@
     <row r="216" spans="1:26" ht="12.75" customHeight="1">
       <c r="A216" s="8"/>
       <c r="B216" s="8"/>
-      <c r="C216" s="8"/>
+      <c r="C216" s="39"/>
       <c r="D216" s="8"/>
       <c r="E216" s="8"/>
       <c r="G216" s="8"/>
@@ -14993,7 +15052,7 @@
     <row r="217" spans="1:26" ht="12.75" customHeight="1">
       <c r="A217" s="8"/>
       <c r="B217" s="8"/>
-      <c r="C217" s="8"/>
+      <c r="C217" s="39"/>
       <c r="D217" s="8"/>
       <c r="E217" s="8"/>
       <c r="G217" s="8"/>
@@ -15020,7 +15079,7 @@
     <row r="218" spans="1:26" ht="12.75" customHeight="1">
       <c r="A218" s="8"/>
       <c r="B218" s="8"/>
-      <c r="C218" s="8"/>
+      <c r="C218" s="39"/>
       <c r="D218" s="8"/>
       <c r="E218" s="8"/>
       <c r="G218" s="8"/>
@@ -15047,7 +15106,7 @@
     <row r="219" spans="1:26" ht="12.75" customHeight="1">
       <c r="A219" s="8"/>
       <c r="B219" s="8"/>
-      <c r="C219" s="8"/>
+      <c r="C219" s="39"/>
       <c r="D219" s="8"/>
       <c r="E219" s="8"/>
       <c r="G219" s="8"/>
@@ -15074,7 +15133,7 @@
     <row r="220" spans="1:26" ht="12.75" customHeight="1">
       <c r="A220" s="8"/>
       <c r="B220" s="8"/>
-      <c r="C220" s="8"/>
+      <c r="C220" s="39"/>
       <c r="D220" s="8"/>
       <c r="E220" s="8"/>
       <c r="G220" s="8"/>
@@ -15101,7 +15160,7 @@
     <row r="221" spans="1:26" ht="12.75" customHeight="1">
       <c r="A221" s="8"/>
       <c r="B221" s="8"/>
-      <c r="C221" s="8"/>
+      <c r="C221" s="39"/>
       <c r="D221" s="8"/>
       <c r="E221" s="8"/>
       <c r="G221" s="8"/>
@@ -15128,7 +15187,7 @@
     <row r="222" spans="1:26" ht="12.75" customHeight="1">
       <c r="A222" s="8"/>
       <c r="B222" s="8"/>
-      <c r="C222" s="8"/>
+      <c r="C222" s="39"/>
       <c r="D222" s="8"/>
       <c r="E222" s="8"/>
       <c r="G222" s="8"/>
@@ -15155,7 +15214,7 @@
     <row r="223" spans="1:26" ht="12.75" customHeight="1">
       <c r="A223" s="8"/>
       <c r="B223" s="8"/>
-      <c r="C223" s="8"/>
+      <c r="C223" s="39"/>
       <c r="D223" s="8"/>
       <c r="E223" s="8"/>
       <c r="G223" s="8"/>
@@ -15182,7 +15241,7 @@
     <row r="224" spans="1:26" ht="12.75" customHeight="1">
       <c r="A224" s="8"/>
       <c r="B224" s="8"/>
-      <c r="C224" s="8"/>
+      <c r="C224" s="39"/>
       <c r="D224" s="8"/>
       <c r="E224" s="8"/>
       <c r="G224" s="8"/>
@@ -15209,7 +15268,7 @@
     <row r="225" spans="1:26" ht="12.75" customHeight="1">
       <c r="A225" s="8"/>
       <c r="B225" s="8"/>
-      <c r="C225" s="8"/>
+      <c r="C225" s="39"/>
       <c r="D225" s="8"/>
       <c r="E225" s="8"/>
       <c r="G225" s="8"/>
@@ -15236,7 +15295,7 @@
     <row r="226" spans="1:26" ht="12.75" customHeight="1">
       <c r="A226" s="8"/>
       <c r="B226" s="8"/>
-      <c r="C226" s="8"/>
+      <c r="C226" s="39"/>
       <c r="D226" s="8"/>
       <c r="E226" s="8"/>
       <c r="G226" s="8"/>
@@ -15263,7 +15322,7 @@
     <row r="227" spans="1:26" ht="12.75" customHeight="1">
       <c r="A227" s="8"/>
       <c r="B227" s="8"/>
-      <c r="C227" s="8"/>
+      <c r="C227" s="39"/>
       <c r="D227" s="8"/>
       <c r="E227" s="8"/>
       <c r="G227" s="8"/>
@@ -15290,7 +15349,7 @@
     <row r="228" spans="1:26" ht="12.75" customHeight="1">
       <c r="A228" s="8"/>
       <c r="B228" s="8"/>
-      <c r="C228" s="8"/>
+      <c r="C228" s="39"/>
       <c r="D228" s="8"/>
       <c r="E228" s="8"/>
       <c r="G228" s="8"/>
@@ -15317,7 +15376,7 @@
     <row r="229" spans="1:26" ht="12.75" customHeight="1">
       <c r="A229" s="8"/>
       <c r="B229" s="8"/>
-      <c r="C229" s="8"/>
+      <c r="C229" s="39"/>
       <c r="D229" s="8"/>
       <c r="E229" s="8"/>
       <c r="G229" s="8"/>
@@ -15344,7 +15403,7 @@
     <row r="230" spans="1:26" ht="12.75" customHeight="1">
       <c r="A230" s="8"/>
       <c r="B230" s="8"/>
-      <c r="C230" s="8"/>
+      <c r="C230" s="39"/>
       <c r="D230" s="8"/>
       <c r="E230" s="8"/>
       <c r="G230" s="8"/>
@@ -15371,7 +15430,7 @@
     <row r="231" spans="1:26" ht="12.75" customHeight="1">
       <c r="A231" s="8"/>
       <c r="B231" s="8"/>
-      <c r="C231" s="8"/>
+      <c r="C231" s="39"/>
       <c r="D231" s="8"/>
       <c r="E231" s="8"/>
       <c r="G231" s="8"/>
@@ -15398,7 +15457,7 @@
     <row r="232" spans="1:26" ht="12.75" customHeight="1">
       <c r="A232" s="8"/>
       <c r="B232" s="8"/>
-      <c r="C232" s="8"/>
+      <c r="C232" s="39"/>
       <c r="D232" s="8"/>
       <c r="E232" s="8"/>
       <c r="G232" s="8"/>
@@ -15425,7 +15484,7 @@
     <row r="233" spans="1:26" ht="12.75" customHeight="1">
       <c r="A233" s="8"/>
       <c r="B233" s="8"/>
-      <c r="C233" s="8"/>
+      <c r="C233" s="39"/>
       <c r="D233" s="8"/>
       <c r="E233" s="8"/>
       <c r="G233" s="8"/>
@@ -15452,7 +15511,7 @@
     <row r="234" spans="1:26" ht="12.75" customHeight="1">
       <c r="A234" s="8"/>
       <c r="B234" s="8"/>
-      <c r="C234" s="8"/>
+      <c r="C234" s="39"/>
       <c r="D234" s="8"/>
       <c r="E234" s="8"/>
       <c r="G234" s="8"/>
@@ -15479,7 +15538,7 @@
     <row r="235" spans="1:26" ht="12.75" customHeight="1">
       <c r="A235" s="8"/>
       <c r="B235" s="8"/>
-      <c r="C235" s="8"/>
+      <c r="C235" s="39"/>
       <c r="D235" s="8"/>
       <c r="E235" s="8"/>
       <c r="G235" s="8"/>
@@ -15506,7 +15565,7 @@
     <row r="236" spans="1:26" ht="12.75" customHeight="1">
       <c r="A236" s="8"/>
       <c r="B236" s="8"/>
-      <c r="C236" s="8"/>
+      <c r="C236" s="39"/>
       <c r="D236" s="8"/>
       <c r="E236" s="8"/>
       <c r="G236" s="8"/>
@@ -15533,7 +15592,7 @@
     <row r="237" spans="1:26" ht="12.75" customHeight="1">
       <c r="A237" s="8"/>
       <c r="B237" s="8"/>
-      <c r="C237" s="8"/>
+      <c r="C237" s="39"/>
       <c r="D237" s="8"/>
       <c r="E237" s="8"/>
       <c r="G237" s="8"/>
@@ -15560,7 +15619,7 @@
     <row r="238" spans="1:26" ht="12.75" customHeight="1">
       <c r="A238" s="8"/>
       <c r="B238" s="8"/>
-      <c r="C238" s="8"/>
+      <c r="C238" s="39"/>
       <c r="D238" s="8"/>
       <c r="E238" s="8"/>
       <c r="G238" s="8"/>
@@ -15587,7 +15646,7 @@
     <row r="239" spans="1:26" ht="12.75" customHeight="1">
       <c r="A239" s="8"/>
       <c r="B239" s="8"/>
-      <c r="C239" s="8"/>
+      <c r="C239" s="39"/>
       <c r="D239" s="8"/>
       <c r="E239" s="8"/>
       <c r="G239" s="8"/>
@@ -15614,7 +15673,7 @@
     <row r="240" spans="1:26" ht="12.75" customHeight="1">
       <c r="A240" s="8"/>
       <c r="B240" s="8"/>
-      <c r="C240" s="8"/>
+      <c r="C240" s="39"/>
       <c r="D240" s="8"/>
       <c r="E240" s="8"/>
       <c r="G240" s="8"/>
@@ -15641,7 +15700,7 @@
     <row r="241" spans="1:26" ht="12.75" customHeight="1">
       <c r="A241" s="8"/>
       <c r="B241" s="8"/>
-      <c r="C241" s="8"/>
+      <c r="C241" s="39"/>
       <c r="D241" s="8"/>
       <c r="E241" s="8"/>
       <c r="G241" s="8"/>
@@ -15668,7 +15727,7 @@
     <row r="242" spans="1:26" ht="12.75" customHeight="1">
       <c r="A242" s="8"/>
       <c r="B242" s="8"/>
-      <c r="C242" s="8"/>
+      <c r="C242" s="39"/>
       <c r="D242" s="8"/>
       <c r="E242" s="8"/>
       <c r="G242" s="8"/>
@@ -15695,7 +15754,7 @@
     <row r="243" spans="1:26" ht="12.75" customHeight="1">
       <c r="A243" s="8"/>
       <c r="B243" s="8"/>
-      <c r="C243" s="8"/>
+      <c r="C243" s="39"/>
       <c r="D243" s="8"/>
       <c r="E243" s="8"/>
       <c r="G243" s="8"/>
@@ -15722,7 +15781,7 @@
     <row r="244" spans="1:26" ht="12.75" customHeight="1">
       <c r="A244" s="8"/>
       <c r="B244" s="8"/>
-      <c r="C244" s="8"/>
+      <c r="C244" s="39"/>
       <c r="D244" s="8"/>
       <c r="E244" s="8"/>
       <c r="G244" s="8"/>
@@ -15749,7 +15808,7 @@
     <row r="245" spans="1:26" ht="12.75" customHeight="1">
       <c r="A245" s="8"/>
       <c r="B245" s="8"/>
-      <c r="C245" s="8"/>
+      <c r="C245" s="39"/>
       <c r="D245" s="8"/>
       <c r="E245" s="8"/>
       <c r="G245" s="8"/>
@@ -15776,7 +15835,7 @@
     <row r="246" spans="1:26" ht="12.75" customHeight="1">
       <c r="A246" s="8"/>
       <c r="B246" s="8"/>
-      <c r="C246" s="8"/>
+      <c r="C246" s="39"/>
       <c r="D246" s="8"/>
       <c r="E246" s="8"/>
       <c r="G246" s="8"/>
@@ -15803,7 +15862,7 @@
     <row r="247" spans="1:26" ht="12.75" customHeight="1">
       <c r="A247" s="8"/>
       <c r="B247" s="8"/>
-      <c r="C247" s="8"/>
+      <c r="C247" s="39"/>
       <c r="D247" s="8"/>
       <c r="E247" s="8"/>
       <c r="G247" s="8"/>
@@ -15830,7 +15889,7 @@
     <row r="248" spans="1:26" ht="12.75" customHeight="1">
       <c r="A248" s="8"/>
       <c r="B248" s="8"/>
-      <c r="C248" s="8"/>
+      <c r="C248" s="39"/>
       <c r="D248" s="8"/>
       <c r="E248" s="8"/>
       <c r="G248" s="8"/>
@@ -15857,7 +15916,7 @@
     <row r="249" spans="1:26" ht="12.75" customHeight="1">
       <c r="A249" s="8"/>
       <c r="B249" s="8"/>
-      <c r="C249" s="8"/>
+      <c r="C249" s="39"/>
       <c r="D249" s="8"/>
       <c r="E249" s="8"/>
       <c r="G249" s="8"/>
@@ -15884,7 +15943,7 @@
     <row r="250" spans="1:26" ht="12.75" customHeight="1">
       <c r="A250" s="8"/>
       <c r="B250" s="8"/>
-      <c r="C250" s="8"/>
+      <c r="C250" s="39"/>
       <c r="D250" s="8"/>
       <c r="E250" s="8"/>
       <c r="G250" s="8"/>
@@ -15911,7 +15970,7 @@
     <row r="251" spans="1:26" ht="12.75" customHeight="1">
       <c r="A251" s="8"/>
       <c r="B251" s="8"/>
-      <c r="C251" s="8"/>
+      <c r="C251" s="39"/>
       <c r="D251" s="8"/>
       <c r="E251" s="8"/>
       <c r="G251" s="8"/>
@@ -15938,7 +15997,7 @@
     <row r="252" spans="1:26" ht="12.75" customHeight="1">
       <c r="A252" s="8"/>
       <c r="B252" s="8"/>
-      <c r="C252" s="8"/>
+      <c r="C252" s="39"/>
       <c r="D252" s="8"/>
       <c r="E252" s="8"/>
       <c r="G252" s="8"/>
@@ -15965,7 +16024,7 @@
     <row r="253" spans="1:26" ht="12.75" customHeight="1">
       <c r="A253" s="12"/>
       <c r="B253" s="12"/>
-      <c r="C253" s="12"/>
+      <c r="C253" s="42"/>
       <c r="D253" s="12"/>
       <c r="E253" s="12"/>
       <c r="G253" s="12"/>
@@ -15992,7 +16051,7 @@
     <row r="254" spans="1:26" ht="12.75" customHeight="1">
       <c r="A254" s="12"/>
       <c r="B254" s="12"/>
-      <c r="C254" s="12"/>
+      <c r="C254" s="42"/>
       <c r="D254" s="12"/>
       <c r="E254" s="12"/>
       <c r="G254" s="12"/>
@@ -16019,7 +16078,7 @@
     <row r="255" spans="1:26" ht="12.75" customHeight="1">
       <c r="A255" s="12"/>
       <c r="B255" s="12"/>
-      <c r="C255" s="12"/>
+      <c r="C255" s="42"/>
       <c r="D255" s="12"/>
       <c r="E255" s="12"/>
       <c r="G255" s="12"/>
@@ -16046,7 +16105,7 @@
     <row r="256" spans="1:26" ht="12.75" customHeight="1">
       <c r="A256" s="12"/>
       <c r="B256" s="12"/>
-      <c r="C256" s="12"/>
+      <c r="C256" s="42"/>
       <c r="D256" s="12"/>
       <c r="E256" s="12"/>
       <c r="G256" s="12"/>
@@ -16073,7 +16132,7 @@
     <row r="257" spans="1:26" ht="12.75" customHeight="1">
       <c r="A257" s="12"/>
       <c r="B257" s="12"/>
-      <c r="C257" s="12"/>
+      <c r="C257" s="42"/>
       <c r="D257" s="12"/>
       <c r="E257" s="12"/>
       <c r="G257" s="12"/>
@@ -16100,7 +16159,7 @@
     <row r="258" spans="1:26" ht="12.75" customHeight="1">
       <c r="A258" s="12"/>
       <c r="B258" s="12"/>
-      <c r="C258" s="12"/>
+      <c r="C258" s="42"/>
       <c r="D258" s="12"/>
       <c r="E258" s="12"/>
       <c r="G258" s="12"/>
@@ -16127,7 +16186,7 @@
     <row r="259" spans="1:26" ht="12.75" customHeight="1">
       <c r="A259" s="12"/>
       <c r="B259" s="12"/>
-      <c r="C259" s="12"/>
+      <c r="C259" s="42"/>
       <c r="D259" s="12"/>
       <c r="E259" s="12"/>
       <c r="G259" s="12"/>
@@ -16154,7 +16213,7 @@
     <row r="260" spans="1:26" ht="12.75" customHeight="1">
       <c r="A260" s="12"/>
       <c r="B260" s="12"/>
-      <c r="C260" s="12"/>
+      <c r="C260" s="42"/>
       <c r="D260" s="12"/>
       <c r="E260" s="12"/>
       <c r="G260" s="12"/>
@@ -16181,7 +16240,7 @@
     <row r="261" spans="1:26" ht="12.75" customHeight="1">
       <c r="A261" s="12"/>
       <c r="B261" s="12"/>
-      <c r="C261" s="12"/>
+      <c r="C261" s="42"/>
       <c r="D261" s="12"/>
       <c r="E261" s="12"/>
       <c r="G261" s="12"/>
@@ -16208,7 +16267,7 @@
     <row r="262" spans="1:26" ht="12.75" customHeight="1">
       <c r="A262" s="12"/>
       <c r="B262" s="12"/>
-      <c r="C262" s="12"/>
+      <c r="C262" s="42"/>
       <c r="D262" s="12"/>
       <c r="E262" s="12"/>
       <c r="G262" s="12"/>
@@ -16235,7 +16294,7 @@
     <row r="263" spans="1:26" ht="12.75" customHeight="1">
       <c r="A263" s="12"/>
       <c r="B263" s="12"/>
-      <c r="C263" s="12"/>
+      <c r="C263" s="42"/>
       <c r="D263" s="12"/>
       <c r="E263" s="12"/>
       <c r="G263" s="12"/>
@@ -16262,7 +16321,7 @@
     <row r="264" spans="1:26" ht="12.75" customHeight="1">
       <c r="A264" s="12"/>
       <c r="B264" s="12"/>
-      <c r="C264" s="12"/>
+      <c r="C264" s="42"/>
       <c r="D264" s="12"/>
       <c r="E264" s="12"/>
       <c r="G264" s="12"/>
@@ -16289,7 +16348,7 @@
     <row r="265" spans="1:26" ht="12.75" customHeight="1">
       <c r="A265" s="12"/>
       <c r="B265" s="12"/>
-      <c r="C265" s="12"/>
+      <c r="C265" s="42"/>
       <c r="D265" s="12"/>
       <c r="E265" s="12"/>
       <c r="G265" s="12"/>
@@ -16316,7 +16375,7 @@
     <row r="266" spans="1:26" ht="12.75" customHeight="1">
       <c r="A266" s="12"/>
       <c r="B266" s="12"/>
-      <c r="C266" s="12"/>
+      <c r="C266" s="42"/>
       <c r="D266" s="12"/>
       <c r="E266" s="12"/>
       <c r="G266" s="12"/>
@@ -16343,7 +16402,7 @@
     <row r="267" spans="1:26" ht="12.75" customHeight="1">
       <c r="A267" s="12"/>
       <c r="B267" s="12"/>
-      <c r="C267" s="12"/>
+      <c r="C267" s="42"/>
       <c r="D267" s="12"/>
       <c r="E267" s="12"/>
       <c r="G267" s="12"/>
@@ -16370,7 +16429,7 @@
     <row r="268" spans="1:26" ht="12.75" customHeight="1">
       <c r="A268" s="12"/>
       <c r="B268" s="12"/>
-      <c r="C268" s="12"/>
+      <c r="C268" s="42"/>
       <c r="D268" s="12"/>
       <c r="E268" s="12"/>
       <c r="G268" s="12"/>
@@ -16397,7 +16456,7 @@
     <row r="269" spans="1:26" ht="12.75" customHeight="1">
       <c r="A269" s="12"/>
       <c r="B269" s="12"/>
-      <c r="C269" s="12"/>
+      <c r="C269" s="42"/>
       <c r="D269" s="12"/>
       <c r="E269" s="12"/>
       <c r="G269" s="12"/>
@@ -16424,7 +16483,7 @@
     <row r="270" spans="1:26" ht="12.75" customHeight="1">
       <c r="A270" s="12"/>
       <c r="B270" s="12"/>
-      <c r="C270" s="12"/>
+      <c r="C270" s="42"/>
       <c r="D270" s="12"/>
       <c r="E270" s="12"/>
       <c r="G270" s="12"/>
@@ -16451,7 +16510,7 @@
     <row r="271" spans="1:26" ht="12.75" customHeight="1">
       <c r="A271" s="12"/>
       <c r="B271" s="12"/>
-      <c r="C271" s="12"/>
+      <c r="C271" s="42"/>
       <c r="D271" s="12"/>
       <c r="E271" s="12"/>
       <c r="G271" s="12"/>
@@ -16478,7 +16537,7 @@
     <row r="272" spans="1:26" ht="12.75" customHeight="1">
       <c r="A272" s="12"/>
       <c r="B272" s="12"/>
-      <c r="C272" s="12"/>
+      <c r="C272" s="42"/>
       <c r="D272" s="12"/>
       <c r="E272" s="12"/>
       <c r="G272" s="12"/>
@@ -16505,7 +16564,7 @@
     <row r="273" spans="1:26" ht="12.75" customHeight="1">
       <c r="A273" s="12"/>
       <c r="B273" s="12"/>
-      <c r="C273" s="12"/>
+      <c r="C273" s="42"/>
       <c r="D273" s="12"/>
       <c r="E273" s="12"/>
       <c r="G273" s="12"/>
@@ -16532,7 +16591,7 @@
     <row r="274" spans="1:26" ht="12.75" customHeight="1">
       <c r="A274" s="12"/>
       <c r="B274" s="12"/>
-      <c r="C274" s="12"/>
+      <c r="C274" s="42"/>
       <c r="D274" s="12"/>
       <c r="E274" s="12"/>
       <c r="G274" s="12"/>
@@ -16559,7 +16618,7 @@
     <row r="275" spans="1:26" ht="12.75" customHeight="1">
       <c r="A275" s="12"/>
       <c r="B275" s="12"/>
-      <c r="C275" s="12"/>
+      <c r="C275" s="42"/>
       <c r="D275" s="12"/>
       <c r="E275" s="12"/>
       <c r="G275" s="12"/>
@@ -16586,7 +16645,7 @@
     <row r="276" spans="1:26" ht="12.75" customHeight="1">
       <c r="A276" s="12"/>
       <c r="B276" s="12"/>
-      <c r="C276" s="12"/>
+      <c r="C276" s="42"/>
       <c r="D276" s="12"/>
       <c r="E276" s="12"/>
       <c r="G276" s="12"/>
@@ -16613,7 +16672,7 @@
     <row r="277" spans="1:26" ht="12.75" customHeight="1">
       <c r="A277" s="12"/>
       <c r="B277" s="12"/>
-      <c r="C277" s="12"/>
+      <c r="C277" s="42"/>
       <c r="D277" s="12"/>
       <c r="E277" s="12"/>
       <c r="G277" s="12"/>
@@ -16640,7 +16699,7 @@
     <row r="278" spans="1:26" ht="12.75" customHeight="1">
       <c r="A278" s="12"/>
       <c r="B278" s="12"/>
-      <c r="C278" s="12"/>
+      <c r="C278" s="42"/>
       <c r="D278" s="12"/>
       <c r="E278" s="12"/>
       <c r="G278" s="12"/>
@@ -16667,7 +16726,7 @@
     <row r="279" spans="1:26" ht="12.75" customHeight="1">
       <c r="A279" s="12"/>
       <c r="B279" s="12"/>
-      <c r="C279" s="12"/>
+      <c r="C279" s="42"/>
       <c r="D279" s="12"/>
       <c r="E279" s="12"/>
       <c r="G279" s="12"/>
@@ -16694,7 +16753,7 @@
     <row r="280" spans="1:26" ht="12.75" customHeight="1">
       <c r="A280" s="12"/>
       <c r="B280" s="12"/>
-      <c r="C280" s="12"/>
+      <c r="C280" s="42"/>
       <c r="D280" s="12"/>
       <c r="E280" s="12"/>
       <c r="G280" s="12"/>
@@ -16721,7 +16780,7 @@
     <row r="281" spans="1:26" ht="12.75" customHeight="1">
       <c r="A281" s="12"/>
       <c r="B281" s="12"/>
-      <c r="C281" s="12"/>
+      <c r="C281" s="42"/>
       <c r="D281" s="12"/>
       <c r="E281" s="12"/>
       <c r="G281" s="12"/>
@@ -16748,7 +16807,7 @@
     <row r="282" spans="1:26" ht="12.75" customHeight="1">
       <c r="A282" s="12"/>
       <c r="B282" s="12"/>
-      <c r="C282" s="12"/>
+      <c r="C282" s="42"/>
       <c r="D282" s="12"/>
       <c r="E282" s="12"/>
       <c r="G282" s="12"/>
@@ -16775,7 +16834,7 @@
     <row r="283" spans="1:26" ht="12.75" customHeight="1">
       <c r="A283" s="12"/>
       <c r="B283" s="12"/>
-      <c r="C283" s="12"/>
+      <c r="C283" s="42"/>
       <c r="D283" s="12"/>
       <c r="E283" s="12"/>
       <c r="G283" s="12"/>
@@ -16802,7 +16861,7 @@
     <row r="284" spans="1:26" ht="12.75" customHeight="1">
       <c r="A284" s="12"/>
       <c r="B284" s="12"/>
-      <c r="C284" s="12"/>
+      <c r="C284" s="42"/>
       <c r="D284" s="12"/>
       <c r="E284" s="12"/>
       <c r="G284" s="12"/>
@@ -16829,7 +16888,7 @@
     <row r="285" spans="1:26" ht="12.75" customHeight="1">
       <c r="A285" s="12"/>
       <c r="B285" s="12"/>
-      <c r="C285" s="12"/>
+      <c r="C285" s="42"/>
       <c r="D285" s="12"/>
       <c r="E285" s="12"/>
       <c r="G285" s="12"/>
@@ -16856,7 +16915,7 @@
     <row r="286" spans="1:26" ht="12.75" customHeight="1">
       <c r="A286" s="12"/>
       <c r="B286" s="12"/>
-      <c r="C286" s="12"/>
+      <c r="C286" s="42"/>
       <c r="D286" s="12"/>
       <c r="E286" s="12"/>
       <c r="G286" s="12"/>
@@ -16883,7 +16942,7 @@
     <row r="287" spans="1:26" ht="12.75" customHeight="1">
       <c r="A287" s="12"/>
       <c r="B287" s="12"/>
-      <c r="C287" s="12"/>
+      <c r="C287" s="42"/>
       <c r="D287" s="12"/>
       <c r="E287" s="12"/>
       <c r="G287" s="12"/>
@@ -16910,7 +16969,7 @@
     <row r="288" spans="1:26" ht="12.75" customHeight="1">
       <c r="A288" s="12"/>
       <c r="B288" s="12"/>
-      <c r="C288" s="12"/>
+      <c r="C288" s="42"/>
       <c r="D288" s="12"/>
       <c r="E288" s="12"/>
       <c r="G288" s="12"/>
@@ -16937,7 +16996,7 @@
     <row r="289" spans="1:26" ht="12.75" customHeight="1">
       <c r="A289" s="12"/>
       <c r="B289" s="12"/>
-      <c r="C289" s="12"/>
+      <c r="C289" s="42"/>
       <c r="D289" s="12"/>
       <c r="E289" s="12"/>
       <c r="G289" s="12"/>
@@ -16964,7 +17023,7 @@
     <row r="290" spans="1:26" ht="12.75" customHeight="1">
       <c r="A290" s="12"/>
       <c r="B290" s="12"/>
-      <c r="C290" s="12"/>
+      <c r="C290" s="42"/>
       <c r="D290" s="12"/>
       <c r="E290" s="12"/>
       <c r="G290" s="12"/>
@@ -16991,7 +17050,7 @@
     <row r="291" spans="1:26" ht="12.75" customHeight="1">
       <c r="A291" s="12"/>
       <c r="B291" s="12"/>
-      <c r="C291" s="12"/>
+      <c r="C291" s="42"/>
       <c r="D291" s="12"/>
       <c r="E291" s="12"/>
       <c r="G291" s="12"/>
@@ -17018,7 +17077,7 @@
     <row r="292" spans="1:26" ht="12.75" customHeight="1">
       <c r="A292" s="12"/>
       <c r="B292" s="12"/>
-      <c r="C292" s="12"/>
+      <c r="C292" s="42"/>
       <c r="D292" s="12"/>
       <c r="E292" s="12"/>
       <c r="G292" s="12"/>
@@ -17045,7 +17104,7 @@
     <row r="293" spans="1:26" ht="12.75" customHeight="1">
       <c r="A293" s="12"/>
       <c r="B293" s="12"/>
-      <c r="C293" s="12"/>
+      <c r="C293" s="42"/>
       <c r="D293" s="12"/>
       <c r="E293" s="12"/>
       <c r="G293" s="12"/>
@@ -17072,7 +17131,7 @@
     <row r="294" spans="1:26" ht="12.75" customHeight="1">
       <c r="A294" s="12"/>
       <c r="B294" s="12"/>
-      <c r="C294" s="12"/>
+      <c r="C294" s="42"/>
       <c r="D294" s="12"/>
       <c r="E294" s="12"/>
       <c r="G294" s="12"/>
@@ -17099,7 +17158,7 @@
     <row r="295" spans="1:26" ht="12.75" customHeight="1">
       <c r="A295" s="12"/>
       <c r="B295" s="12"/>
-      <c r="C295" s="12"/>
+      <c r="C295" s="42"/>
       <c r="D295" s="12"/>
       <c r="E295" s="12"/>
       <c r="G295" s="12"/>
@@ -17126,7 +17185,7 @@
     <row r="296" spans="1:26" ht="12.75" customHeight="1">
       <c r="A296" s="12"/>
       <c r="B296" s="12"/>
-      <c r="C296" s="12"/>
+      <c r="C296" s="42"/>
       <c r="D296" s="12"/>
       <c r="E296" s="12"/>
       <c r="G296" s="12"/>
@@ -17153,7 +17212,7 @@
     <row r="297" spans="1:26" ht="12.75" customHeight="1">
       <c r="A297" s="12"/>
       <c r="B297" s="12"/>
-      <c r="C297" s="12"/>
+      <c r="C297" s="42"/>
       <c r="D297" s="12"/>
       <c r="E297" s="12"/>
       <c r="G297" s="12"/>
@@ -17180,7 +17239,7 @@
     <row r="298" spans="1:26" ht="12.75" customHeight="1">
       <c r="A298" s="12"/>
       <c r="B298" s="12"/>
-      <c r="C298" s="12"/>
+      <c r="C298" s="42"/>
       <c r="D298" s="12"/>
       <c r="E298" s="12"/>
       <c r="G298" s="12"/>
@@ -17207,7 +17266,7 @@
     <row r="299" spans="1:26" ht="12.75" customHeight="1">
       <c r="A299" s="12"/>
       <c r="B299" s="12"/>
-      <c r="C299" s="12"/>
+      <c r="C299" s="42"/>
       <c r="D299" s="12"/>
       <c r="E299" s="12"/>
       <c r="G299" s="12"/>
@@ -17234,7 +17293,7 @@
     <row r="300" spans="1:26" ht="12.75" customHeight="1">
       <c r="A300" s="12"/>
       <c r="B300" s="12"/>
-      <c r="C300" s="12"/>
+      <c r="C300" s="42"/>
       <c r="D300" s="12"/>
       <c r="E300" s="12"/>
       <c r="G300" s="12"/>
@@ -17261,7 +17320,7 @@
     <row r="301" spans="1:26" ht="12.75" customHeight="1">
       <c r="A301" s="12"/>
       <c r="B301" s="12"/>
-      <c r="C301" s="12"/>
+      <c r="C301" s="42"/>
       <c r="D301" s="12"/>
       <c r="E301" s="12"/>
       <c r="G301" s="12"/>
@@ -17288,7 +17347,7 @@
     <row r="302" spans="1:26" ht="12.75" customHeight="1">
       <c r="A302" s="12"/>
       <c r="B302" s="12"/>
-      <c r="C302" s="12"/>
+      <c r="C302" s="42"/>
       <c r="D302" s="12"/>
       <c r="E302" s="12"/>
       <c r="G302" s="12"/>
@@ -17315,7 +17374,7 @@
     <row r="303" spans="1:26" ht="12.75" customHeight="1">
       <c r="A303" s="12"/>
       <c r="B303" s="12"/>
-      <c r="C303" s="12"/>
+      <c r="C303" s="42"/>
       <c r="D303" s="12"/>
       <c r="E303" s="12"/>
       <c r="G303" s="12"/>
@@ -17342,7 +17401,7 @@
     <row r="304" spans="1:26" ht="12.75" customHeight="1">
       <c r="A304" s="12"/>
       <c r="B304" s="12"/>
-      <c r="C304" s="12"/>
+      <c r="C304" s="42"/>
       <c r="D304" s="12"/>
       <c r="E304" s="12"/>
       <c r="G304" s="12"/>
@@ -17369,7 +17428,7 @@
     <row r="305" spans="1:26" ht="12.75" customHeight="1">
       <c r="A305" s="12"/>
       <c r="B305" s="12"/>
-      <c r="C305" s="12"/>
+      <c r="C305" s="42"/>
       <c r="D305" s="12"/>
       <c r="E305" s="12"/>
       <c r="G305" s="12"/>
@@ -17396,7 +17455,7 @@
     <row r="306" spans="1:26" ht="12.75" customHeight="1">
       <c r="A306" s="12"/>
       <c r="B306" s="12"/>
-      <c r="C306" s="12"/>
+      <c r="C306" s="42"/>
       <c r="D306" s="12"/>
       <c r="E306" s="12"/>
       <c r="G306" s="12"/>
@@ -17423,7 +17482,7 @@
     <row r="307" spans="1:26" ht="12.75" customHeight="1">
       <c r="A307" s="12"/>
       <c r="B307" s="12"/>
-      <c r="C307" s="12"/>
+      <c r="C307" s="42"/>
       <c r="D307" s="12"/>
       <c r="E307" s="12"/>
       <c r="G307" s="12"/>
@@ -17450,7 +17509,7 @@
     <row r="308" spans="1:26" ht="12.75" customHeight="1">
       <c r="A308" s="12"/>
       <c r="B308" s="12"/>
-      <c r="C308" s="12"/>
+      <c r="C308" s="42"/>
       <c r="D308" s="12"/>
       <c r="E308" s="12"/>
       <c r="G308" s="12"/>
@@ -17477,7 +17536,7 @@
     <row r="309" spans="1:26" ht="12.75" customHeight="1">
       <c r="A309" s="12"/>
       <c r="B309" s="12"/>
-      <c r="C309" s="12"/>
+      <c r="C309" s="42"/>
       <c r="D309" s="12"/>
       <c r="E309" s="12"/>
       <c r="G309" s="12"/>
@@ -17504,7 +17563,7 @@
     <row r="310" spans="1:26" ht="12.75" customHeight="1">
       <c r="A310" s="12"/>
       <c r="B310" s="12"/>
-      <c r="C310" s="12"/>
+      <c r="C310" s="42"/>
       <c r="D310" s="12"/>
       <c r="E310" s="12"/>
       <c r="G310" s="12"/>
@@ -17531,7 +17590,7 @@
     <row r="311" spans="1:26" ht="12.75" customHeight="1">
       <c r="A311" s="12"/>
       <c r="B311" s="12"/>
-      <c r="C311" s="12"/>
+      <c r="C311" s="42"/>
       <c r="D311" s="12"/>
       <c r="E311" s="12"/>
       <c r="G311" s="12"/>
@@ -17558,7 +17617,7 @@
     <row r="312" spans="1:26" ht="12.75" customHeight="1">
       <c r="A312" s="12"/>
       <c r="B312" s="12"/>
-      <c r="C312" s="12"/>
+      <c r="C312" s="42"/>
       <c r="D312" s="12"/>
       <c r="E312" s="12"/>
       <c r="G312" s="12"/>
@@ -17585,7 +17644,7 @@
     <row r="313" spans="1:26" ht="12.75" customHeight="1">
       <c r="A313" s="12"/>
       <c r="B313" s="12"/>
-      <c r="C313" s="12"/>
+      <c r="C313" s="42"/>
       <c r="D313" s="12"/>
       <c r="E313" s="12"/>
       <c r="G313" s="12"/>
@@ -17612,7 +17671,7 @@
     <row r="314" spans="1:26" ht="12.75" customHeight="1">
       <c r="A314" s="12"/>
       <c r="B314" s="12"/>
-      <c r="C314" s="12"/>
+      <c r="C314" s="42"/>
       <c r="D314" s="12"/>
       <c r="E314" s="12"/>
       <c r="G314" s="12"/>
@@ -17639,7 +17698,7 @@
     <row r="315" spans="1:26" ht="12.75" customHeight="1">
       <c r="A315" s="12"/>
       <c r="B315" s="12"/>
-      <c r="C315" s="12"/>
+      <c r="C315" s="42"/>
       <c r="D315" s="12"/>
       <c r="E315" s="12"/>
       <c r="G315" s="12"/>
@@ -17666,7 +17725,7 @@
     <row r="316" spans="1:26" ht="12.75" customHeight="1">
       <c r="A316" s="12"/>
       <c r="B316" s="12"/>
-      <c r="C316" s="12"/>
+      <c r="C316" s="42"/>
       <c r="D316" s="12"/>
       <c r="E316" s="12"/>
       <c r="G316" s="12"/>
@@ -17693,7 +17752,7 @@
     <row r="317" spans="1:26" ht="12.75" customHeight="1">
       <c r="A317" s="12"/>
       <c r="B317" s="12"/>
-      <c r="C317" s="12"/>
+      <c r="C317" s="42"/>
       <c r="D317" s="12"/>
       <c r="E317" s="12"/>
       <c r="G317" s="12"/>
@@ -17720,7 +17779,7 @@
     <row r="318" spans="1:26" ht="12.75" customHeight="1">
       <c r="A318" s="12"/>
       <c r="B318" s="12"/>
-      <c r="C318" s="12"/>
+      <c r="C318" s="42"/>
       <c r="D318" s="12"/>
       <c r="E318" s="12"/>
       <c r="G318" s="12"/>
@@ -17747,7 +17806,7 @@
     <row r="319" spans="1:26" ht="12.75" customHeight="1">
       <c r="A319" s="12"/>
       <c r="B319" s="12"/>
-      <c r="C319" s="12"/>
+      <c r="C319" s="42"/>
       <c r="D319" s="12"/>
       <c r="E319" s="12"/>
       <c r="G319" s="12"/>
@@ -17774,7 +17833,7 @@
     <row r="320" spans="1:26" ht="12.75" customHeight="1">
       <c r="A320" s="12"/>
       <c r="B320" s="12"/>
-      <c r="C320" s="12"/>
+      <c r="C320" s="42"/>
       <c r="D320" s="12"/>
       <c r="E320" s="12"/>
       <c r="G320" s="12"/>
@@ -17801,7 +17860,7 @@
     <row r="321" spans="1:26" ht="12.75" customHeight="1">
       <c r="A321" s="12"/>
       <c r="B321" s="12"/>
-      <c r="C321" s="12"/>
+      <c r="C321" s="42"/>
       <c r="D321" s="12"/>
       <c r="E321" s="12"/>
       <c r="G321" s="12"/>
@@ -17828,7 +17887,7 @@
     <row r="322" spans="1:26" ht="12.75" customHeight="1">
       <c r="A322" s="12"/>
       <c r="B322" s="12"/>
-      <c r="C322" s="12"/>
+      <c r="C322" s="42"/>
       <c r="D322" s="12"/>
       <c r="E322" s="12"/>
       <c r="G322" s="12"/>
@@ -17855,7 +17914,7 @@
     <row r="323" spans="1:26" ht="12.75" customHeight="1">
       <c r="A323" s="12"/>
       <c r="B323" s="12"/>
-      <c r="C323" s="12"/>
+      <c r="C323" s="42"/>
       <c r="D323" s="12"/>
       <c r="E323" s="12"/>
       <c r="G323" s="12"/>
@@ -17882,7 +17941,7 @@
     <row r="324" spans="1:26" ht="12.75" customHeight="1">
       <c r="A324" s="12"/>
       <c r="B324" s="12"/>
-      <c r="C324" s="12"/>
+      <c r="C324" s="42"/>
       <c r="D324" s="12"/>
       <c r="E324" s="12"/>
       <c r="G324" s="12"/>
@@ -17909,7 +17968,7 @@
     <row r="325" spans="1:26" ht="12.75" customHeight="1">
       <c r="A325" s="12"/>
       <c r="B325" s="12"/>
-      <c r="C325" s="12"/>
+      <c r="C325" s="42"/>
       <c r="D325" s="12"/>
       <c r="E325" s="12"/>
       <c r="G325" s="12"/>
@@ -17936,7 +17995,7 @@
     <row r="326" spans="1:26" ht="12.75" customHeight="1">
       <c r="A326" s="12"/>
       <c r="B326" s="12"/>
-      <c r="C326" s="12"/>
+      <c r="C326" s="42"/>
       <c r="D326" s="12"/>
       <c r="E326" s="12"/>
       <c r="G326" s="12"/>
@@ -17963,7 +18022,7 @@
     <row r="327" spans="1:26" ht="12.75" customHeight="1">
       <c r="A327" s="12"/>
       <c r="B327" s="12"/>
-      <c r="C327" s="12"/>
+      <c r="C327" s="42"/>
       <c r="D327" s="12"/>
       <c r="E327" s="12"/>
       <c r="G327" s="12"/>
@@ -17990,7 +18049,7 @@
     <row r="328" spans="1:26" ht="12.75" customHeight="1">
       <c r="A328" s="12"/>
       <c r="B328" s="12"/>
-      <c r="C328" s="12"/>
+      <c r="C328" s="42"/>
       <c r="D328" s="12"/>
       <c r="E328" s="12"/>
       <c r="G328" s="12"/>
@@ -18017,7 +18076,7 @@
     <row r="329" spans="1:26" ht="12.75" customHeight="1">
       <c r="A329" s="12"/>
       <c r="B329" s="12"/>
-      <c r="C329" s="12"/>
+      <c r="C329" s="42"/>
       <c r="D329" s="12"/>
       <c r="E329" s="12"/>
       <c r="G329" s="12"/>
@@ -18044,7 +18103,7 @@
     <row r="330" spans="1:26" ht="12.75" customHeight="1">
       <c r="A330" s="12"/>
       <c r="B330" s="12"/>
-      <c r="C330" s="12"/>
+      <c r="C330" s="42"/>
       <c r="D330" s="12"/>
       <c r="E330" s="12"/>
       <c r="G330" s="12"/>
@@ -18071,7 +18130,7 @@
     <row r="331" spans="1:26" ht="12.75" customHeight="1">
       <c r="A331" s="12"/>
       <c r="B331" s="12"/>
-      <c r="C331" s="12"/>
+      <c r="C331" s="42"/>
       <c r="D331" s="12"/>
       <c r="E331" s="12"/>
       <c r="G331" s="12"/>
@@ -18098,7 +18157,7 @@
     <row r="332" spans="1:26" ht="12.75" customHeight="1">
       <c r="A332" s="12"/>
       <c r="B332" s="12"/>
-      <c r="C332" s="12"/>
+      <c r="C332" s="42"/>
       <c r="D332" s="12"/>
       <c r="E332" s="12"/>
       <c r="G332" s="12"/>
@@ -18125,7 +18184,7 @@
     <row r="333" spans="1:26" ht="12.75" customHeight="1">
       <c r="A333" s="12"/>
       <c r="B333" s="12"/>
-      <c r="C333" s="12"/>
+      <c r="C333" s="42"/>
       <c r="D333" s="12"/>
       <c r="E333" s="12"/>
       <c r="G333" s="12"/>
@@ -18152,7 +18211,7 @@
     <row r="334" spans="1:26" ht="12.75" customHeight="1">
       <c r="A334" s="12"/>
       <c r="B334" s="12"/>
-      <c r="C334" s="12"/>
+      <c r="C334" s="42"/>
       <c r="D334" s="12"/>
       <c r="E334" s="12"/>
       <c r="G334" s="12"/>
@@ -18179,7 +18238,7 @@
     <row r="335" spans="1:26" ht="12.75" customHeight="1">
       <c r="A335" s="12"/>
       <c r="B335" s="12"/>
-      <c r="C335" s="12"/>
+      <c r="C335" s="42"/>
       <c r="D335" s="12"/>
       <c r="E335" s="12"/>
       <c r="G335" s="12"/>

</xml_diff>

<commit_message>
updated which events need to be skipped and which need to be read.
</commit_message>
<xml_diff>
--- a/Event_Points.xlsx
+++ b/Event_Points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michellexbui/python/tailwagtools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3035FD2-1E08-4144-A046-D167A805F00B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F925C6FD-CBF5-704B-BF28-4E9205D3CA8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15480" yWindow="460" windowWidth="13220" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12980" yWindow="460" windowWidth="15820" windowHeight="12860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event Data" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,16 @@
     <sheet name="OLD DATA" sheetId="3" r:id="rId3"/>
     <sheet name="User Notes" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -28,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4438" uniqueCount="1419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4431" uniqueCount="1419">
   <si>
     <t>Narrowed Point</t>
   </si>
@@ -4391,7 +4399,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4407,6 +4415,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4438,7 +4458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4534,6 +4554,22 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -4853,7 +4889,7 @@
   <dimension ref="A1:Z1128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C95" sqref="C95:C183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="13"/>
@@ -5070,7 +5106,9 @@
       <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="39"/>
+      <c r="C4" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D4" s="9" t="s">
         <v>37</v>
       </c>
@@ -5300,7 +5338,9 @@
       <c r="B8" s="7">
         <v>1</v>
       </c>
-      <c r="C8" s="39"/>
+      <c r="C8" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D8" s="9" t="s">
         <v>67</v>
       </c>
@@ -5522,7 +5562,9 @@
       <c r="B12" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="39"/>
+      <c r="C12" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D12" s="9" t="s">
         <v>96</v>
       </c>
@@ -5632,7 +5674,9 @@
       <c r="B14" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="39"/>
+      <c r="C14" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D14" s="9" t="s">
         <v>52</v>
       </c>
@@ -5686,7 +5730,9 @@
       <c r="B15" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="39"/>
+      <c r="C15" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D15" s="9" t="s">
         <v>89</v>
       </c>
@@ -5740,7 +5786,9 @@
       <c r="B16" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="41"/>
+      <c r="C16" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D16" s="9" t="s">
         <v>125</v>
       </c>
@@ -6018,7 +6066,9 @@
       <c r="B21" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="39"/>
+      <c r="C21" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D21" s="9" t="s">
         <v>154</v>
       </c>
@@ -6072,7 +6122,9 @@
       <c r="B22" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="39"/>
+      <c r="C22" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D22" s="9" t="s">
         <v>162</v>
       </c>
@@ -6238,7 +6290,7 @@
       <c r="B25" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -6278,7 +6330,9 @@
       <c r="B26" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="39"/>
+      <c r="C26" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D26" s="9" t="s">
         <v>162</v>
       </c>
@@ -6388,7 +6442,9 @@
       <c r="B28" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="39"/>
+      <c r="C28" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D28" s="9" t="s">
         <v>197</v>
       </c>
@@ -6442,7 +6498,9 @@
       <c r="B29" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="39"/>
+      <c r="C29" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D29" s="9" t="s">
         <v>205</v>
       </c>
@@ -6496,7 +6554,7 @@
       <c r="B30" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="41" t="s">
+      <c r="C30" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="9" t="s">
@@ -6552,7 +6610,9 @@
       <c r="B31" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="39"/>
+      <c r="C31" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D31" s="9" t="s">
         <v>162</v>
       </c>
@@ -6718,7 +6778,9 @@
       <c r="B34" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="39"/>
+      <c r="C34" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D34" s="9" t="s">
         <v>154</v>
       </c>
@@ -6756,7 +6818,7 @@
       <c r="B35" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C35" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D35" s="9" t="s">
@@ -7096,7 +7158,9 @@
       <c r="B41" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="39"/>
+      <c r="C41" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D41" s="9" t="s">
         <v>286</v>
       </c>
@@ -7150,7 +7214,9 @@
       <c r="B42" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C42" s="39"/>
+      <c r="C42" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D42" s="9" t="s">
         <v>37</v>
       </c>
@@ -7316,7 +7382,9 @@
       <c r="B45" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C45" s="39"/>
+      <c r="C45" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D45" s="9" t="s">
         <v>304</v>
       </c>
@@ -7370,7 +7438,9 @@
       <c r="B46" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C46" s="39"/>
+      <c r="C46" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D46" s="9" t="s">
         <v>67</v>
       </c>
@@ -7424,7 +7494,9 @@
       <c r="B47" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C47" s="39"/>
+      <c r="C47" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D47" s="9" t="s">
         <v>311</v>
       </c>
@@ -7534,7 +7606,9 @@
       <c r="B49" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C49" s="39"/>
+      <c r="C49" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D49" s="9" t="s">
         <v>320</v>
       </c>
@@ -7972,7 +8046,9 @@
       <c r="B58" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C58" s="39"/>
+      <c r="C58" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D58" s="9" t="s">
         <v>361</v>
       </c>
@@ -8082,7 +8158,9 @@
       <c r="B60" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C60" s="39"/>
+      <c r="C60" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D60" s="9" t="s">
         <v>134</v>
       </c>
@@ -8136,7 +8214,9 @@
       <c r="B61" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C61" s="39"/>
+      <c r="C61" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D61" s="9" t="s">
         <v>382</v>
       </c>
@@ -8190,7 +8270,9 @@
       <c r="B62" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C62" s="39"/>
+      <c r="C62" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D62" s="9" t="s">
         <v>389</v>
       </c>
@@ -8300,7 +8382,9 @@
       <c r="B64" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C64" s="39"/>
+      <c r="C64" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D64" s="9" t="s">
         <v>298</v>
       </c>
@@ -8354,7 +8438,7 @@
       <c r="B65" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C65" s="41" t="s">
+      <c r="C65" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D65" s="9" t="s">
@@ -8410,7 +8494,9 @@
       <c r="B66" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C66" s="39"/>
+      <c r="C66" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D66" s="9" t="s">
         <v>89</v>
       </c>
@@ -8810,7 +8896,9 @@
       <c r="B73" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C73" s="39"/>
+      <c r="C73" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D73" s="9" t="s">
         <v>162</v>
       </c>
@@ -8864,7 +8952,7 @@
       <c r="B74" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C74" s="41" t="s">
+      <c r="C74" s="39" t="s">
         <v>20</v>
       </c>
       <c r="D74" s="9" t="s">
@@ -8920,7 +9008,9 @@
       <c r="B75" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C75" s="39"/>
+      <c r="C75" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D75" s="9" t="s">
         <v>478</v>
       </c>
@@ -8974,7 +9064,9 @@
       <c r="B76" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C76" s="39"/>
+      <c r="C76" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D76" s="9" t="s">
         <v>162</v>
       </c>
@@ -9332,7 +9424,9 @@
       <c r="B83" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="C83" s="39"/>
+      <c r="C83" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D83" s="9" t="s">
         <v>246</v>
       </c>
@@ -9386,7 +9480,9 @@
       <c r="B84" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="C84" s="39"/>
+      <c r="C84" s="39" t="s">
+        <v>20</v>
+      </c>
       <c r="D84" s="9" t="s">
         <v>260</v>
       </c>
@@ -9977,61 +10073,59 @@
       <c r="Y94" s="8"/>
       <c r="Z94" s="8"/>
     </row>
-    <row r="95" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A95" s="8" t="s">
+    <row r="95" spans="1:26" s="46" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A95" s="43" t="s">
         <v>587</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B95" s="43" t="s">
         <v>294</v>
       </c>
-      <c r="C95" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="D95" s="9" t="s">
+      <c r="C95" s="47"/>
+      <c r="D95" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="E95" s="10"/>
-      <c r="F95">
+      <c r="E95" s="45"/>
+      <c r="F95" s="46">
         <v>-11.0140909090909</v>
       </c>
-      <c r="G95" s="8" t="s">
+      <c r="G95" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="H95" s="8" t="s">
+      <c r="H95" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="I95" s="8"/>
-      <c r="J95" s="8" t="s">
+      <c r="I95" s="43"/>
+      <c r="J95" s="43" t="s">
         <v>588</v>
       </c>
-      <c r="K95" s="8" t="s">
+      <c r="K95" s="43" t="s">
         <v>589</v>
       </c>
-      <c r="L95" s="8" t="s">
+      <c r="L95" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="M95" s="8" t="s">
+      <c r="M95" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="N95" s="8" t="s">
+      <c r="N95" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="O95" s="8" t="s">
+      <c r="O95" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="P95" s="8" t="s">
+      <c r="P95" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="Q95" s="8"/>
-      <c r="R95" s="8"/>
-      <c r="S95" s="8"/>
-      <c r="T95" s="8"/>
-      <c r="U95" s="8"/>
-      <c r="V95" s="8"/>
-      <c r="W95" s="8"/>
-      <c r="X95" s="8"/>
-      <c r="Y95" s="8"/>
-      <c r="Z95" s="8"/>
+      <c r="Q95" s="43"/>
+      <c r="R95" s="43"/>
+      <c r="S95" s="43"/>
+      <c r="T95" s="43"/>
+      <c r="U95" s="43"/>
+      <c r="V95" s="43"/>
+      <c r="W95" s="43"/>
+      <c r="X95" s="43"/>
+      <c r="Y95" s="43"/>
+      <c r="Z95" s="43"/>
     </row>
     <row r="96" spans="1:26" ht="12.75" customHeight="1">
       <c r="A96" s="8" t="s">
@@ -10040,9 +10134,7 @@
       <c r="B96" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C96" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C96" s="8"/>
       <c r="D96" s="9" t="s">
         <v>591</v>
       </c>
@@ -10096,9 +10188,7 @@
       <c r="B97" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C97" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C97" s="8"/>
       <c r="D97" s="9" t="s">
         <v>52</v>
       </c>
@@ -10152,9 +10242,7 @@
       <c r="B98" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C98" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C98" s="8"/>
       <c r="D98" s="9" t="s">
         <v>60</v>
       </c>
@@ -10208,9 +10296,7 @@
       <c r="B99" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C99" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C99" s="8"/>
       <c r="D99" s="9" t="s">
         <v>154</v>
       </c>
@@ -10264,9 +10350,7 @@
       <c r="B100" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C100" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C100" s="8"/>
       <c r="D100" s="9" t="s">
         <v>52</v>
       </c>
@@ -10320,9 +10404,7 @@
       <c r="B101" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C101" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C101" s="8"/>
       <c r="D101" s="9" t="s">
         <v>606</v>
       </c>
@@ -10376,9 +10458,7 @@
       <c r="B102" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C102" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C102" s="8"/>
       <c r="D102" s="9" t="s">
         <v>37</v>
       </c>
@@ -10432,9 +10512,7 @@
       <c r="B103" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C103" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C103" s="8"/>
       <c r="D103" s="9" t="s">
         <v>428</v>
       </c>
@@ -10488,9 +10566,7 @@
       <c r="B104" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C104" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C104" s="8"/>
       <c r="D104" s="9" t="s">
         <v>134</v>
       </c>
@@ -10544,9 +10620,7 @@
       <c r="B105" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C105" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C105" s="8"/>
       <c r="D105" s="9" t="s">
         <v>616</v>
       </c>
@@ -10600,9 +10674,7 @@
       <c r="B106" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C106" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C106" s="8"/>
       <c r="D106" s="9" t="s">
         <v>620</v>
       </c>
@@ -10656,7 +10728,7 @@
       <c r="B107" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C107" s="39" t="s">
+      <c r="C107" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D107" s="9" t="s">
@@ -10696,7 +10768,7 @@
       <c r="B108" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C108" s="39" t="s">
+      <c r="C108" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D108" s="9" t="s">
@@ -10736,7 +10808,7 @@
       <c r="B109" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C109" s="39" t="s">
+      <c r="C109" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D109" s="9" t="s">
@@ -10776,7 +10848,7 @@
       <c r="B110" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C110" s="39" t="s">
+      <c r="C110" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D110" s="9" t="s">
@@ -10816,7 +10888,7 @@
       <c r="B111" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C111" s="39" t="s">
+      <c r="C111" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D111" s="9" t="s">
@@ -10856,7 +10928,7 @@
       <c r="B112" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C112" s="39" t="s">
+      <c r="C112" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D112" s="9" t="s">
@@ -10896,7 +10968,7 @@
       <c r="B113" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C113" s="39" t="s">
+      <c r="C113" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D113" s="9" t="s">
@@ -10936,7 +11008,7 @@
       <c r="B114" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C114" s="39" t="s">
+      <c r="C114" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D114" s="9" t="s">
@@ -10976,7 +11048,7 @@
       <c r="B115" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C115" s="39" t="s">
+      <c r="C115" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D115" s="9" t="s">
@@ -11016,7 +11088,7 @@
       <c r="B116" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C116" s="39" t="s">
+      <c r="C116" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D116" s="9" t="s">
@@ -11056,7 +11128,7 @@
       <c r="B117" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C117" s="39" t="s">
+      <c r="C117" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D117" s="9" t="s">
@@ -11096,7 +11168,7 @@
       <c r="B118" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C118" s="39" t="s">
+      <c r="C118" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D118" s="9" t="s">
@@ -11136,7 +11208,7 @@
       <c r="B119" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C119" s="39" t="s">
+      <c r="C119" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D119" s="9" t="s">
@@ -11176,7 +11248,7 @@
       <c r="B120" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C120" s="39" t="s">
+      <c r="C120" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D120" s="9" t="s">
@@ -11216,7 +11288,7 @@
       <c r="B121" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C121" s="39" t="s">
+      <c r="C121" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D121" s="9" t="s">
@@ -11256,7 +11328,7 @@
       <c r="B122" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C122" s="39" t="s">
+      <c r="C122" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D122" s="9" t="s">
@@ -11296,7 +11368,7 @@
       <c r="B123" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C123" s="39" t="s">
+      <c r="C123" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D123" s="9" t="s">
@@ -11336,7 +11408,7 @@
       <c r="B124" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C124" s="39" t="s">
+      <c r="C124" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D124" s="9" t="s">
@@ -11376,7 +11448,7 @@
       <c r="B125" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C125" s="39" t="s">
+      <c r="C125" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D125" s="9" t="s">
@@ -11416,7 +11488,7 @@
       <c r="B126" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C126" s="39" t="s">
+      <c r="C126" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D126" s="9" t="s">
@@ -11456,7 +11528,7 @@
       <c r="B127" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C127" s="39" t="s">
+      <c r="C127" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D127" s="9" t="s">
@@ -11496,7 +11568,7 @@
       <c r="B128" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C128" s="39" t="s">
+      <c r="C128" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D128" s="9" t="s">
@@ -11536,7 +11608,7 @@
       <c r="B129" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C129" s="39" t="s">
+      <c r="C129" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D129" s="9" t="s">
@@ -11576,9 +11648,7 @@
       <c r="B130" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C130" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C130" s="8"/>
       <c r="D130" s="9" t="s">
         <v>134</v>
       </c>
@@ -11632,9 +11702,7 @@
       <c r="B131" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C131" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C131" s="8"/>
       <c r="D131" s="9" t="s">
         <v>37</v>
       </c>
@@ -11688,7 +11756,7 @@
       <c r="B132" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C132" s="39" t="s">
+      <c r="C132" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D132" s="9" t="s">
@@ -11728,7 +11796,7 @@
       <c r="B133" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C133" s="39" t="s">
+      <c r="C133" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D133" s="9" t="s">
@@ -11768,9 +11836,7 @@
       <c r="B134" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C134" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C134" s="8"/>
       <c r="D134" s="9" t="s">
         <v>149</v>
       </c>
@@ -11824,7 +11890,7 @@
       <c r="B135" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C135" s="39" t="s">
+      <c r="C135" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D135" s="9" t="s">
@@ -11864,7 +11930,7 @@
       <c r="B136" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C136" s="39" t="s">
+      <c r="C136" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D136" s="9" t="s">
@@ -11904,9 +11970,7 @@
       <c r="B137" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C137" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C137" s="8"/>
       <c r="D137" s="9" t="s">
         <v>30</v>
       </c>
@@ -11960,7 +12024,7 @@
       <c r="B138" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C138" s="39" t="s">
+      <c r="C138" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D138" s="9" t="s">
@@ -12000,9 +12064,7 @@
       <c r="B139" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C139" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C139" s="8"/>
       <c r="D139" s="9" t="s">
         <v>149</v>
       </c>
@@ -12056,9 +12118,7 @@
       <c r="B140" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C140" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C140" s="8"/>
       <c r="D140" s="9" t="s">
         <v>260</v>
       </c>
@@ -12112,7 +12172,7 @@
       <c r="B141" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C141" s="39" t="s">
+      <c r="C141" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D141" s="9" t="s">
@@ -12168,7 +12228,7 @@
       <c r="B142" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C142" s="39" t="s">
+      <c r="C142" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D142" s="9" t="s">
@@ -12208,9 +12268,7 @@
       <c r="B143" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C143" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C143" s="48"/>
       <c r="D143" s="9" t="s">
         <v>304</v>
       </c>
@@ -12264,9 +12322,7 @@
       <c r="B144" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C144" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C144" s="8"/>
       <c r="D144" s="9" t="s">
         <v>689</v>
       </c>
@@ -12320,7 +12376,7 @@
       <c r="B145" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C145" s="39" t="s">
+      <c r="C145" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D145" s="9" t="s">
@@ -12360,9 +12416,7 @@
       <c r="B146" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C146" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C146" s="8"/>
       <c r="D146" s="9" t="s">
         <v>89</v>
       </c>
@@ -12416,9 +12470,7 @@
       <c r="B147" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C147" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C147" s="8"/>
       <c r="D147" s="9" t="s">
         <v>286</v>
       </c>
@@ -12472,9 +12524,7 @@
       <c r="B148" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C148" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C148" s="8"/>
       <c r="D148" s="9" t="s">
         <v>298</v>
       </c>
@@ -12528,9 +12578,7 @@
       <c r="B149" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C149" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C149" s="8"/>
       <c r="D149" s="9" t="s">
         <v>304</v>
       </c>
@@ -12584,9 +12632,7 @@
       <c r="B150" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C150" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C150" s="8"/>
       <c r="D150" s="9" t="s">
         <v>89</v>
       </c>
@@ -12640,7 +12686,7 @@
       <c r="B151" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C151" s="39" t="s">
+      <c r="C151" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D151" s="9" t="s">
@@ -12693,7 +12739,7 @@
       <c r="B152" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C152" s="39" t="s">
+      <c r="C152" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D152" s="9" t="s">
@@ -12733,9 +12779,7 @@
       <c r="B153" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C153" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C153" s="8"/>
       <c r="D153" s="9" t="s">
         <v>713</v>
       </c>
@@ -12789,7 +12833,7 @@
       <c r="B154" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C154" s="39" t="s">
+      <c r="C154" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D154" s="9" t="s">
@@ -12829,9 +12873,7 @@
       <c r="B155" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C155" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C155" s="8"/>
       <c r="D155" s="9" t="s">
         <v>52</v>
       </c>
@@ -12885,9 +12927,7 @@
       <c r="B156" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C156" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C156" s="8"/>
       <c r="D156" s="9" t="s">
         <v>67</v>
       </c>
@@ -12941,9 +12981,7 @@
       <c r="B157" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C157" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C157" s="8"/>
       <c r="D157" s="9" t="s">
         <v>725</v>
       </c>
@@ -12997,9 +13035,7 @@
       <c r="B158" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C158" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C158" s="8"/>
       <c r="D158" s="9" t="s">
         <v>154</v>
       </c>
@@ -13053,9 +13089,7 @@
       <c r="B159" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C159" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C159" s="8"/>
       <c r="D159" s="9" t="s">
         <v>89</v>
       </c>
@@ -13109,9 +13143,7 @@
       <c r="B160" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C160" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C160" s="8"/>
       <c r="D160" s="9" t="s">
         <v>734</v>
       </c>
@@ -13165,9 +13197,7 @@
       <c r="B161" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C161" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C161" s="8"/>
       <c r="D161" s="9" t="s">
         <v>162</v>
       </c>
@@ -13221,7 +13251,7 @@
       <c r="B162" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C162" s="39" t="s">
+      <c r="C162" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D162" s="9" t="s">
@@ -13261,7 +13291,7 @@
       <c r="B163" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C163" s="39" t="s">
+      <c r="C163" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D163" s="9" t="s">
@@ -13301,7 +13331,7 @@
       <c r="B164" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C164" s="39" t="s">
+      <c r="C164" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D164" s="9" t="s">
@@ -13341,7 +13371,7 @@
       <c r="B165" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C165" s="39" t="s">
+      <c r="C165" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D165" s="9" t="s">
@@ -13381,7 +13411,7 @@
       <c r="B166" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C166" s="39" t="s">
+      <c r="C166" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D166" s="9" t="s">
@@ -13421,7 +13451,7 @@
       <c r="B167" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C167" s="39" t="s">
+      <c r="C167" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D167" s="9" t="s">
@@ -13461,9 +13491,7 @@
       <c r="B168" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C168" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C168" s="8"/>
       <c r="D168" s="9" t="s">
         <v>37</v>
       </c>
@@ -13517,9 +13545,7 @@
       <c r="B169" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C169" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C169" s="8"/>
       <c r="D169" s="9" t="s">
         <v>591</v>
       </c>
@@ -13573,7 +13599,7 @@
       <c r="B170" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C170" s="39" t="s">
+      <c r="C170" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D170" s="9" t="s">
@@ -13613,7 +13639,7 @@
       <c r="B171" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C171" s="39" t="s">
+      <c r="C171" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D171" s="9" t="s">
@@ -13653,7 +13679,7 @@
       <c r="B172" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C172" s="39" t="s">
+      <c r="C172" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D172" s="9" t="s">
@@ -13693,7 +13719,7 @@
       <c r="B173" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C173" s="39" t="s">
+      <c r="C173" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D173" s="9" t="s">
@@ -13733,7 +13759,7 @@
       <c r="B174" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C174" s="39" t="s">
+      <c r="C174" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D174" s="9" t="s">
@@ -13773,7 +13799,7 @@
       <c r="B175" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C175" s="39" t="s">
+      <c r="C175" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D175" s="9" t="s">
@@ -13813,7 +13839,7 @@
       <c r="B176" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C176" s="39" t="s">
+      <c r="C176" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D176" s="9" t="s">
@@ -13853,7 +13879,7 @@
       <c r="B177" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C177" s="39" t="s">
+      <c r="C177" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D177" s="9" t="s">
@@ -13893,9 +13919,7 @@
       <c r="B178" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C178" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C178" s="8"/>
       <c r="D178" s="9" t="s">
         <v>67</v>
       </c>
@@ -13949,9 +13973,7 @@
       <c r="B179" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C179" s="39" t="s">
-        <v>20</v>
-      </c>
+      <c r="C179" s="8"/>
       <c r="D179" s="9" t="s">
         <v>134</v>
       </c>
@@ -14005,7 +14027,7 @@
       <c r="B180" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C180" s="39" t="s">
+      <c r="C180" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D180" s="9" t="s">
@@ -14045,7 +14067,7 @@
       <c r="B181" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C181" s="39" t="s">
+      <c r="C181" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D181" s="9" t="s">
@@ -14085,7 +14107,7 @@
       <c r="B182" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C182" s="39" t="s">
+      <c r="C182" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D182" s="9" t="s">
@@ -14125,7 +14147,7 @@
       <c r="B183" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C183" s="39" t="s">
+      <c r="C183" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D183" s="9" t="s">

</xml_diff>

<commit_message>
lots of files to add (:
</commit_message>
<xml_diff>
--- a/Event_Points.xlsx
+++ b/Event_Points.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michellexbui/python/tailwagtools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F925C6FD-CBF5-704B-BF28-4E9205D3CA8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB95C9DF-4BD4-8B4B-BD56-27F2AB258A3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12980" yWindow="460" windowWidth="15820" windowHeight="12860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="14680" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4431" uniqueCount="1419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4483" uniqueCount="1420">
   <si>
     <t>Narrowed Point</t>
   </si>
@@ -4274,25 +4274,28 @@
     <t>F10.7 data from here</t>
   </si>
   <si>
-    <t>North/South/??</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>CLEAN</t>
-  </si>
-  <si>
-    <t>LACKING</t>
-  </si>
-  <si>
-    <t>MESSY</t>
+    <t>2006-08-13 16:29:55.000</t>
+  </si>
+  <si>
+    <t>2006-09-01 13:43:39.000</t>
+  </si>
+  <si>
+    <t>2007-08-14 18:03:00.000</t>
+  </si>
+  <si>
+    <t>2007-08-17 07:33:00.000</t>
+  </si>
+  <si>
+    <t>2008-08-22 10:47:53.000</t>
+  </si>
+  <si>
+    <t>2008-09-17 09:00:30.000</t>
+  </si>
+  <si>
+    <t>2008-09-29 06:22:00.000</t>
+  </si>
+  <si>
+    <t>f10.7</t>
   </si>
 </sst>
 </file>
@@ -4305,7 +4308,7 @@
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\Thh:mm:ss"/>
     <numFmt numFmtId="167" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4316,13 +4319,13 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -4335,7 +4338,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4348,18 +4351,18 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4387,30 +4390,18 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -4421,12 +4412,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4458,7 +4443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4530,48 +4515,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4888,14 +4859,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95:C183"/>
+    <sheetView tabSelected="1" topLeftCell="A168" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C189" sqref="C189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="31.1640625" customWidth="1"/>
-    <col min="3" max="4" width="22" customWidth="1"/>
+    <col min="3" max="3" width="22" style="44" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="22" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="33.6640625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="64.6640625" customWidth="1"/>
@@ -4916,7 +4888,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -4968,11 +4940,9 @@
         <v>18</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>1412</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>1413</v>
-      </c>
+        <v>1419</v>
+      </c>
+      <c r="U1" s="5"/>
       <c r="V1" s="5"/>
       <c r="W1" s="5"/>
       <c r="X1" s="5"/>
@@ -4986,7 +4956,7 @@
       <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="9" t="s">
@@ -5027,12 +4997,8 @@
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
-      <c r="T2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>1418</v>
-      </c>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
       <c r="V2" s="8"/>
       <c r="W2" s="8"/>
       <c r="X2" s="8"/>
@@ -5046,7 +5012,7 @@
       <c r="B3" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -5087,12 +5053,8 @@
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
-      <c r="T3" s="8" t="s">
-        <v>1414</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>1417</v>
-      </c>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
@@ -5106,7 +5068,7 @@
       <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -5147,12 +5109,8 @@
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="8" t="s">
-        <v>1415</v>
-      </c>
-      <c r="U4" s="8" t="s">
-        <v>1416</v>
-      </c>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
@@ -5166,7 +5124,7 @@
       <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -5207,12 +5165,8 @@
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
-      <c r="T5" s="8" t="s">
-        <v>1415</v>
-      </c>
-      <c r="U5" s="8" t="s">
-        <v>1418</v>
-      </c>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
       <c r="V5" s="8"/>
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
@@ -5226,7 +5180,7 @@
       <c r="B6" s="7">
         <v>1</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="9" t="s">
@@ -5282,7 +5236,7 @@
       <c r="B7" s="34">
         <v>1</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="35" t="s">
@@ -5338,7 +5292,7 @@
       <c r="B8" s="7">
         <v>1</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="9" t="s">
@@ -5394,7 +5348,7 @@
       <c r="B9" s="7">
         <v>1</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="9" t="s">
@@ -5450,7 +5404,7 @@
       <c r="B10" s="7">
         <v>1</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -5506,7 +5460,7 @@
       <c r="B11" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="9" t="s">
@@ -5562,7 +5516,7 @@
       <c r="B12" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -5618,7 +5572,7 @@
       <c r="B13" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -5674,7 +5628,7 @@
       <c r="B14" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="9" t="s">
@@ -5730,7 +5684,7 @@
       <c r="B15" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="9" t="s">
@@ -5786,7 +5740,7 @@
       <c r="B16" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="9" t="s">
@@ -5842,7 +5796,7 @@
       <c r="B17" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="9" t="s">
@@ -5898,7 +5852,7 @@
       <c r="B18" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -5954,7 +5908,7 @@
       <c r="B19" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="9" t="s">
@@ -6010,7 +5964,7 @@
       <c r="B20" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -6066,7 +6020,7 @@
       <c r="B21" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="9" t="s">
@@ -6122,7 +6076,7 @@
       <c r="B22" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="9" t="s">
@@ -6178,7 +6132,7 @@
       <c r="B23" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -6234,7 +6188,7 @@
       <c r="B24" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -6290,7 +6244,7 @@
       <c r="B25" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -6330,7 +6284,7 @@
       <c r="B26" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -6386,7 +6340,7 @@
       <c r="B27" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D27" s="9" t="s">
@@ -6442,7 +6396,7 @@
       <c r="B28" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="39" t="s">
+      <c r="C28" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -6498,7 +6452,7 @@
       <c r="B29" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D29" s="9" t="s">
@@ -6554,7 +6508,7 @@
       <c r="B30" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="9" t="s">
@@ -6610,7 +6564,7 @@
       <c r="B31" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="39" t="s">
+      <c r="C31" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D31" s="9" t="s">
@@ -6666,7 +6620,7 @@
       <c r="B32" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="39" t="s">
+      <c r="C32" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="9" t="s">
@@ -6722,7 +6676,7 @@
       <c r="B33" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D33" s="9" t="s">
@@ -6778,7 +6732,7 @@
       <c r="B34" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="39" t="s">
+      <c r="C34" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="9" t="s">
@@ -6818,7 +6772,7 @@
       <c r="B35" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="39" t="s">
+      <c r="C35" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D35" s="9" t="s">
@@ -6874,7 +6828,7 @@
       <c r="B36" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="9" t="s">
@@ -6930,7 +6884,7 @@
       <c r="B37" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="39" t="s">
+      <c r="C37" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D37" s="9" t="s">
@@ -6986,7 +6940,7 @@
       <c r="B38" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D38" s="9" t="s">
@@ -7044,7 +6998,7 @@
       <c r="B39" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D39" s="9" t="s">
@@ -7100,7 +7054,7 @@
       <c r="B40" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C40" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D40" s="9" t="s">
@@ -7158,7 +7112,7 @@
       <c r="B41" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C41" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D41" s="9" t="s">
@@ -7214,7 +7168,7 @@
       <c r="B42" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C42" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D42" s="9" t="s">
@@ -7270,7 +7224,7 @@
       <c r="B43" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D43" s="9" t="s">
@@ -7326,7 +7280,7 @@
       <c r="B44" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C44" s="39" t="s">
+      <c r="C44" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -7382,7 +7336,7 @@
       <c r="B45" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C45" s="39" t="s">
+      <c r="C45" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D45" s="9" t="s">
@@ -7438,7 +7392,7 @@
       <c r="B46" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C46" s="39" t="s">
+      <c r="C46" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D46" s="9" t="s">
@@ -7494,7 +7448,7 @@
       <c r="B47" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C47" s="39" t="s">
+      <c r="C47" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D47" s="9" t="s">
@@ -7550,7 +7504,7 @@
       <c r="B48" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C48" s="39" t="s">
+      <c r="C48" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D48" s="9" t="s">
@@ -7606,7 +7560,7 @@
       <c r="B49" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C49" s="39" t="s">
+      <c r="C49" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="9" t="s">
@@ -7646,7 +7600,7 @@
       <c r="B50" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C50" s="41" t="s">
+      <c r="C50" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D50" s="9" t="s">
@@ -7686,7 +7640,7 @@
       <c r="B51" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="41" t="s">
+      <c r="C51" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D51" s="9" t="s">
@@ -7742,7 +7696,7 @@
       <c r="B52" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="41" t="s">
+      <c r="C52" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D52" s="9" t="s">
@@ -7798,7 +7752,7 @@
       <c r="B53" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="39" t="s">
+      <c r="C53" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D53" s="9" t="s">
@@ -7854,7 +7808,7 @@
       <c r="B54" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="41" t="s">
+      <c r="C54" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D54" s="9" t="s">
@@ -7910,7 +7864,7 @@
       <c r="B55" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C55" s="39" t="s">
+      <c r="C55" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D55" s="9" t="s">
@@ -7966,7 +7920,7 @@
       <c r="B56" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C56" s="41" t="s">
+      <c r="C56" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D56" s="9" t="s">
@@ -8006,7 +7960,7 @@
       <c r="B57" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C57" s="41" t="s">
+      <c r="C57" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D57" s="9" t="s">
@@ -8046,7 +8000,7 @@
       <c r="B58" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C58" s="39" t="s">
+      <c r="C58" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D58" s="9" t="s">
@@ -8102,7 +8056,7 @@
       <c r="B59" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C59" s="39" t="s">
+      <c r="C59" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D59" s="9" t="s">
@@ -8158,7 +8112,7 @@
       <c r="B60" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C60" s="39" t="s">
+      <c r="C60" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D60" s="9" t="s">
@@ -8214,7 +8168,7 @@
       <c r="B61" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C61" s="39" t="s">
+      <c r="C61" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D61" s="9" t="s">
@@ -8270,7 +8224,7 @@
       <c r="B62" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C62" s="39" t="s">
+      <c r="C62" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D62" s="9" t="s">
@@ -8326,7 +8280,7 @@
       <c r="B63" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C63" s="39" t="s">
+      <c r="C63" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D63" s="9" t="s">
@@ -8382,7 +8336,7 @@
       <c r="B64" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C64" s="39" t="s">
+      <c r="C64" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D64" s="9" t="s">
@@ -8438,7 +8392,7 @@
       <c r="B65" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C65" s="39" t="s">
+      <c r="C65" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D65" s="9" t="s">
@@ -8494,7 +8448,7 @@
       <c r="B66" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C66" s="39" t="s">
+      <c r="C66" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D66" s="9" t="s">
@@ -8552,7 +8506,7 @@
       <c r="B67" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C67" s="41" t="s">
+      <c r="C67" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D67" s="9" t="s">
@@ -8610,7 +8564,7 @@
       <c r="B68" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C68" s="41" t="s">
+      <c r="C68" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D68" s="9" t="s">
@@ -8668,7 +8622,7 @@
       <c r="B69" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C69" s="40" t="s">
+      <c r="C69" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D69" s="9" t="s">
@@ -8726,7 +8680,7 @@
       <c r="B70" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C70" s="41" t="s">
+      <c r="C70" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D70" s="9" t="s">
@@ -8784,7 +8738,7 @@
       <c r="B71" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C71" s="41" t="s">
+      <c r="C71" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D71" s="9" t="s">
@@ -8840,7 +8794,7 @@
       <c r="B72" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C72" s="39" t="s">
+      <c r="C72" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D72" s="9" t="s">
@@ -8896,7 +8850,7 @@
       <c r="B73" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C73" s="39" t="s">
+      <c r="C73" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D73" s="9" t="s">
@@ -8952,7 +8906,7 @@
       <c r="B74" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C74" s="39" t="s">
+      <c r="C74" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D74" s="9" t="s">
@@ -9008,7 +8962,7 @@
       <c r="B75" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C75" s="39" t="s">
+      <c r="C75" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D75" s="9" t="s">
@@ -9064,7 +9018,7 @@
       <c r="B76" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C76" s="39" t="s">
+      <c r="C76" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D76" s="9" t="s">
@@ -9120,7 +9074,7 @@
       <c r="B77" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C77" s="39" t="s">
+      <c r="C77" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D77" s="9" t="s">
@@ -9176,7 +9130,7 @@
       <c r="B78" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C78" s="39" t="s">
+      <c r="C78" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D78" s="9" t="s">
@@ -9224,7 +9178,7 @@
       <c r="B79" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C79" s="41" t="s">
+      <c r="C79" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D79" s="11">
@@ -9272,7 +9226,7 @@
       <c r="B80" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="C80" s="41" t="s">
+      <c r="C80" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D80" s="11">
@@ -9312,7 +9266,7 @@
       <c r="B81" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C81" s="41" t="s">
+      <c r="C81" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D81" s="11">
@@ -9368,7 +9322,7 @@
       <c r="B82" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="C82" s="39" t="s">
+      <c r="C82" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D82" s="11">
@@ -9424,7 +9378,7 @@
       <c r="B83" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="C83" s="39" t="s">
+      <c r="C83" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D83" s="9" t="s">
@@ -9480,7 +9434,7 @@
       <c r="B84" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="C84" s="39" t="s">
+      <c r="C84" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D84" s="9" t="s">
@@ -9536,7 +9490,7 @@
       <c r="B85" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="C85" s="39" t="s">
+      <c r="C85" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D85" s="9" t="s">
@@ -9592,7 +9546,7 @@
       <c r="B86" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C86" s="39" t="s">
+      <c r="C86" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D86" s="9" t="s">
@@ -9648,7 +9602,7 @@
       <c r="B87" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C87" s="39" t="s">
+      <c r="C87" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D87" s="9" t="s">
@@ -9704,7 +9658,7 @@
       <c r="B88" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C88" s="39" t="s">
+      <c r="C88" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D88" s="9" t="s">
@@ -9760,7 +9714,7 @@
       <c r="B89" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C89" s="39" t="s">
+      <c r="C89" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D89" s="9" t="s">
@@ -9816,7 +9770,7 @@
       <c r="B90" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="39" t="s">
+      <c r="C90" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D90" s="9" t="s">
@@ -9872,7 +9826,7 @@
       <c r="B91" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="39" t="s">
+      <c r="C91" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D91" s="9" t="s">
@@ -9928,7 +9882,7 @@
       <c r="B92" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C92" s="39" t="s">
+      <c r="C92" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D92" s="9" t="s">
@@ -9984,7 +9938,7 @@
       <c r="B93" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C93" s="39" t="s">
+      <c r="C93" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D93" s="9" t="s">
@@ -10040,7 +9994,7 @@
       <c r="B94" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C94" s="39" t="s">
+      <c r="C94" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D94" s="9" t="s">
@@ -10073,59 +10027,61 @@
       <c r="Y94" s="8"/>
       <c r="Z94" s="8"/>
     </row>
-    <row r="95" spans="1:26" s="46" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A95" s="43" t="s">
+    <row r="95" spans="1:26" s="41" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A95" s="38" t="s">
         <v>587</v>
       </c>
-      <c r="B95" s="43" t="s">
+      <c r="B95" s="38" t="s">
         <v>294</v>
       </c>
-      <c r="C95" s="47"/>
-      <c r="D95" s="44" t="s">
+      <c r="C95" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D95" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="E95" s="45"/>
-      <c r="F95" s="46">
+      <c r="E95" s="40"/>
+      <c r="F95" s="41">
         <v>-11.0140909090909</v>
       </c>
-      <c r="G95" s="43" t="s">
+      <c r="G95" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="H95" s="43" t="s">
+      <c r="H95" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="I95" s="43"/>
-      <c r="J95" s="43" t="s">
+      <c r="I95" s="38"/>
+      <c r="J95" s="38" t="s">
         <v>588</v>
       </c>
-      <c r="K95" s="43" t="s">
+      <c r="K95" s="38" t="s">
         <v>589</v>
       </c>
-      <c r="L95" s="43" t="s">
+      <c r="L95" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="M95" s="43" t="s">
+      <c r="M95" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="N95" s="43" t="s">
+      <c r="N95" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="O95" s="43" t="s">
+      <c r="O95" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="P95" s="43" t="s">
+      <c r="P95" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="Q95" s="43"/>
-      <c r="R95" s="43"/>
-      <c r="S95" s="43"/>
-      <c r="T95" s="43"/>
-      <c r="U95" s="43"/>
-      <c r="V95" s="43"/>
-      <c r="W95" s="43"/>
-      <c r="X95" s="43"/>
-      <c r="Y95" s="43"/>
-      <c r="Z95" s="43"/>
+      <c r="Q95" s="38"/>
+      <c r="R95" s="38"/>
+      <c r="S95" s="38"/>
+      <c r="T95" s="38"/>
+      <c r="U95" s="38"/>
+      <c r="V95" s="38"/>
+      <c r="W95" s="38"/>
+      <c r="X95" s="38"/>
+      <c r="Y95" s="38"/>
+      <c r="Z95" s="38"/>
     </row>
     <row r="96" spans="1:26" ht="12.75" customHeight="1">
       <c r="A96" s="8" t="s">
@@ -10134,7 +10090,9 @@
       <c r="B96" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C96" s="8"/>
+      <c r="C96" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D96" s="9" t="s">
         <v>591</v>
       </c>
@@ -10188,7 +10146,9 @@
       <c r="B97" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C97" s="8"/>
+      <c r="C97" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D97" s="9" t="s">
         <v>52</v>
       </c>
@@ -10242,7 +10202,9 @@
       <c r="B98" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C98" s="8"/>
+      <c r="C98" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D98" s="9" t="s">
         <v>60</v>
       </c>
@@ -10296,7 +10258,9 @@
       <c r="B99" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C99" s="8"/>
+      <c r="C99" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D99" s="9" t="s">
         <v>154</v>
       </c>
@@ -10350,7 +10314,9 @@
       <c r="B100" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C100" s="8"/>
+      <c r="C100" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D100" s="9" t="s">
         <v>52</v>
       </c>
@@ -10404,7 +10370,9 @@
       <c r="B101" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C101" s="8"/>
+      <c r="C101" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D101" s="9" t="s">
         <v>606</v>
       </c>
@@ -10458,7 +10426,9 @@
       <c r="B102" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C102" s="8"/>
+      <c r="C102" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D102" s="9" t="s">
         <v>37</v>
       </c>
@@ -10512,7 +10482,9 @@
       <c r="B103" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C103" s="8"/>
+      <c r="C103" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D103" s="9" t="s">
         <v>428</v>
       </c>
@@ -10566,7 +10538,9 @@
       <c r="B104" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C104" s="8"/>
+      <c r="C104" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D104" s="9" t="s">
         <v>134</v>
       </c>
@@ -10620,7 +10594,9 @@
       <c r="B105" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C105" s="8"/>
+      <c r="C105" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D105" s="9" t="s">
         <v>616</v>
       </c>
@@ -10674,7 +10650,9 @@
       <c r="B106" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C106" s="8"/>
+      <c r="C106" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D106" s="9" t="s">
         <v>620</v>
       </c>
@@ -11648,7 +11626,9 @@
       <c r="B130" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C130" s="8"/>
+      <c r="C130" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D130" s="9" t="s">
         <v>134</v>
       </c>
@@ -11702,7 +11682,9 @@
       <c r="B131" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C131" s="8"/>
+      <c r="C131" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D131" s="9" t="s">
         <v>37</v>
       </c>
@@ -11836,7 +11818,9 @@
       <c r="B134" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C134" s="8"/>
+      <c r="C134" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D134" s="9" t="s">
         <v>149</v>
       </c>
@@ -11970,7 +11954,9 @@
       <c r="B137" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C137" s="8"/>
+      <c r="C137" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D137" s="9" t="s">
         <v>30</v>
       </c>
@@ -12064,7 +12050,9 @@
       <c r="B139" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C139" s="8"/>
+      <c r="C139" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D139" s="9" t="s">
         <v>149</v>
       </c>
@@ -12118,7 +12106,9 @@
       <c r="B140" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C140" s="8"/>
+      <c r="C140" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D140" s="9" t="s">
         <v>260</v>
       </c>
@@ -12268,7 +12258,9 @@
       <c r="B143" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C143" s="48"/>
+      <c r="C143" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D143" s="9" t="s">
         <v>304</v>
       </c>
@@ -12322,7 +12314,9 @@
       <c r="B144" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C144" s="8"/>
+      <c r="C144" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D144" s="9" t="s">
         <v>689</v>
       </c>
@@ -12416,7 +12410,9 @@
       <c r="B146" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C146" s="8"/>
+      <c r="C146" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D146" s="9" t="s">
         <v>89</v>
       </c>
@@ -12470,7 +12466,9 @@
       <c r="B147" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C147" s="8"/>
+      <c r="C147" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D147" s="9" t="s">
         <v>286</v>
       </c>
@@ -12524,7 +12522,9 @@
       <c r="B148" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C148" s="8"/>
+      <c r="C148" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D148" s="9" t="s">
         <v>298</v>
       </c>
@@ -12578,7 +12578,9 @@
       <c r="B149" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C149" s="8"/>
+      <c r="C149" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D149" s="9" t="s">
         <v>304</v>
       </c>
@@ -12632,7 +12634,9 @@
       <c r="B150" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C150" s="8"/>
+      <c r="C150" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D150" s="9" t="s">
         <v>89</v>
       </c>
@@ -12779,7 +12783,9 @@
       <c r="B153" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C153" s="8"/>
+      <c r="C153" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D153" s="9" t="s">
         <v>713</v>
       </c>
@@ -12873,7 +12879,9 @@
       <c r="B155" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C155" s="8"/>
+      <c r="C155" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D155" s="9" t="s">
         <v>52</v>
       </c>
@@ -12927,7 +12935,9 @@
       <c r="B156" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C156" s="8"/>
+      <c r="C156" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D156" s="9" t="s">
         <v>67</v>
       </c>
@@ -12981,7 +12991,9 @@
       <c r="B157" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C157" s="8"/>
+      <c r="C157" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D157" s="9" t="s">
         <v>725</v>
       </c>
@@ -13035,7 +13047,9 @@
       <c r="B158" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C158" s="8"/>
+      <c r="C158" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D158" s="9" t="s">
         <v>154</v>
       </c>
@@ -13089,7 +13103,9 @@
       <c r="B159" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C159" s="8"/>
+      <c r="C159" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D159" s="9" t="s">
         <v>89</v>
       </c>
@@ -13143,7 +13159,9 @@
       <c r="B160" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C160" s="8"/>
+      <c r="C160" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D160" s="9" t="s">
         <v>734</v>
       </c>
@@ -13197,7 +13215,9 @@
       <c r="B161" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C161" s="8"/>
+      <c r="C161" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D161" s="9" t="s">
         <v>162</v>
       </c>
@@ -13491,7 +13511,9 @@
       <c r="B168" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C168" s="8"/>
+      <c r="C168" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D168" s="9" t="s">
         <v>37</v>
       </c>
@@ -13545,7 +13567,9 @@
       <c r="B169" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C169" s="8"/>
+      <c r="C169" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D169" s="9" t="s">
         <v>591</v>
       </c>
@@ -13919,7 +13943,9 @@
       <c r="B178" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C178" s="8"/>
+      <c r="C178" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D178" s="9" t="s">
         <v>67</v>
       </c>
@@ -13973,7 +13999,9 @@
       <c r="B179" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C179" s="8"/>
+      <c r="C179" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D179" s="9" t="s">
         <v>134</v>
       </c>
@@ -14181,12 +14209,20 @@
       <c r="Z183" s="8"/>
     </row>
     <row r="184" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A184" s="8"/>
-      <c r="B184" s="8"/>
-      <c r="C184" s="39"/>
+      <c r="A184" s="8" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C184" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D184" s="8"/>
       <c r="E184" s="8"/>
-      <c r="G184" s="8"/>
+      <c r="G184" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H184" s="8"/>
       <c r="I184" s="8"/>
       <c r="J184" s="8"/>
@@ -14208,12 +14244,20 @@
       <c r="Z184" s="8"/>
     </row>
     <row r="185" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A185" s="8"/>
-      <c r="B185" s="8"/>
-      <c r="C185" s="39"/>
+      <c r="A185" s="8" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C185" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D185" s="8"/>
       <c r="E185" s="8"/>
-      <c r="G185" s="8"/>
+      <c r="G185" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H185" s="8"/>
       <c r="I185" s="8"/>
       <c r="J185" s="8"/>
@@ -14235,12 +14279,20 @@
       <c r="Z185" s="8"/>
     </row>
     <row r="186" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A186" s="8"/>
-      <c r="B186" s="8"/>
-      <c r="C186" s="39"/>
+      <c r="A186" s="8" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C186" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D186" s="8"/>
       <c r="E186" s="8"/>
-      <c r="G186" s="8"/>
+      <c r="G186" s="8" t="s">
+        <v>321</v>
+      </c>
       <c r="H186" s="8"/>
       <c r="I186" s="8"/>
       <c r="J186" s="8"/>
@@ -14262,12 +14314,20 @@
       <c r="Z186" s="8"/>
     </row>
     <row r="187" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A187" s="8"/>
-      <c r="B187" s="8"/>
-      <c r="C187" s="39"/>
+      <c r="A187" s="8" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C187" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D187" s="8"/>
       <c r="E187" s="8"/>
-      <c r="G187" s="8"/>
+      <c r="G187" s="8" t="s">
+        <v>185</v>
+      </c>
       <c r="H187" s="8"/>
       <c r="I187" s="8"/>
       <c r="J187" s="8"/>
@@ -14289,12 +14349,20 @@
       <c r="Z187" s="8"/>
     </row>
     <row r="188" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A188" s="8"/>
-      <c r="B188" s="8"/>
-      <c r="C188" s="39"/>
+      <c r="A188" s="8" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B188" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C188" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D188" s="8"/>
       <c r="E188" s="8"/>
-      <c r="G188" s="8"/>
+      <c r="G188" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H188" s="8"/>
       <c r="I188" s="8"/>
       <c r="J188" s="8"/>
@@ -14316,9 +14384,13 @@
       <c r="Z188" s="8"/>
     </row>
     <row r="189" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A189" s="8"/>
-      <c r="B189" s="8"/>
-      <c r="C189" s="39"/>
+      <c r="A189" s="8" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B189" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C189" s="8"/>
       <c r="D189" s="10"/>
       <c r="E189" s="8"/>
       <c r="G189" s="8"/>
@@ -14343,9 +14415,13 @@
       <c r="Z189" s="8"/>
     </row>
     <row r="190" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A190" s="8"/>
-      <c r="B190" s="8"/>
-      <c r="C190" s="39"/>
+      <c r="A190" s="8" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C190" s="8"/>
       <c r="D190" s="8"/>
       <c r="E190" s="8"/>
       <c r="G190" s="8"/>
@@ -14372,7 +14448,7 @@
     <row r="191" spans="1:26" ht="12.75" customHeight="1">
       <c r="A191" s="8"/>
       <c r="B191" s="8"/>
-      <c r="C191" s="39"/>
+      <c r="C191" s="42"/>
       <c r="D191" s="8"/>
       <c r="E191" s="8"/>
       <c r="G191" s="8"/>
@@ -14399,7 +14475,7 @@
     <row r="192" spans="1:26" ht="12.75" customHeight="1">
       <c r="A192" s="8"/>
       <c r="B192" s="8"/>
-      <c r="C192" s="39"/>
+      <c r="C192" s="42"/>
       <c r="D192" s="8"/>
       <c r="E192" s="8"/>
       <c r="G192" s="8"/>
@@ -14426,7 +14502,7 @@
     <row r="193" spans="1:26" ht="12.75" customHeight="1">
       <c r="A193" s="8"/>
       <c r="B193" s="8"/>
-      <c r="C193" s="39"/>
+      <c r="C193" s="42"/>
       <c r="D193" s="8"/>
       <c r="E193" s="8"/>
       <c r="G193" s="8"/>
@@ -14453,7 +14529,7 @@
     <row r="194" spans="1:26" ht="12.75" customHeight="1">
       <c r="A194" s="8"/>
       <c r="B194" s="8"/>
-      <c r="C194" s="39"/>
+      <c r="C194" s="42"/>
       <c r="D194" s="8"/>
       <c r="E194" s="8"/>
       <c r="G194" s="8"/>
@@ -14480,7 +14556,7 @@
     <row r="195" spans="1:26" ht="12.75" customHeight="1">
       <c r="A195" s="8"/>
       <c r="B195" s="8"/>
-      <c r="C195" s="39"/>
+      <c r="C195" s="42"/>
       <c r="D195" s="8"/>
       <c r="E195" s="8"/>
       <c r="G195" s="8"/>
@@ -14507,7 +14583,7 @@
     <row r="196" spans="1:26" ht="12.75" customHeight="1">
       <c r="A196" s="8"/>
       <c r="B196" s="8"/>
-      <c r="C196" s="39"/>
+      <c r="C196" s="42"/>
       <c r="D196" s="8"/>
       <c r="E196" s="8"/>
       <c r="G196" s="8"/>
@@ -14534,7 +14610,7 @@
     <row r="197" spans="1:26" ht="12.75" customHeight="1">
       <c r="A197" s="8"/>
       <c r="B197" s="8"/>
-      <c r="C197" s="39"/>
+      <c r="C197" s="42"/>
       <c r="D197" s="8"/>
       <c r="E197" s="8"/>
       <c r="G197" s="8"/>
@@ -14561,7 +14637,7 @@
     <row r="198" spans="1:26" ht="12.75" customHeight="1">
       <c r="A198" s="8"/>
       <c r="B198" s="8"/>
-      <c r="C198" s="39"/>
+      <c r="C198" s="42"/>
       <c r="D198" s="8"/>
       <c r="E198" s="8"/>
       <c r="G198" s="8"/>
@@ -14588,7 +14664,7 @@
     <row r="199" spans="1:26" ht="12.75" customHeight="1">
       <c r="A199" s="8"/>
       <c r="B199" s="8"/>
-      <c r="C199" s="39"/>
+      <c r="C199" s="42"/>
       <c r="D199" s="8"/>
       <c r="E199" s="8"/>
       <c r="G199" s="8"/>
@@ -14615,7 +14691,7 @@
     <row r="200" spans="1:26" ht="12.75" customHeight="1">
       <c r="A200" s="8"/>
       <c r="B200" s="8"/>
-      <c r="C200" s="39"/>
+      <c r="C200" s="42"/>
       <c r="D200" s="8"/>
       <c r="E200" s="8"/>
       <c r="G200" s="8"/>
@@ -14642,7 +14718,7 @@
     <row r="201" spans="1:26" ht="12.75" customHeight="1">
       <c r="A201" s="8"/>
       <c r="B201" s="8"/>
-      <c r="C201" s="39"/>
+      <c r="C201" s="42"/>
       <c r="D201" s="8"/>
       <c r="E201" s="8"/>
       <c r="G201" s="8"/>
@@ -14669,7 +14745,7 @@
     <row r="202" spans="1:26" ht="12.75" customHeight="1">
       <c r="A202" s="8"/>
       <c r="B202" s="8"/>
-      <c r="C202" s="39"/>
+      <c r="C202" s="42"/>
       <c r="D202" s="8"/>
       <c r="E202" s="8"/>
       <c r="G202" s="8"/>
@@ -14696,7 +14772,7 @@
     <row r="203" spans="1:26" ht="12.75" customHeight="1">
       <c r="A203" s="8"/>
       <c r="B203" s="8"/>
-      <c r="C203" s="39"/>
+      <c r="C203" s="42"/>
       <c r="D203" s="8"/>
       <c r="E203" s="8"/>
       <c r="G203" s="8"/>
@@ -14723,7 +14799,7 @@
     <row r="204" spans="1:26" ht="12.75" customHeight="1">
       <c r="A204" s="8"/>
       <c r="B204" s="8"/>
-      <c r="C204" s="39"/>
+      <c r="C204" s="42"/>
       <c r="D204" s="8"/>
       <c r="E204" s="8"/>
       <c r="G204" s="8"/>
@@ -14750,7 +14826,7 @@
     <row r="205" spans="1:26" ht="12.75" customHeight="1">
       <c r="A205" s="8"/>
       <c r="B205" s="8"/>
-      <c r="C205" s="39"/>
+      <c r="C205" s="42"/>
       <c r="D205" s="8"/>
       <c r="E205" s="8"/>
       <c r="G205" s="8"/>
@@ -14777,7 +14853,7 @@
     <row r="206" spans="1:26" ht="12.75" customHeight="1">
       <c r="A206" s="8"/>
       <c r="B206" s="8"/>
-      <c r="C206" s="39"/>
+      <c r="C206" s="42"/>
       <c r="D206" s="8"/>
       <c r="E206" s="8"/>
       <c r="G206" s="8"/>
@@ -14804,7 +14880,7 @@
     <row r="207" spans="1:26" ht="12.75" customHeight="1">
       <c r="A207" s="8"/>
       <c r="B207" s="8"/>
-      <c r="C207" s="39"/>
+      <c r="C207" s="42"/>
       <c r="D207" s="8"/>
       <c r="E207" s="8"/>
       <c r="G207" s="8"/>
@@ -14831,7 +14907,7 @@
     <row r="208" spans="1:26" ht="12.75" customHeight="1">
       <c r="A208" s="8"/>
       <c r="B208" s="8"/>
-      <c r="C208" s="39"/>
+      <c r="C208" s="42"/>
       <c r="D208" s="8"/>
       <c r="E208" s="8"/>
       <c r="G208" s="8"/>
@@ -14858,7 +14934,7 @@
     <row r="209" spans="1:26" ht="12.75" customHeight="1">
       <c r="A209" s="8"/>
       <c r="B209" s="8"/>
-      <c r="C209" s="39"/>
+      <c r="C209" s="42"/>
       <c r="D209" s="8"/>
       <c r="E209" s="8"/>
       <c r="G209" s="8"/>
@@ -14885,7 +14961,7 @@
     <row r="210" spans="1:26" ht="12.75" customHeight="1">
       <c r="A210" s="8"/>
       <c r="B210" s="8"/>
-      <c r="C210" s="39"/>
+      <c r="C210" s="42"/>
       <c r="D210" s="8"/>
       <c r="E210" s="8"/>
       <c r="G210" s="8"/>
@@ -14912,7 +14988,7 @@
     <row r="211" spans="1:26" ht="12.75" customHeight="1">
       <c r="A211" s="8"/>
       <c r="B211" s="8"/>
-      <c r="C211" s="39"/>
+      <c r="C211" s="42"/>
       <c r="D211" s="8"/>
       <c r="E211" s="8"/>
       <c r="G211" s="8"/>
@@ -14939,7 +15015,7 @@
     <row r="212" spans="1:26" ht="12.75" customHeight="1">
       <c r="A212" s="8"/>
       <c r="B212" s="8"/>
-      <c r="C212" s="39"/>
+      <c r="C212" s="42"/>
       <c r="D212" s="8"/>
       <c r="E212" s="8"/>
       <c r="G212" s="8"/>
@@ -14966,7 +15042,7 @@
     <row r="213" spans="1:26" ht="12.75" customHeight="1">
       <c r="A213" s="8"/>
       <c r="B213" s="8"/>
-      <c r="C213" s="39"/>
+      <c r="C213" s="42"/>
       <c r="D213" s="8"/>
       <c r="E213" s="8"/>
       <c r="G213" s="8"/>
@@ -14993,7 +15069,7 @@
     <row r="214" spans="1:26" ht="12.75" customHeight="1">
       <c r="A214" s="8"/>
       <c r="B214" s="8"/>
-      <c r="C214" s="39"/>
+      <c r="C214" s="42"/>
       <c r="D214" s="8"/>
       <c r="E214" s="8"/>
       <c r="G214" s="8"/>
@@ -15020,7 +15096,7 @@
     <row r="215" spans="1:26" ht="12.75" customHeight="1">
       <c r="A215" s="8"/>
       <c r="B215" s="8"/>
-      <c r="C215" s="39"/>
+      <c r="C215" s="42"/>
       <c r="D215" s="8"/>
       <c r="E215" s="8"/>
       <c r="G215" s="8"/>
@@ -15047,7 +15123,7 @@
     <row r="216" spans="1:26" ht="12.75" customHeight="1">
       <c r="A216" s="8"/>
       <c r="B216" s="8"/>
-      <c r="C216" s="39"/>
+      <c r="C216" s="42"/>
       <c r="D216" s="8"/>
       <c r="E216" s="8"/>
       <c r="G216" s="8"/>
@@ -15074,7 +15150,7 @@
     <row r="217" spans="1:26" ht="12.75" customHeight="1">
       <c r="A217" s="8"/>
       <c r="B217" s="8"/>
-      <c r="C217" s="39"/>
+      <c r="C217" s="42"/>
       <c r="D217" s="8"/>
       <c r="E217" s="8"/>
       <c r="G217" s="8"/>
@@ -15101,7 +15177,7 @@
     <row r="218" spans="1:26" ht="12.75" customHeight="1">
       <c r="A218" s="8"/>
       <c r="B218" s="8"/>
-      <c r="C218" s="39"/>
+      <c r="C218" s="42"/>
       <c r="D218" s="8"/>
       <c r="E218" s="8"/>
       <c r="G218" s="8"/>
@@ -15128,7 +15204,7 @@
     <row r="219" spans="1:26" ht="12.75" customHeight="1">
       <c r="A219" s="8"/>
       <c r="B219" s="8"/>
-      <c r="C219" s="39"/>
+      <c r="C219" s="42"/>
       <c r="D219" s="8"/>
       <c r="E219" s="8"/>
       <c r="G219" s="8"/>
@@ -15155,7 +15231,7 @@
     <row r="220" spans="1:26" ht="12.75" customHeight="1">
       <c r="A220" s="8"/>
       <c r="B220" s="8"/>
-      <c r="C220" s="39"/>
+      <c r="C220" s="42"/>
       <c r="D220" s="8"/>
       <c r="E220" s="8"/>
       <c r="G220" s="8"/>
@@ -15182,7 +15258,7 @@
     <row r="221" spans="1:26" ht="12.75" customHeight="1">
       <c r="A221" s="8"/>
       <c r="B221" s="8"/>
-      <c r="C221" s="39"/>
+      <c r="C221" s="42"/>
       <c r="D221" s="8"/>
       <c r="E221" s="8"/>
       <c r="G221" s="8"/>
@@ -15209,7 +15285,7 @@
     <row r="222" spans="1:26" ht="12.75" customHeight="1">
       <c r="A222" s="8"/>
       <c r="B222" s="8"/>
-      <c r="C222" s="39"/>
+      <c r="C222" s="42"/>
       <c r="D222" s="8"/>
       <c r="E222" s="8"/>
       <c r="G222" s="8"/>
@@ -15236,7 +15312,7 @@
     <row r="223" spans="1:26" ht="12.75" customHeight="1">
       <c r="A223" s="8"/>
       <c r="B223" s="8"/>
-      <c r="C223" s="39"/>
+      <c r="C223" s="42"/>
       <c r="D223" s="8"/>
       <c r="E223" s="8"/>
       <c r="G223" s="8"/>
@@ -15263,7 +15339,7 @@
     <row r="224" spans="1:26" ht="12.75" customHeight="1">
       <c r="A224" s="8"/>
       <c r="B224" s="8"/>
-      <c r="C224" s="39"/>
+      <c r="C224" s="42"/>
       <c r="D224" s="8"/>
       <c r="E224" s="8"/>
       <c r="G224" s="8"/>
@@ -15290,7 +15366,7 @@
     <row r="225" spans="1:26" ht="12.75" customHeight="1">
       <c r="A225" s="8"/>
       <c r="B225" s="8"/>
-      <c r="C225" s="39"/>
+      <c r="C225" s="42"/>
       <c r="D225" s="8"/>
       <c r="E225" s="8"/>
       <c r="G225" s="8"/>
@@ -15317,7 +15393,7 @@
     <row r="226" spans="1:26" ht="12.75" customHeight="1">
       <c r="A226" s="8"/>
       <c r="B226" s="8"/>
-      <c r="C226" s="39"/>
+      <c r="C226" s="42"/>
       <c r="D226" s="8"/>
       <c r="E226" s="8"/>
       <c r="G226" s="8"/>
@@ -15344,7 +15420,7 @@
     <row r="227" spans="1:26" ht="12.75" customHeight="1">
       <c r="A227" s="8"/>
       <c r="B227" s="8"/>
-      <c r="C227" s="39"/>
+      <c r="C227" s="42"/>
       <c r="D227" s="8"/>
       <c r="E227" s="8"/>
       <c r="G227" s="8"/>
@@ -15371,7 +15447,7 @@
     <row r="228" spans="1:26" ht="12.75" customHeight="1">
       <c r="A228" s="8"/>
       <c r="B228" s="8"/>
-      <c r="C228" s="39"/>
+      <c r="C228" s="42"/>
       <c r="D228" s="8"/>
       <c r="E228" s="8"/>
       <c r="G228" s="8"/>
@@ -15398,7 +15474,7 @@
     <row r="229" spans="1:26" ht="12.75" customHeight="1">
       <c r="A229" s="8"/>
       <c r="B229" s="8"/>
-      <c r="C229" s="39"/>
+      <c r="C229" s="42"/>
       <c r="D229" s="8"/>
       <c r="E229" s="8"/>
       <c r="G229" s="8"/>
@@ -15425,7 +15501,7 @@
     <row r="230" spans="1:26" ht="12.75" customHeight="1">
       <c r="A230" s="8"/>
       <c r="B230" s="8"/>
-      <c r="C230" s="39"/>
+      <c r="C230" s="42"/>
       <c r="D230" s="8"/>
       <c r="E230" s="8"/>
       <c r="G230" s="8"/>
@@ -15452,7 +15528,7 @@
     <row r="231" spans="1:26" ht="12.75" customHeight="1">
       <c r="A231" s="8"/>
       <c r="B231" s="8"/>
-      <c r="C231" s="39"/>
+      <c r="C231" s="42"/>
       <c r="D231" s="8"/>
       <c r="E231" s="8"/>
       <c r="G231" s="8"/>
@@ -15479,7 +15555,7 @@
     <row r="232" spans="1:26" ht="12.75" customHeight="1">
       <c r="A232" s="8"/>
       <c r="B232" s="8"/>
-      <c r="C232" s="39"/>
+      <c r="C232" s="42"/>
       <c r="D232" s="8"/>
       <c r="E232" s="8"/>
       <c r="G232" s="8"/>
@@ -15506,7 +15582,7 @@
     <row r="233" spans="1:26" ht="12.75" customHeight="1">
       <c r="A233" s="8"/>
       <c r="B233" s="8"/>
-      <c r="C233" s="39"/>
+      <c r="C233" s="42"/>
       <c r="D233" s="8"/>
       <c r="E233" s="8"/>
       <c r="G233" s="8"/>
@@ -15533,7 +15609,7 @@
     <row r="234" spans="1:26" ht="12.75" customHeight="1">
       <c r="A234" s="8"/>
       <c r="B234" s="8"/>
-      <c r="C234" s="39"/>
+      <c r="C234" s="42"/>
       <c r="D234" s="8"/>
       <c r="E234" s="8"/>
       <c r="G234" s="8"/>
@@ -15560,7 +15636,7 @@
     <row r="235" spans="1:26" ht="12.75" customHeight="1">
       <c r="A235" s="8"/>
       <c r="B235" s="8"/>
-      <c r="C235" s="39"/>
+      <c r="C235" s="42"/>
       <c r="D235" s="8"/>
       <c r="E235" s="8"/>
       <c r="G235" s="8"/>
@@ -15587,7 +15663,7 @@
     <row r="236" spans="1:26" ht="12.75" customHeight="1">
       <c r="A236" s="8"/>
       <c r="B236" s="8"/>
-      <c r="C236" s="39"/>
+      <c r="C236" s="42"/>
       <c r="D236" s="8"/>
       <c r="E236" s="8"/>
       <c r="G236" s="8"/>
@@ -15614,7 +15690,7 @@
     <row r="237" spans="1:26" ht="12.75" customHeight="1">
       <c r="A237" s="8"/>
       <c r="B237" s="8"/>
-      <c r="C237" s="39"/>
+      <c r="C237" s="42"/>
       <c r="D237" s="8"/>
       <c r="E237" s="8"/>
       <c r="G237" s="8"/>
@@ -15641,7 +15717,7 @@
     <row r="238" spans="1:26" ht="12.75" customHeight="1">
       <c r="A238" s="8"/>
       <c r="B238" s="8"/>
-      <c r="C238" s="39"/>
+      <c r="C238" s="42"/>
       <c r="D238" s="8"/>
       <c r="E238" s="8"/>
       <c r="G238" s="8"/>
@@ -15668,7 +15744,7 @@
     <row r="239" spans="1:26" ht="12.75" customHeight="1">
       <c r="A239" s="8"/>
       <c r="B239" s="8"/>
-      <c r="C239" s="39"/>
+      <c r="C239" s="42"/>
       <c r="D239" s="8"/>
       <c r="E239" s="8"/>
       <c r="G239" s="8"/>
@@ -15695,7 +15771,7 @@
     <row r="240" spans="1:26" ht="12.75" customHeight="1">
       <c r="A240" s="8"/>
       <c r="B240" s="8"/>
-      <c r="C240" s="39"/>
+      <c r="C240" s="42"/>
       <c r="D240" s="8"/>
       <c r="E240" s="8"/>
       <c r="G240" s="8"/>
@@ -15722,7 +15798,7 @@
     <row r="241" spans="1:26" ht="12.75" customHeight="1">
       <c r="A241" s="8"/>
       <c r="B241" s="8"/>
-      <c r="C241" s="39"/>
+      <c r="C241" s="42"/>
       <c r="D241" s="8"/>
       <c r="E241" s="8"/>
       <c r="G241" s="8"/>
@@ -15749,7 +15825,7 @@
     <row r="242" spans="1:26" ht="12.75" customHeight="1">
       <c r="A242" s="8"/>
       <c r="B242" s="8"/>
-      <c r="C242" s="39"/>
+      <c r="C242" s="42"/>
       <c r="D242" s="8"/>
       <c r="E242" s="8"/>
       <c r="G242" s="8"/>
@@ -15776,7 +15852,7 @@
     <row r="243" spans="1:26" ht="12.75" customHeight="1">
       <c r="A243" s="8"/>
       <c r="B243" s="8"/>
-      <c r="C243" s="39"/>
+      <c r="C243" s="42"/>
       <c r="D243" s="8"/>
       <c r="E243" s="8"/>
       <c r="G243" s="8"/>
@@ -15803,7 +15879,7 @@
     <row r="244" spans="1:26" ht="12.75" customHeight="1">
       <c r="A244" s="8"/>
       <c r="B244" s="8"/>
-      <c r="C244" s="39"/>
+      <c r="C244" s="42"/>
       <c r="D244" s="8"/>
       <c r="E244" s="8"/>
       <c r="G244" s="8"/>
@@ -15830,7 +15906,7 @@
     <row r="245" spans="1:26" ht="12.75" customHeight="1">
       <c r="A245" s="8"/>
       <c r="B245" s="8"/>
-      <c r="C245" s="39"/>
+      <c r="C245" s="42"/>
       <c r="D245" s="8"/>
       <c r="E245" s="8"/>
       <c r="G245" s="8"/>
@@ -15857,7 +15933,7 @@
     <row r="246" spans="1:26" ht="12.75" customHeight="1">
       <c r="A246" s="8"/>
       <c r="B246" s="8"/>
-      <c r="C246" s="39"/>
+      <c r="C246" s="42"/>
       <c r="D246" s="8"/>
       <c r="E246" s="8"/>
       <c r="G246" s="8"/>
@@ -15884,7 +15960,7 @@
     <row r="247" spans="1:26" ht="12.75" customHeight="1">
       <c r="A247" s="8"/>
       <c r="B247" s="8"/>
-      <c r="C247" s="39"/>
+      <c r="C247" s="42"/>
       <c r="D247" s="8"/>
       <c r="E247" s="8"/>
       <c r="G247" s="8"/>
@@ -15911,7 +15987,7 @@
     <row r="248" spans="1:26" ht="12.75" customHeight="1">
       <c r="A248" s="8"/>
       <c r="B248" s="8"/>
-      <c r="C248" s="39"/>
+      <c r="C248" s="42"/>
       <c r="D248" s="8"/>
       <c r="E248" s="8"/>
       <c r="G248" s="8"/>
@@ -15938,7 +16014,7 @@
     <row r="249" spans="1:26" ht="12.75" customHeight="1">
       <c r="A249" s="8"/>
       <c r="B249" s="8"/>
-      <c r="C249" s="39"/>
+      <c r="C249" s="42"/>
       <c r="D249" s="8"/>
       <c r="E249" s="8"/>
       <c r="G249" s="8"/>
@@ -15965,7 +16041,7 @@
     <row r="250" spans="1:26" ht="12.75" customHeight="1">
       <c r="A250" s="8"/>
       <c r="B250" s="8"/>
-      <c r="C250" s="39"/>
+      <c r="C250" s="42"/>
       <c r="D250" s="8"/>
       <c r="E250" s="8"/>
       <c r="G250" s="8"/>
@@ -15992,7 +16068,7 @@
     <row r="251" spans="1:26" ht="12.75" customHeight="1">
       <c r="A251" s="8"/>
       <c r="B251" s="8"/>
-      <c r="C251" s="39"/>
+      <c r="C251" s="42"/>
       <c r="D251" s="8"/>
       <c r="E251" s="8"/>
       <c r="G251" s="8"/>
@@ -16019,7 +16095,7 @@
     <row r="252" spans="1:26" ht="12.75" customHeight="1">
       <c r="A252" s="8"/>
       <c r="B252" s="8"/>
-      <c r="C252" s="39"/>
+      <c r="C252" s="42"/>
       <c r="D252" s="8"/>
       <c r="E252" s="8"/>
       <c r="G252" s="8"/>
@@ -16046,7 +16122,7 @@
     <row r="253" spans="1:26" ht="12.75" customHeight="1">
       <c r="A253" s="12"/>
       <c r="B253" s="12"/>
-      <c r="C253" s="42"/>
+      <c r="C253" s="43"/>
       <c r="D253" s="12"/>
       <c r="E253" s="12"/>
       <c r="G253" s="12"/>
@@ -16073,7 +16149,7 @@
     <row r="254" spans="1:26" ht="12.75" customHeight="1">
       <c r="A254" s="12"/>
       <c r="B254" s="12"/>
-      <c r="C254" s="42"/>
+      <c r="C254" s="43"/>
       <c r="D254" s="12"/>
       <c r="E254" s="12"/>
       <c r="G254" s="12"/>
@@ -16100,7 +16176,7 @@
     <row r="255" spans="1:26" ht="12.75" customHeight="1">
       <c r="A255" s="12"/>
       <c r="B255" s="12"/>
-      <c r="C255" s="42"/>
+      <c r="C255" s="43"/>
       <c r="D255" s="12"/>
       <c r="E255" s="12"/>
       <c r="G255" s="12"/>
@@ -16127,7 +16203,7 @@
     <row r="256" spans="1:26" ht="12.75" customHeight="1">
       <c r="A256" s="12"/>
       <c r="B256" s="12"/>
-      <c r="C256" s="42"/>
+      <c r="C256" s="43"/>
       <c r="D256" s="12"/>
       <c r="E256" s="12"/>
       <c r="G256" s="12"/>
@@ -16154,7 +16230,7 @@
     <row r="257" spans="1:26" ht="12.75" customHeight="1">
       <c r="A257" s="12"/>
       <c r="B257" s="12"/>
-      <c r="C257" s="42"/>
+      <c r="C257" s="43"/>
       <c r="D257" s="12"/>
       <c r="E257" s="12"/>
       <c r="G257" s="12"/>
@@ -16181,7 +16257,7 @@
     <row r="258" spans="1:26" ht="12.75" customHeight="1">
       <c r="A258" s="12"/>
       <c r="B258" s="12"/>
-      <c r="C258" s="42"/>
+      <c r="C258" s="43"/>
       <c r="D258" s="12"/>
       <c r="E258" s="12"/>
       <c r="G258" s="12"/>
@@ -16208,7 +16284,7 @@
     <row r="259" spans="1:26" ht="12.75" customHeight="1">
       <c r="A259" s="12"/>
       <c r="B259" s="12"/>
-      <c r="C259" s="42"/>
+      <c r="C259" s="43"/>
       <c r="D259" s="12"/>
       <c r="E259" s="12"/>
       <c r="G259" s="12"/>
@@ -16235,7 +16311,7 @@
     <row r="260" spans="1:26" ht="12.75" customHeight="1">
       <c r="A260" s="12"/>
       <c r="B260" s="12"/>
-      <c r="C260" s="42"/>
+      <c r="C260" s="43"/>
       <c r="D260" s="12"/>
       <c r="E260" s="12"/>
       <c r="G260" s="12"/>
@@ -16262,7 +16338,7 @@
     <row r="261" spans="1:26" ht="12.75" customHeight="1">
       <c r="A261" s="12"/>
       <c r="B261" s="12"/>
-      <c r="C261" s="42"/>
+      <c r="C261" s="43"/>
       <c r="D261" s="12"/>
       <c r="E261" s="12"/>
       <c r="G261" s="12"/>
@@ -16289,7 +16365,7 @@
     <row r="262" spans="1:26" ht="12.75" customHeight="1">
       <c r="A262" s="12"/>
       <c r="B262" s="12"/>
-      <c r="C262" s="42"/>
+      <c r="C262" s="43"/>
       <c r="D262" s="12"/>
       <c r="E262" s="12"/>
       <c r="G262" s="12"/>
@@ -16316,7 +16392,7 @@
     <row r="263" spans="1:26" ht="12.75" customHeight="1">
       <c r="A263" s="12"/>
       <c r="B263" s="12"/>
-      <c r="C263" s="42"/>
+      <c r="C263" s="43"/>
       <c r="D263" s="12"/>
       <c r="E263" s="12"/>
       <c r="G263" s="12"/>
@@ -16343,7 +16419,7 @@
     <row r="264" spans="1:26" ht="12.75" customHeight="1">
       <c r="A264" s="12"/>
       <c r="B264" s="12"/>
-      <c r="C264" s="42"/>
+      <c r="C264" s="43"/>
       <c r="D264" s="12"/>
       <c r="E264" s="12"/>
       <c r="G264" s="12"/>
@@ -16370,7 +16446,7 @@
     <row r="265" spans="1:26" ht="12.75" customHeight="1">
       <c r="A265" s="12"/>
       <c r="B265" s="12"/>
-      <c r="C265" s="42"/>
+      <c r="C265" s="43"/>
       <c r="D265" s="12"/>
       <c r="E265" s="12"/>
       <c r="G265" s="12"/>
@@ -16397,7 +16473,7 @@
     <row r="266" spans="1:26" ht="12.75" customHeight="1">
       <c r="A266" s="12"/>
       <c r="B266" s="12"/>
-      <c r="C266" s="42"/>
+      <c r="C266" s="43"/>
       <c r="D266" s="12"/>
       <c r="E266" s="12"/>
       <c r="G266" s="12"/>
@@ -16424,7 +16500,7 @@
     <row r="267" spans="1:26" ht="12.75" customHeight="1">
       <c r="A267" s="12"/>
       <c r="B267" s="12"/>
-      <c r="C267" s="42"/>
+      <c r="C267" s="43"/>
       <c r="D267" s="12"/>
       <c r="E267" s="12"/>
       <c r="G267" s="12"/>
@@ -16451,7 +16527,7 @@
     <row r="268" spans="1:26" ht="12.75" customHeight="1">
       <c r="A268" s="12"/>
       <c r="B268" s="12"/>
-      <c r="C268" s="42"/>
+      <c r="C268" s="43"/>
       <c r="D268" s="12"/>
       <c r="E268" s="12"/>
       <c r="G268" s="12"/>
@@ -16478,7 +16554,7 @@
     <row r="269" spans="1:26" ht="12.75" customHeight="1">
       <c r="A269" s="12"/>
       <c r="B269" s="12"/>
-      <c r="C269" s="42"/>
+      <c r="C269" s="43"/>
       <c r="D269" s="12"/>
       <c r="E269" s="12"/>
       <c r="G269" s="12"/>
@@ -16505,7 +16581,7 @@
     <row r="270" spans="1:26" ht="12.75" customHeight="1">
       <c r="A270" s="12"/>
       <c r="B270" s="12"/>
-      <c r="C270" s="42"/>
+      <c r="C270" s="43"/>
       <c r="D270" s="12"/>
       <c r="E270" s="12"/>
       <c r="G270" s="12"/>
@@ -16532,7 +16608,7 @@
     <row r="271" spans="1:26" ht="12.75" customHeight="1">
       <c r="A271" s="12"/>
       <c r="B271" s="12"/>
-      <c r="C271" s="42"/>
+      <c r="C271" s="43"/>
       <c r="D271" s="12"/>
       <c r="E271" s="12"/>
       <c r="G271" s="12"/>
@@ -16559,7 +16635,7 @@
     <row r="272" spans="1:26" ht="12.75" customHeight="1">
       <c r="A272" s="12"/>
       <c r="B272" s="12"/>
-      <c r="C272" s="42"/>
+      <c r="C272" s="43"/>
       <c r="D272" s="12"/>
       <c r="E272" s="12"/>
       <c r="G272" s="12"/>
@@ -16586,7 +16662,7 @@
     <row r="273" spans="1:26" ht="12.75" customHeight="1">
       <c r="A273" s="12"/>
       <c r="B273" s="12"/>
-      <c r="C273" s="42"/>
+      <c r="C273" s="43"/>
       <c r="D273" s="12"/>
       <c r="E273" s="12"/>
       <c r="G273" s="12"/>
@@ -16613,7 +16689,7 @@
     <row r="274" spans="1:26" ht="12.75" customHeight="1">
       <c r="A274" s="12"/>
       <c r="B274" s="12"/>
-      <c r="C274" s="42"/>
+      <c r="C274" s="43"/>
       <c r="D274" s="12"/>
       <c r="E274" s="12"/>
       <c r="G274" s="12"/>
@@ -16640,7 +16716,7 @@
     <row r="275" spans="1:26" ht="12.75" customHeight="1">
       <c r="A275" s="12"/>
       <c r="B275" s="12"/>
-      <c r="C275" s="42"/>
+      <c r="C275" s="43"/>
       <c r="D275" s="12"/>
       <c r="E275" s="12"/>
       <c r="G275" s="12"/>
@@ -16667,7 +16743,7 @@
     <row r="276" spans="1:26" ht="12.75" customHeight="1">
       <c r="A276" s="12"/>
       <c r="B276" s="12"/>
-      <c r="C276" s="42"/>
+      <c r="C276" s="43"/>
       <c r="D276" s="12"/>
       <c r="E276" s="12"/>
       <c r="G276" s="12"/>
@@ -16694,7 +16770,7 @@
     <row r="277" spans="1:26" ht="12.75" customHeight="1">
       <c r="A277" s="12"/>
       <c r="B277" s="12"/>
-      <c r="C277" s="42"/>
+      <c r="C277" s="43"/>
       <c r="D277" s="12"/>
       <c r="E277" s="12"/>
       <c r="G277" s="12"/>
@@ -16721,7 +16797,7 @@
     <row r="278" spans="1:26" ht="12.75" customHeight="1">
       <c r="A278" s="12"/>
       <c r="B278" s="12"/>
-      <c r="C278" s="42"/>
+      <c r="C278" s="43"/>
       <c r="D278" s="12"/>
       <c r="E278" s="12"/>
       <c r="G278" s="12"/>
@@ -16748,7 +16824,7 @@
     <row r="279" spans="1:26" ht="12.75" customHeight="1">
       <c r="A279" s="12"/>
       <c r="B279" s="12"/>
-      <c r="C279" s="42"/>
+      <c r="C279" s="43"/>
       <c r="D279" s="12"/>
       <c r="E279" s="12"/>
       <c r="G279" s="12"/>
@@ -16775,7 +16851,7 @@
     <row r="280" spans="1:26" ht="12.75" customHeight="1">
       <c r="A280" s="12"/>
       <c r="B280" s="12"/>
-      <c r="C280" s="42"/>
+      <c r="C280" s="43"/>
       <c r="D280" s="12"/>
       <c r="E280" s="12"/>
       <c r="G280" s="12"/>
@@ -16802,7 +16878,7 @@
     <row r="281" spans="1:26" ht="12.75" customHeight="1">
       <c r="A281" s="12"/>
       <c r="B281" s="12"/>
-      <c r="C281" s="42"/>
+      <c r="C281" s="43"/>
       <c r="D281" s="12"/>
       <c r="E281" s="12"/>
       <c r="G281" s="12"/>
@@ -16829,7 +16905,7 @@
     <row r="282" spans="1:26" ht="12.75" customHeight="1">
       <c r="A282" s="12"/>
       <c r="B282" s="12"/>
-      <c r="C282" s="42"/>
+      <c r="C282" s="43"/>
       <c r="D282" s="12"/>
       <c r="E282" s="12"/>
       <c r="G282" s="12"/>
@@ -16856,7 +16932,7 @@
     <row r="283" spans="1:26" ht="12.75" customHeight="1">
       <c r="A283" s="12"/>
       <c r="B283" s="12"/>
-      <c r="C283" s="42"/>
+      <c r="C283" s="43"/>
       <c r="D283" s="12"/>
       <c r="E283" s="12"/>
       <c r="G283" s="12"/>
@@ -16883,7 +16959,7 @@
     <row r="284" spans="1:26" ht="12.75" customHeight="1">
       <c r="A284" s="12"/>
       <c r="B284" s="12"/>
-      <c r="C284" s="42"/>
+      <c r="C284" s="43"/>
       <c r="D284" s="12"/>
       <c r="E284" s="12"/>
       <c r="G284" s="12"/>
@@ -16910,7 +16986,7 @@
     <row r="285" spans="1:26" ht="12.75" customHeight="1">
       <c r="A285" s="12"/>
       <c r="B285" s="12"/>
-      <c r="C285" s="42"/>
+      <c r="C285" s="43"/>
       <c r="D285" s="12"/>
       <c r="E285" s="12"/>
       <c r="G285" s="12"/>
@@ -16937,7 +17013,7 @@
     <row r="286" spans="1:26" ht="12.75" customHeight="1">
       <c r="A286" s="12"/>
       <c r="B286" s="12"/>
-      <c r="C286" s="42"/>
+      <c r="C286" s="43"/>
       <c r="D286" s="12"/>
       <c r="E286" s="12"/>
       <c r="G286" s="12"/>
@@ -16964,7 +17040,7 @@
     <row r="287" spans="1:26" ht="12.75" customHeight="1">
       <c r="A287" s="12"/>
       <c r="B287" s="12"/>
-      <c r="C287" s="42"/>
+      <c r="C287" s="43"/>
       <c r="D287" s="12"/>
       <c r="E287" s="12"/>
       <c r="G287" s="12"/>
@@ -16991,7 +17067,7 @@
     <row r="288" spans="1:26" ht="12.75" customHeight="1">
       <c r="A288" s="12"/>
       <c r="B288" s="12"/>
-      <c r="C288" s="42"/>
+      <c r="C288" s="43"/>
       <c r="D288" s="12"/>
       <c r="E288" s="12"/>
       <c r="G288" s="12"/>
@@ -17018,7 +17094,7 @@
     <row r="289" spans="1:26" ht="12.75" customHeight="1">
       <c r="A289" s="12"/>
       <c r="B289" s="12"/>
-      <c r="C289" s="42"/>
+      <c r="C289" s="43"/>
       <c r="D289" s="12"/>
       <c r="E289" s="12"/>
       <c r="G289" s="12"/>
@@ -17045,7 +17121,7 @@
     <row r="290" spans="1:26" ht="12.75" customHeight="1">
       <c r="A290" s="12"/>
       <c r="B290" s="12"/>
-      <c r="C290" s="42"/>
+      <c r="C290" s="43"/>
       <c r="D290" s="12"/>
       <c r="E290" s="12"/>
       <c r="G290" s="12"/>
@@ -17072,7 +17148,7 @@
     <row r="291" spans="1:26" ht="12.75" customHeight="1">
       <c r="A291" s="12"/>
       <c r="B291" s="12"/>
-      <c r="C291" s="42"/>
+      <c r="C291" s="43"/>
       <c r="D291" s="12"/>
       <c r="E291" s="12"/>
       <c r="G291" s="12"/>
@@ -17099,7 +17175,7 @@
     <row r="292" spans="1:26" ht="12.75" customHeight="1">
       <c r="A292" s="12"/>
       <c r="B292" s="12"/>
-      <c r="C292" s="42"/>
+      <c r="C292" s="43"/>
       <c r="D292" s="12"/>
       <c r="E292" s="12"/>
       <c r="G292" s="12"/>
@@ -17126,7 +17202,7 @@
     <row r="293" spans="1:26" ht="12.75" customHeight="1">
       <c r="A293" s="12"/>
       <c r="B293" s="12"/>
-      <c r="C293" s="42"/>
+      <c r="C293" s="43"/>
       <c r="D293" s="12"/>
       <c r="E293" s="12"/>
       <c r="G293" s="12"/>
@@ -17153,7 +17229,7 @@
     <row r="294" spans="1:26" ht="12.75" customHeight="1">
       <c r="A294" s="12"/>
       <c r="B294" s="12"/>
-      <c r="C294" s="42"/>
+      <c r="C294" s="43"/>
       <c r="D294" s="12"/>
       <c r="E294" s="12"/>
       <c r="G294" s="12"/>
@@ -17180,7 +17256,7 @@
     <row r="295" spans="1:26" ht="12.75" customHeight="1">
       <c r="A295" s="12"/>
       <c r="B295" s="12"/>
-      <c r="C295" s="42"/>
+      <c r="C295" s="43"/>
       <c r="D295" s="12"/>
       <c r="E295" s="12"/>
       <c r="G295" s="12"/>
@@ -17207,7 +17283,7 @@
     <row r="296" spans="1:26" ht="12.75" customHeight="1">
       <c r="A296" s="12"/>
       <c r="B296" s="12"/>
-      <c r="C296" s="42"/>
+      <c r="C296" s="43"/>
       <c r="D296" s="12"/>
       <c r="E296" s="12"/>
       <c r="G296" s="12"/>
@@ -17234,7 +17310,7 @@
     <row r="297" spans="1:26" ht="12.75" customHeight="1">
       <c r="A297" s="12"/>
       <c r="B297" s="12"/>
-      <c r="C297" s="42"/>
+      <c r="C297" s="43"/>
       <c r="D297" s="12"/>
       <c r="E297" s="12"/>
       <c r="G297" s="12"/>
@@ -17261,7 +17337,7 @@
     <row r="298" spans="1:26" ht="12.75" customHeight="1">
       <c r="A298" s="12"/>
       <c r="B298" s="12"/>
-      <c r="C298" s="42"/>
+      <c r="C298" s="43"/>
       <c r="D298" s="12"/>
       <c r="E298" s="12"/>
       <c r="G298" s="12"/>
@@ -17288,7 +17364,7 @@
     <row r="299" spans="1:26" ht="12.75" customHeight="1">
       <c r="A299" s="12"/>
       <c r="B299" s="12"/>
-      <c r="C299" s="42"/>
+      <c r="C299" s="43"/>
       <c r="D299" s="12"/>
       <c r="E299" s="12"/>
       <c r="G299" s="12"/>
@@ -17315,7 +17391,7 @@
     <row r="300" spans="1:26" ht="12.75" customHeight="1">
       <c r="A300" s="12"/>
       <c r="B300" s="12"/>
-      <c r="C300" s="42"/>
+      <c r="C300" s="43"/>
       <c r="D300" s="12"/>
       <c r="E300" s="12"/>
       <c r="G300" s="12"/>
@@ -17342,7 +17418,7 @@
     <row r="301" spans="1:26" ht="12.75" customHeight="1">
       <c r="A301" s="12"/>
       <c r="B301" s="12"/>
-      <c r="C301" s="42"/>
+      <c r="C301" s="43"/>
       <c r="D301" s="12"/>
       <c r="E301" s="12"/>
       <c r="G301" s="12"/>
@@ -17369,7 +17445,7 @@
     <row r="302" spans="1:26" ht="12.75" customHeight="1">
       <c r="A302" s="12"/>
       <c r="B302" s="12"/>
-      <c r="C302" s="42"/>
+      <c r="C302" s="43"/>
       <c r="D302" s="12"/>
       <c r="E302" s="12"/>
       <c r="G302" s="12"/>
@@ -17396,7 +17472,7 @@
     <row r="303" spans="1:26" ht="12.75" customHeight="1">
       <c r="A303" s="12"/>
       <c r="B303" s="12"/>
-      <c r="C303" s="42"/>
+      <c r="C303" s="43"/>
       <c r="D303" s="12"/>
       <c r="E303" s="12"/>
       <c r="G303" s="12"/>
@@ -17423,7 +17499,7 @@
     <row r="304" spans="1:26" ht="12.75" customHeight="1">
       <c r="A304" s="12"/>
       <c r="B304" s="12"/>
-      <c r="C304" s="42"/>
+      <c r="C304" s="43"/>
       <c r="D304" s="12"/>
       <c r="E304" s="12"/>
       <c r="G304" s="12"/>
@@ -17450,7 +17526,7 @@
     <row r="305" spans="1:26" ht="12.75" customHeight="1">
       <c r="A305" s="12"/>
       <c r="B305" s="12"/>
-      <c r="C305" s="42"/>
+      <c r="C305" s="43"/>
       <c r="D305" s="12"/>
       <c r="E305" s="12"/>
       <c r="G305" s="12"/>
@@ -17477,7 +17553,7 @@
     <row r="306" spans="1:26" ht="12.75" customHeight="1">
       <c r="A306" s="12"/>
       <c r="B306" s="12"/>
-      <c r="C306" s="42"/>
+      <c r="C306" s="43"/>
       <c r="D306" s="12"/>
       <c r="E306" s="12"/>
       <c r="G306" s="12"/>
@@ -17504,7 +17580,7 @@
     <row r="307" spans="1:26" ht="12.75" customHeight="1">
       <c r="A307" s="12"/>
       <c r="B307" s="12"/>
-      <c r="C307" s="42"/>
+      <c r="C307" s="43"/>
       <c r="D307" s="12"/>
       <c r="E307" s="12"/>
       <c r="G307" s="12"/>
@@ -17531,7 +17607,7 @@
     <row r="308" spans="1:26" ht="12.75" customHeight="1">
       <c r="A308" s="12"/>
       <c r="B308" s="12"/>
-      <c r="C308" s="42"/>
+      <c r="C308" s="43"/>
       <c r="D308" s="12"/>
       <c r="E308" s="12"/>
       <c r="G308" s="12"/>
@@ -17558,7 +17634,7 @@
     <row r="309" spans="1:26" ht="12.75" customHeight="1">
       <c r="A309" s="12"/>
       <c r="B309" s="12"/>
-      <c r="C309" s="42"/>
+      <c r="C309" s="43"/>
       <c r="D309" s="12"/>
       <c r="E309" s="12"/>
       <c r="G309" s="12"/>
@@ -17585,7 +17661,7 @@
     <row r="310" spans="1:26" ht="12.75" customHeight="1">
       <c r="A310" s="12"/>
       <c r="B310" s="12"/>
-      <c r="C310" s="42"/>
+      <c r="C310" s="43"/>
       <c r="D310" s="12"/>
       <c r="E310" s="12"/>
       <c r="G310" s="12"/>
@@ -17612,7 +17688,7 @@
     <row r="311" spans="1:26" ht="12.75" customHeight="1">
       <c r="A311" s="12"/>
       <c r="B311" s="12"/>
-      <c r="C311" s="42"/>
+      <c r="C311" s="43"/>
       <c r="D311" s="12"/>
       <c r="E311" s="12"/>
       <c r="G311" s="12"/>
@@ -17639,7 +17715,7 @@
     <row r="312" spans="1:26" ht="12.75" customHeight="1">
       <c r="A312" s="12"/>
       <c r="B312" s="12"/>
-      <c r="C312" s="42"/>
+      <c r="C312" s="43"/>
       <c r="D312" s="12"/>
       <c r="E312" s="12"/>
       <c r="G312" s="12"/>
@@ -17666,7 +17742,7 @@
     <row r="313" spans="1:26" ht="12.75" customHeight="1">
       <c r="A313" s="12"/>
       <c r="B313" s="12"/>
-      <c r="C313" s="42"/>
+      <c r="C313" s="43"/>
       <c r="D313" s="12"/>
       <c r="E313" s="12"/>
       <c r="G313" s="12"/>
@@ -17693,7 +17769,7 @@
     <row r="314" spans="1:26" ht="12.75" customHeight="1">
       <c r="A314" s="12"/>
       <c r="B314" s="12"/>
-      <c r="C314" s="42"/>
+      <c r="C314" s="43"/>
       <c r="D314" s="12"/>
       <c r="E314" s="12"/>
       <c r="G314" s="12"/>
@@ -17720,7 +17796,7 @@
     <row r="315" spans="1:26" ht="12.75" customHeight="1">
       <c r="A315" s="12"/>
       <c r="B315" s="12"/>
-      <c r="C315" s="42"/>
+      <c r="C315" s="43"/>
       <c r="D315" s="12"/>
       <c r="E315" s="12"/>
       <c r="G315" s="12"/>
@@ -17747,7 +17823,7 @@
     <row r="316" spans="1:26" ht="12.75" customHeight="1">
       <c r="A316" s="12"/>
       <c r="B316" s="12"/>
-      <c r="C316" s="42"/>
+      <c r="C316" s="43"/>
       <c r="D316" s="12"/>
       <c r="E316" s="12"/>
       <c r="G316" s="12"/>
@@ -17774,7 +17850,7 @@
     <row r="317" spans="1:26" ht="12.75" customHeight="1">
       <c r="A317" s="12"/>
       <c r="B317" s="12"/>
-      <c r="C317" s="42"/>
+      <c r="C317" s="43"/>
       <c r="D317" s="12"/>
       <c r="E317" s="12"/>
       <c r="G317" s="12"/>
@@ -17801,7 +17877,7 @@
     <row r="318" spans="1:26" ht="12.75" customHeight="1">
       <c r="A318" s="12"/>
       <c r="B318" s="12"/>
-      <c r="C318" s="42"/>
+      <c r="C318" s="43"/>
       <c r="D318" s="12"/>
       <c r="E318" s="12"/>
       <c r="G318" s="12"/>
@@ -17828,7 +17904,7 @@
     <row r="319" spans="1:26" ht="12.75" customHeight="1">
       <c r="A319" s="12"/>
       <c r="B319" s="12"/>
-      <c r="C319" s="42"/>
+      <c r="C319" s="43"/>
       <c r="D319" s="12"/>
       <c r="E319" s="12"/>
       <c r="G319" s="12"/>
@@ -17855,7 +17931,7 @@
     <row r="320" spans="1:26" ht="12.75" customHeight="1">
       <c r="A320" s="12"/>
       <c r="B320" s="12"/>
-      <c r="C320" s="42"/>
+      <c r="C320" s="43"/>
       <c r="D320" s="12"/>
       <c r="E320" s="12"/>
       <c r="G320" s="12"/>
@@ -17882,7 +17958,7 @@
     <row r="321" spans="1:26" ht="12.75" customHeight="1">
       <c r="A321" s="12"/>
       <c r="B321" s="12"/>
-      <c r="C321" s="42"/>
+      <c r="C321" s="43"/>
       <c r="D321" s="12"/>
       <c r="E321" s="12"/>
       <c r="G321" s="12"/>
@@ -17909,7 +17985,7 @@
     <row r="322" spans="1:26" ht="12.75" customHeight="1">
       <c r="A322" s="12"/>
       <c r="B322" s="12"/>
-      <c r="C322" s="42"/>
+      <c r="C322" s="43"/>
       <c r="D322" s="12"/>
       <c r="E322" s="12"/>
       <c r="G322" s="12"/>
@@ -17936,7 +18012,7 @@
     <row r="323" spans="1:26" ht="12.75" customHeight="1">
       <c r="A323" s="12"/>
       <c r="B323" s="12"/>
-      <c r="C323" s="42"/>
+      <c r="C323" s="43"/>
       <c r="D323" s="12"/>
       <c r="E323" s="12"/>
       <c r="G323" s="12"/>
@@ -17963,7 +18039,7 @@
     <row r="324" spans="1:26" ht="12.75" customHeight="1">
       <c r="A324" s="12"/>
       <c r="B324" s="12"/>
-      <c r="C324" s="42"/>
+      <c r="C324" s="43"/>
       <c r="D324" s="12"/>
       <c r="E324" s="12"/>
       <c r="G324" s="12"/>
@@ -17990,7 +18066,7 @@
     <row r="325" spans="1:26" ht="12.75" customHeight="1">
       <c r="A325" s="12"/>
       <c r="B325" s="12"/>
-      <c r="C325" s="42"/>
+      <c r="C325" s="43"/>
       <c r="D325" s="12"/>
       <c r="E325" s="12"/>
       <c r="G325" s="12"/>
@@ -18017,7 +18093,7 @@
     <row r="326" spans="1:26" ht="12.75" customHeight="1">
       <c r="A326" s="12"/>
       <c r="B326" s="12"/>
-      <c r="C326" s="42"/>
+      <c r="C326" s="43"/>
       <c r="D326" s="12"/>
       <c r="E326" s="12"/>
       <c r="G326" s="12"/>
@@ -18044,7 +18120,7 @@
     <row r="327" spans="1:26" ht="12.75" customHeight="1">
       <c r="A327" s="12"/>
       <c r="B327" s="12"/>
-      <c r="C327" s="42"/>
+      <c r="C327" s="43"/>
       <c r="D327" s="12"/>
       <c r="E327" s="12"/>
       <c r="G327" s="12"/>
@@ -18071,7 +18147,7 @@
     <row r="328" spans="1:26" ht="12.75" customHeight="1">
       <c r="A328" s="12"/>
       <c r="B328" s="12"/>
-      <c r="C328" s="42"/>
+      <c r="C328" s="43"/>
       <c r="D328" s="12"/>
       <c r="E328" s="12"/>
       <c r="G328" s="12"/>
@@ -18098,7 +18174,7 @@
     <row r="329" spans="1:26" ht="12.75" customHeight="1">
       <c r="A329" s="12"/>
       <c r="B329" s="12"/>
-      <c r="C329" s="42"/>
+      <c r="C329" s="43"/>
       <c r="D329" s="12"/>
       <c r="E329" s="12"/>
       <c r="G329" s="12"/>
@@ -18125,7 +18201,7 @@
     <row r="330" spans="1:26" ht="12.75" customHeight="1">
       <c r="A330" s="12"/>
       <c r="B330" s="12"/>
-      <c r="C330" s="42"/>
+      <c r="C330" s="43"/>
       <c r="D330" s="12"/>
       <c r="E330" s="12"/>
       <c r="G330" s="12"/>
@@ -18152,7 +18228,7 @@
     <row r="331" spans="1:26" ht="12.75" customHeight="1">
       <c r="A331" s="12"/>
       <c r="B331" s="12"/>
-      <c r="C331" s="42"/>
+      <c r="C331" s="43"/>
       <c r="D331" s="12"/>
       <c r="E331" s="12"/>
       <c r="G331" s="12"/>
@@ -18179,7 +18255,7 @@
     <row r="332" spans="1:26" ht="12.75" customHeight="1">
       <c r="A332" s="12"/>
       <c r="B332" s="12"/>
-      <c r="C332" s="42"/>
+      <c r="C332" s="43"/>
       <c r="D332" s="12"/>
       <c r="E332" s="12"/>
       <c r="G332" s="12"/>
@@ -18206,7 +18282,7 @@
     <row r="333" spans="1:26" ht="12.75" customHeight="1">
       <c r="A333" s="12"/>
       <c r="B333" s="12"/>
-      <c r="C333" s="42"/>
+      <c r="C333" s="43"/>
       <c r="D333" s="12"/>
       <c r="E333" s="12"/>
       <c r="G333" s="12"/>
@@ -18233,7 +18309,7 @@
     <row r="334" spans="1:26" ht="12.75" customHeight="1">
       <c r="A334" s="12"/>
       <c r="B334" s="12"/>
-      <c r="C334" s="42"/>
+      <c r="C334" s="43"/>
       <c r="D334" s="12"/>
       <c r="E334" s="12"/>
       <c r="G334" s="12"/>
@@ -18260,7 +18336,7 @@
     <row r="335" spans="1:26" ht="12.75" customHeight="1">
       <c r="A335" s="12"/>
       <c r="B335" s="12"/>
-      <c r="C335" s="42"/>
+      <c r="C335" s="43"/>
       <c r="D335" s="12"/>
       <c r="E335" s="12"/>
       <c r="G335" s="12"/>
@@ -19087,7 +19163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V1144"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H201" sqref="H201"/>
     </sheetView>
   </sheetViews>
@@ -33093,7 +33169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -34649,7 +34725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D182"/>
     </sheetView>
   </sheetViews>

</xml_diff>